<commit_message>
hospitalización en ucis, al 27 de abril
Signed-off-by: MinCiencia GitHub Actions Bot <actions@github.com>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -2905,10 +2905,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NB1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NC2" sqref="NC2:NI17"/>
+      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,7 +2930,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4050,8 +4050,29 @@
       <c r="NI1" s="8">
         <v>44306</v>
       </c>
+      <c r="NJ1" s="8">
+        <v>44307</v>
+      </c>
+      <c r="NK1" s="8">
+        <v>44308</v>
+      </c>
+      <c r="NL1" s="8">
+        <v>44309</v>
+      </c>
+      <c r="NM1" s="8">
+        <v>44310</v>
+      </c>
+      <c r="NN1" s="8">
+        <v>44311</v>
+      </c>
+      <c r="NO1" s="8">
+        <v>44312</v>
+      </c>
+      <c r="NP1" s="8">
+        <v>44313</v>
+      </c>
     </row>
-    <row r="2" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5171,8 +5192,29 @@
       <c r="NI2" s="11">
         <v>40</v>
       </c>
+      <c r="NJ2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NK2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NL2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NM2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NN2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NO2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NP2" s="11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6292,8 +6334,29 @@
       <c r="NI3" s="11">
         <v>62</v>
       </c>
+      <c r="NJ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NK3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NL3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NM3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NN3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NO3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NP3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7413,8 +7476,29 @@
       <c r="NI4" s="11">
         <v>170</v>
       </c>
+      <c r="NJ4" s="11">
+        <v>173</v>
+      </c>
+      <c r="NK4" s="11">
+        <v>173</v>
+      </c>
+      <c r="NL4" s="11">
+        <v>172</v>
+      </c>
+      <c r="NM4" s="11">
+        <v>170</v>
+      </c>
+      <c r="NN4" s="11">
+        <v>168</v>
+      </c>
+      <c r="NO4" s="11">
+        <v>172</v>
+      </c>
+      <c r="NP4" s="11">
+        <v>172</v>
+      </c>
     </row>
-    <row r="5" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -8534,8 +8618,29 @@
       <c r="NI5" s="11">
         <v>34</v>
       </c>
+      <c r="NJ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NK5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NL5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NM5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NN5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NO5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NP5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -9655,8 +9760,29 @@
       <c r="NI6" s="11">
         <v>144</v>
       </c>
+      <c r="NJ6" s="11">
+        <v>144</v>
+      </c>
+      <c r="NK6" s="11">
+        <v>143</v>
+      </c>
+      <c r="NL6" s="11">
+        <v>144</v>
+      </c>
+      <c r="NM6" s="11">
+        <v>143</v>
+      </c>
+      <c r="NN6" s="11">
+        <v>144</v>
+      </c>
+      <c r="NO6" s="11">
+        <v>144</v>
+      </c>
+      <c r="NP6" s="11">
+        <v>144</v>
+      </c>
     </row>
-    <row r="7" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -10776,8 +10902,29 @@
       <c r="NI7" s="11">
         <v>320</v>
       </c>
+      <c r="NJ7" s="11">
+        <v>320</v>
+      </c>
+      <c r="NK7" s="11">
+        <v>325</v>
+      </c>
+      <c r="NL7" s="11">
+        <v>328</v>
+      </c>
+      <c r="NM7" s="11">
+        <v>330</v>
+      </c>
+      <c r="NN7" s="11">
+        <v>344</v>
+      </c>
+      <c r="NO7" s="11">
+        <v>344</v>
+      </c>
+      <c r="NP7" s="11">
+        <v>344</v>
+      </c>
     </row>
-    <row r="8" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -11897,8 +12044,29 @@
       <c r="NI8" s="11">
         <v>2517</v>
       </c>
+      <c r="NJ8" s="11">
+        <v>2530</v>
+      </c>
+      <c r="NK8" s="11">
+        <v>2560</v>
+      </c>
+      <c r="NL8" s="11">
+        <v>2586</v>
+      </c>
+      <c r="NM8" s="11">
+        <v>2583</v>
+      </c>
+      <c r="NN8" s="11">
+        <v>2582</v>
+      </c>
+      <c r="NO8" s="11">
+        <v>2579</v>
+      </c>
+      <c r="NP8" s="11">
+        <v>2590</v>
+      </c>
     </row>
-    <row r="9" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13018,8 +13186,29 @@
       <c r="NI9" s="11">
         <v>199</v>
       </c>
+      <c r="NJ9" s="11">
+        <v>207</v>
+      </c>
+      <c r="NK9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NL9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NM9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NN9" s="11">
+        <v>207</v>
+      </c>
+      <c r="NO9" s="11">
+        <v>203</v>
+      </c>
+      <c r="NP9" s="11">
+        <v>203</v>
+      </c>
     </row>
-    <row r="10" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -14139,8 +14328,29 @@
       <c r="NI10" s="11">
         <v>163</v>
       </c>
+      <c r="NJ10" s="11">
+        <v>165</v>
+      </c>
+      <c r="NK10" s="11">
+        <v>165</v>
+      </c>
+      <c r="NL10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NM10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NN10" s="11">
+        <v>161</v>
+      </c>
+      <c r="NO10" s="11">
+        <v>162</v>
+      </c>
+      <c r="NP10" s="11">
+        <v>166</v>
+      </c>
     </row>
-    <row r="11" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -15260,8 +15470,29 @@
       <c r="NI11" s="11">
         <v>72</v>
       </c>
+      <c r="NJ11" s="11">
+        <v>72</v>
+      </c>
+      <c r="NK11" s="11">
+        <v>72</v>
+      </c>
+      <c r="NL11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NM11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NN11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NO11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NP11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -16381,8 +16612,29 @@
       <c r="NI12" s="11">
         <v>313</v>
       </c>
+      <c r="NJ12" s="11">
+        <v>312</v>
+      </c>
+      <c r="NK12" s="11">
+        <v>313</v>
+      </c>
+      <c r="NL12" s="11">
+        <v>313</v>
+      </c>
+      <c r="NM12" s="11">
+        <v>313</v>
+      </c>
+      <c r="NN12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NO12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NP12" s="11">
+        <v>315</v>
+      </c>
     </row>
-    <row r="13" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -17502,8 +17754,29 @@
       <c r="NI13" s="11">
         <v>132</v>
       </c>
+      <c r="NJ13" s="11">
+        <v>136</v>
+      </c>
+      <c r="NK13" s="11">
+        <v>141</v>
+      </c>
+      <c r="NL13" s="11">
+        <v>140</v>
+      </c>
+      <c r="NM13" s="11">
+        <v>141</v>
+      </c>
+      <c r="NN13" s="11">
+        <v>142</v>
+      </c>
+      <c r="NO13" s="11">
+        <v>143</v>
+      </c>
+      <c r="NP13" s="11">
+        <v>145</v>
+      </c>
     </row>
-    <row r="14" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -18623,8 +18896,29 @@
       <c r="NI14" s="11">
         <v>46</v>
       </c>
+      <c r="NJ14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NK14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NL14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NM14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NN14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NO14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NP14" s="11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="15" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -19744,8 +20038,29 @@
       <c r="NI15" s="11">
         <v>128</v>
       </c>
+      <c r="NJ15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NK15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NL15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NM15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NN15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NO15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NP15" s="11">
+        <v>129</v>
+      </c>
     </row>
-    <row r="16" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -20865,8 +21180,29 @@
       <c r="NI16" s="11">
         <v>10</v>
       </c>
+      <c r="NJ16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NK16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NL16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NM16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NN16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NO16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NP16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:373 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -21986,8 +22322,29 @@
       <c r="NI17" s="11">
         <v>40</v>
       </c>
+      <c r="NJ17" s="11">
+        <v>40</v>
+      </c>
+      <c r="NK17" s="11">
+        <v>40</v>
+      </c>
+      <c r="NL17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NM17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NN17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NO17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NP17" s="11">
+        <v>42</v>
+      </c>
     </row>
-    <row r="18" spans="1:373 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -23163,7 +23520,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:NI18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:NP18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -23206,9 +23563,37 @@
         <f t="shared" si="7"/>
         <v>4390</v>
       </c>
+      <c r="NJ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4420</v>
+      </c>
+      <c r="NK18" s="6">
+        <f t="shared" si="7"/>
+        <v>4459</v>
+      </c>
+      <c r="NL18" s="6">
+        <f t="shared" si="7"/>
+        <v>4491</v>
+      </c>
+      <c r="NM18" s="6">
+        <f t="shared" si="7"/>
+        <v>4488</v>
+      </c>
+      <c r="NN18" s="6">
+        <f t="shared" si="7"/>
+        <v>4499</v>
+      </c>
+      <c r="NO18" s="6">
+        <f t="shared" si="7"/>
+        <v>4495</v>
+      </c>
+      <c r="NP18" s="6">
+        <f t="shared" si="7"/>
+        <v>4512</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:373 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -23226,12 +23611,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NI36"/>
+  <dimension ref="A1:NP36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NB1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NI2" sqref="NI2:NI17"/>
+      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23251,7 +23636,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -24371,8 +24756,29 @@
       <c r="NI1" s="8">
         <v>44306</v>
       </c>
+      <c r="NJ1" s="8">
+        <v>44307</v>
+      </c>
+      <c r="NK1" s="8">
+        <v>44308</v>
+      </c>
+      <c r="NL1" s="8">
+        <v>44309</v>
+      </c>
+      <c r="NM1" s="8">
+        <v>44310</v>
+      </c>
+      <c r="NN1" s="8">
+        <v>44311</v>
+      </c>
+      <c r="NO1" s="8">
+        <v>44312</v>
+      </c>
+      <c r="NP1" s="8">
+        <v>44313</v>
+      </c>
     </row>
-    <row r="2" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -25492,8 +25898,29 @@
       <c r="NI2">
         <v>36</v>
       </c>
+      <c r="NJ2">
+        <v>33</v>
+      </c>
+      <c r="NK2">
+        <v>34</v>
+      </c>
+      <c r="NL2">
+        <v>37</v>
+      </c>
+      <c r="NM2">
+        <v>36</v>
+      </c>
+      <c r="NN2">
+        <v>35</v>
+      </c>
+      <c r="NO2">
+        <v>37</v>
+      </c>
+      <c r="NP2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -26613,8 +27040,29 @@
       <c r="NI3">
         <v>52</v>
       </c>
+      <c r="NJ3">
+        <v>58</v>
+      </c>
+      <c r="NK3">
+        <v>59</v>
+      </c>
+      <c r="NL3">
+        <v>61</v>
+      </c>
+      <c r="NM3">
+        <v>60</v>
+      </c>
+      <c r="NN3">
+        <v>60</v>
+      </c>
+      <c r="NO3">
+        <v>58</v>
+      </c>
+      <c r="NP3">
+        <v>60</v>
+      </c>
     </row>
-    <row r="4" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -27734,8 +28182,29 @@
       <c r="NI4">
         <v>164</v>
       </c>
+      <c r="NJ4">
+        <v>158</v>
+      </c>
+      <c r="NK4">
+        <v>159</v>
+      </c>
+      <c r="NL4">
+        <v>156</v>
+      </c>
+      <c r="NM4">
+        <v>148</v>
+      </c>
+      <c r="NN4">
+        <v>147</v>
+      </c>
+      <c r="NO4">
+        <v>156</v>
+      </c>
+      <c r="NP4">
+        <v>152</v>
+      </c>
     </row>
-    <row r="5" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -28855,8 +29324,29 @@
       <c r="NI5">
         <v>34</v>
       </c>
+      <c r="NJ5">
+        <v>33</v>
+      </c>
+      <c r="NK5">
+        <v>31</v>
+      </c>
+      <c r="NL5">
+        <v>31</v>
+      </c>
+      <c r="NM5">
+        <v>33</v>
+      </c>
+      <c r="NN5">
+        <v>33</v>
+      </c>
+      <c r="NO5">
+        <v>32</v>
+      </c>
+      <c r="NP5">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -29976,8 +30466,29 @@
       <c r="NI6">
         <v>137</v>
       </c>
+      <c r="NJ6">
+        <v>133</v>
+      </c>
+      <c r="NK6">
+        <v>127</v>
+      </c>
+      <c r="NL6">
+        <v>127</v>
+      </c>
+      <c r="NM6">
+        <v>130</v>
+      </c>
+      <c r="NN6">
+        <v>128</v>
+      </c>
+      <c r="NO6">
+        <v>132</v>
+      </c>
+      <c r="NP6">
+        <v>135</v>
+      </c>
     </row>
-    <row r="7" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -31097,8 +31608,29 @@
       <c r="NI7">
         <v>311</v>
       </c>
+      <c r="NJ7">
+        <v>313</v>
+      </c>
+      <c r="NK7">
+        <v>319</v>
+      </c>
+      <c r="NL7">
+        <v>318</v>
+      </c>
+      <c r="NM7">
+        <v>315</v>
+      </c>
+      <c r="NN7">
+        <v>338</v>
+      </c>
+      <c r="NO7">
+        <v>338</v>
+      </c>
+      <c r="NP7">
+        <v>334</v>
+      </c>
     </row>
-    <row r="8" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -32218,8 +32750,29 @@
       <c r="NI8">
         <v>2447</v>
       </c>
+      <c r="NJ8">
+        <v>2447</v>
+      </c>
+      <c r="NK8">
+        <v>2472</v>
+      </c>
+      <c r="NL8">
+        <v>2492</v>
+      </c>
+      <c r="NM8">
+        <v>2494</v>
+      </c>
+      <c r="NN8">
+        <v>2474</v>
+      </c>
+      <c r="NO8">
+        <v>2492</v>
+      </c>
+      <c r="NP8">
+        <v>2508</v>
+      </c>
     </row>
-    <row r="9" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -33339,8 +33892,29 @@
       <c r="NI9">
         <v>185</v>
       </c>
+      <c r="NJ9">
+        <v>184</v>
+      </c>
+      <c r="NK9">
+        <v>184</v>
+      </c>
+      <c r="NL9">
+        <v>183</v>
+      </c>
+      <c r="NM9">
+        <v>184</v>
+      </c>
+      <c r="NN9">
+        <v>180</v>
+      </c>
+      <c r="NO9">
+        <v>182</v>
+      </c>
+      <c r="NP9">
+        <v>179</v>
+      </c>
     </row>
-    <row r="10" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -34460,8 +35034,29 @@
       <c r="NI10">
         <v>160</v>
       </c>
+      <c r="NJ10">
+        <v>161</v>
+      </c>
+      <c r="NK10">
+        <v>163</v>
+      </c>
+      <c r="NL10">
+        <v>160</v>
+      </c>
+      <c r="NM10">
+        <v>156</v>
+      </c>
+      <c r="NN10">
+        <v>159</v>
+      </c>
+      <c r="NO10">
+        <v>155</v>
+      </c>
+      <c r="NP10">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -35581,8 +36176,29 @@
       <c r="NI11">
         <v>64</v>
       </c>
+      <c r="NJ11">
+        <v>61</v>
+      </c>
+      <c r="NK11">
+        <v>63</v>
+      </c>
+      <c r="NL11">
+        <v>64</v>
+      </c>
+      <c r="NM11">
+        <v>67</v>
+      </c>
+      <c r="NN11">
+        <v>65</v>
+      </c>
+      <c r="NO11">
+        <v>69</v>
+      </c>
+      <c r="NP11">
+        <v>68</v>
+      </c>
     </row>
-    <row r="12" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -36702,8 +37318,29 @@
       <c r="NI12">
         <v>294</v>
       </c>
+      <c r="NJ12">
+        <v>294</v>
+      </c>
+      <c r="NK12">
+        <v>295</v>
+      </c>
+      <c r="NL12">
+        <v>296</v>
+      </c>
+      <c r="NM12">
+        <v>294</v>
+      </c>
+      <c r="NN12">
+        <v>293</v>
+      </c>
+      <c r="NO12">
+        <v>289</v>
+      </c>
+      <c r="NP12">
+        <v>292</v>
+      </c>
     </row>
-    <row r="13" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -37823,8 +38460,29 @@
       <c r="NI13">
         <v>129</v>
       </c>
+      <c r="NJ13">
+        <v>132</v>
+      </c>
+      <c r="NK13">
+        <v>135</v>
+      </c>
+      <c r="NL13">
+        <v>137</v>
+      </c>
+      <c r="NM13">
+        <v>137</v>
+      </c>
+      <c r="NN13">
+        <v>137</v>
+      </c>
+      <c r="NO13">
+        <v>136</v>
+      </c>
+      <c r="NP13">
+        <v>140</v>
+      </c>
     </row>
-    <row r="14" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -38944,8 +39602,29 @@
       <c r="NI14">
         <v>42</v>
       </c>
+      <c r="NJ14">
+        <v>44</v>
+      </c>
+      <c r="NK14">
+        <v>42</v>
+      </c>
+      <c r="NL14">
+        <v>43</v>
+      </c>
+      <c r="NM14">
+        <v>40</v>
+      </c>
+      <c r="NN14">
+        <v>40</v>
+      </c>
+      <c r="NO14">
+        <v>40</v>
+      </c>
+      <c r="NP14">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -40065,8 +40744,29 @@
       <c r="NI15">
         <v>118</v>
       </c>
+      <c r="NJ15">
+        <v>119</v>
+      </c>
+      <c r="NK15">
+        <v>122</v>
+      </c>
+      <c r="NL15">
+        <v>116</v>
+      </c>
+      <c r="NM15">
+        <v>118</v>
+      </c>
+      <c r="NN15">
+        <v>122</v>
+      </c>
+      <c r="NO15">
+        <v>122</v>
+      </c>
+      <c r="NP15">
+        <v>118</v>
+      </c>
     </row>
-    <row r="16" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -41186,8 +41886,29 @@
       <c r="NI16">
         <v>10</v>
       </c>
+      <c r="NJ16">
+        <v>7</v>
+      </c>
+      <c r="NK16">
+        <v>10</v>
+      </c>
+      <c r="NL16">
+        <v>10</v>
+      </c>
+      <c r="NM16">
+        <v>10</v>
+      </c>
+      <c r="NN16">
+        <v>10</v>
+      </c>
+      <c r="NO16">
+        <v>10</v>
+      </c>
+      <c r="NP16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -42307,8 +43028,29 @@
       <c r="NI17">
         <v>31</v>
       </c>
+      <c r="NJ17">
+        <v>30</v>
+      </c>
+      <c r="NK17">
+        <v>30</v>
+      </c>
+      <c r="NL17">
+        <v>34</v>
+      </c>
+      <c r="NM17">
+        <v>34</v>
+      </c>
+      <c r="NN17">
+        <v>34</v>
+      </c>
+      <c r="NO17">
+        <v>30</v>
+      </c>
+      <c r="NP17">
+        <v>36</v>
+      </c>
     </row>
-    <row r="18" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -43400,7 +44142,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:NI18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:NP18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -43507,8 +44249,36 @@
         <f t="shared" si="1"/>
         <v>4214</v>
       </c>
+      <c r="NJ18" s="6">
+        <f t="shared" si="1"/>
+        <v>4207</v>
+      </c>
+      <c r="NK18" s="6">
+        <f t="shared" si="1"/>
+        <v>4245</v>
+      </c>
+      <c r="NL18" s="6">
+        <f t="shared" si="1"/>
+        <v>4265</v>
+      </c>
+      <c r="NM18" s="6">
+        <f t="shared" si="1"/>
+        <v>4256</v>
+      </c>
+      <c r="NN18" s="6">
+        <f t="shared" si="1"/>
+        <v>4255</v>
+      </c>
+      <c r="NO18" s="6">
+        <f t="shared" si="1"/>
+        <v>4278</v>
+      </c>
+      <c r="NP18" s="6">
+        <f t="shared" si="1"/>
+        <v>4295</v>
+      </c>
     </row>
-    <row r="20" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -43791,7 +44561,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -44074,7 +44844,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -44357,7 +45127,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -44640,7 +45410,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -44923,7 +45693,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -45206,7 +45976,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -45489,7 +46259,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -45772,7 +46542,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -46055,7 +46825,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -46338,7 +47108,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -46621,7 +47391,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -46904,7 +47674,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -48327,12 +49097,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NI34"/>
+  <dimension ref="A1:NP34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NB1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NC2" sqref="NC2:NI17"/>
+      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48353,7 +49123,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -49473,8 +50243,29 @@
       <c r="NI1" s="8">
         <v>44306</v>
       </c>
+      <c r="NJ1" s="8">
+        <v>44307</v>
+      </c>
+      <c r="NK1" s="8">
+        <v>44308</v>
+      </c>
+      <c r="NL1" s="8">
+        <v>44309</v>
+      </c>
+      <c r="NM1" s="8">
+        <v>44310</v>
+      </c>
+      <c r="NN1" s="8">
+        <v>44311</v>
+      </c>
+      <c r="NO1" s="8">
+        <v>44312</v>
+      </c>
+      <c r="NP1" s="8">
+        <v>44313</v>
+      </c>
     </row>
-    <row r="2" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -50594,8 +51385,29 @@
       <c r="NI2">
         <v>30</v>
       </c>
+      <c r="NJ2">
+        <v>28</v>
+      </c>
+      <c r="NK2">
+        <v>29</v>
+      </c>
+      <c r="NL2">
+        <v>30</v>
+      </c>
+      <c r="NM2">
+        <v>32</v>
+      </c>
+      <c r="NN2">
+        <v>31</v>
+      </c>
+      <c r="NO2">
+        <v>33</v>
+      </c>
+      <c r="NP2">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -51715,8 +52527,29 @@
       <c r="NI3">
         <v>50</v>
       </c>
+      <c r="NJ3">
+        <v>56</v>
+      </c>
+      <c r="NK3">
+        <v>56</v>
+      </c>
+      <c r="NL3">
+        <v>59</v>
+      </c>
+      <c r="NM3">
+        <v>58</v>
+      </c>
+      <c r="NN3">
+        <v>58</v>
+      </c>
+      <c r="NO3">
+        <v>56</v>
+      </c>
+      <c r="NP3">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -52836,8 +53669,29 @@
       <c r="NI4">
         <v>106</v>
       </c>
+      <c r="NJ4">
+        <v>103</v>
+      </c>
+      <c r="NK4">
+        <v>105</v>
+      </c>
+      <c r="NL4">
+        <v>99</v>
+      </c>
+      <c r="NM4">
+        <v>97</v>
+      </c>
+      <c r="NN4">
+        <v>92</v>
+      </c>
+      <c r="NO4">
+        <v>94</v>
+      </c>
+      <c r="NP4">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -53957,8 +54811,29 @@
       <c r="NI5">
         <v>31</v>
       </c>
+      <c r="NJ5">
+        <v>30</v>
+      </c>
+      <c r="NK5">
+        <v>28</v>
+      </c>
+      <c r="NL5">
+        <v>28</v>
+      </c>
+      <c r="NM5">
+        <v>31</v>
+      </c>
+      <c r="NN5">
+        <v>31</v>
+      </c>
+      <c r="NO5">
+        <v>30</v>
+      </c>
+      <c r="NP5">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -55078,8 +55953,29 @@
       <c r="NI6">
         <v>100</v>
       </c>
+      <c r="NJ6">
+        <v>103</v>
+      </c>
+      <c r="NK6">
+        <v>100</v>
+      </c>
+      <c r="NL6">
+        <v>99</v>
+      </c>
+      <c r="NM6">
+        <v>100</v>
+      </c>
+      <c r="NN6">
+        <v>100</v>
+      </c>
+      <c r="NO6">
+        <v>102</v>
+      </c>
+      <c r="NP6">
+        <v>106</v>
+      </c>
     </row>
-    <row r="7" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -56199,8 +57095,29 @@
       <c r="NI7">
         <v>262</v>
       </c>
+      <c r="NJ7">
+        <v>260</v>
+      </c>
+      <c r="NK7">
+        <v>273</v>
+      </c>
+      <c r="NL7">
+        <v>271</v>
+      </c>
+      <c r="NM7">
+        <v>266</v>
+      </c>
+      <c r="NN7">
+        <v>274</v>
+      </c>
+      <c r="NO7">
+        <v>278</v>
+      </c>
+      <c r="NP7">
+        <v>272</v>
+      </c>
     </row>
-    <row r="8" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -57320,8 +58237,29 @@
       <c r="NI8">
         <v>1958</v>
       </c>
+      <c r="NJ8">
+        <v>1984</v>
+      </c>
+      <c r="NK8">
+        <v>1939</v>
+      </c>
+      <c r="NL8">
+        <v>1969</v>
+      </c>
+      <c r="NM8">
+        <v>1963</v>
+      </c>
+      <c r="NN8">
+        <v>1937</v>
+      </c>
+      <c r="NO8">
+        <v>1942</v>
+      </c>
+      <c r="NP8">
+        <v>1987</v>
+      </c>
     </row>
-    <row r="9" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -58441,8 +59379,29 @@
       <c r="NI9">
         <v>156</v>
       </c>
+      <c r="NJ9">
+        <v>157</v>
+      </c>
+      <c r="NK9">
+        <v>156</v>
+      </c>
+      <c r="NL9">
+        <v>157</v>
+      </c>
+      <c r="NM9">
+        <v>153</v>
+      </c>
+      <c r="NN9">
+        <v>156</v>
+      </c>
+      <c r="NO9">
+        <v>160</v>
+      </c>
+      <c r="NP9">
+        <v>156</v>
+      </c>
     </row>
-    <row r="10" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -59562,8 +60521,29 @@
       <c r="NI10">
         <v>143</v>
       </c>
+      <c r="NJ10">
+        <v>144</v>
+      </c>
+      <c r="NK10">
+        <v>146</v>
+      </c>
+      <c r="NL10">
+        <v>144</v>
+      </c>
+      <c r="NM10">
+        <v>137</v>
+      </c>
+      <c r="NN10">
+        <v>137</v>
+      </c>
+      <c r="NO10">
+        <v>134</v>
+      </c>
+      <c r="NP10">
+        <v>136</v>
+      </c>
     </row>
-    <row r="11" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -60683,8 +61663,29 @@
       <c r="NI11">
         <v>48</v>
       </c>
+      <c r="NJ11">
+        <v>44</v>
+      </c>
+      <c r="NK11">
+        <v>49</v>
+      </c>
+      <c r="NL11">
+        <v>49</v>
+      </c>
+      <c r="NM11">
+        <v>51</v>
+      </c>
+      <c r="NN11">
+        <v>49</v>
+      </c>
+      <c r="NO11">
+        <v>54</v>
+      </c>
+      <c r="NP11">
+        <v>52</v>
+      </c>
     </row>
-    <row r="12" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -61804,8 +62805,29 @@
       <c r="NI12">
         <v>238</v>
       </c>
+      <c r="NJ12">
+        <v>235</v>
+      </c>
+      <c r="NK12">
+        <v>233</v>
+      </c>
+      <c r="NL12">
+        <v>232</v>
+      </c>
+      <c r="NM12">
+        <v>229</v>
+      </c>
+      <c r="NN12">
+        <v>226</v>
+      </c>
+      <c r="NO12">
+        <v>224</v>
+      </c>
+      <c r="NP12">
+        <v>226</v>
+      </c>
     </row>
-    <row r="13" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -62925,8 +63947,29 @@
       <c r="NI13">
         <v>107</v>
       </c>
+      <c r="NJ13">
+        <v>111</v>
+      </c>
+      <c r="NK13">
+        <v>116</v>
+      </c>
+      <c r="NL13">
+        <v>113</v>
+      </c>
+      <c r="NM13">
+        <v>114</v>
+      </c>
+      <c r="NN13">
+        <v>117</v>
+      </c>
+      <c r="NO13">
+        <v>110</v>
+      </c>
+      <c r="NP13">
+        <v>113</v>
+      </c>
     </row>
-    <row r="14" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -64046,8 +65089,29 @@
       <c r="NI14">
         <v>30</v>
       </c>
+      <c r="NJ14">
+        <v>30</v>
+      </c>
+      <c r="NK14">
+        <v>29</v>
+      </c>
+      <c r="NL14">
+        <v>28</v>
+      </c>
+      <c r="NM14">
+        <v>30</v>
+      </c>
+      <c r="NN14">
+        <v>29</v>
+      </c>
+      <c r="NO14">
+        <v>29</v>
+      </c>
+      <c r="NP14">
+        <v>29</v>
+      </c>
     </row>
-    <row r="15" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -65167,8 +66231,29 @@
       <c r="NI15">
         <v>90</v>
       </c>
+      <c r="NJ15">
+        <v>92</v>
+      </c>
+      <c r="NK15">
+        <v>92</v>
+      </c>
+      <c r="NL15">
+        <v>88</v>
+      </c>
+      <c r="NM15">
+        <v>86</v>
+      </c>
+      <c r="NN15">
+        <v>86</v>
+      </c>
+      <c r="NO15">
+        <v>88</v>
+      </c>
+      <c r="NP15">
+        <v>87</v>
+      </c>
     </row>
-    <row r="16" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -66288,8 +67373,29 @@
       <c r="NI16">
         <v>7</v>
       </c>
+      <c r="NJ16">
+        <v>7</v>
+      </c>
+      <c r="NK16">
+        <v>6</v>
+      </c>
+      <c r="NL16">
+        <v>6</v>
+      </c>
+      <c r="NM16">
+        <v>7</v>
+      </c>
+      <c r="NN16">
+        <v>8</v>
+      </c>
+      <c r="NO16">
+        <v>8</v>
+      </c>
+      <c r="NP16">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -67409,8 +68515,29 @@
       <c r="NI17">
         <v>16</v>
       </c>
+      <c r="NJ17">
+        <v>17</v>
+      </c>
+      <c r="NK17">
+        <v>18</v>
+      </c>
+      <c r="NL17">
+        <v>19</v>
+      </c>
+      <c r="NM17">
+        <v>20</v>
+      </c>
+      <c r="NN17">
+        <v>22</v>
+      </c>
+      <c r="NO17">
+        <v>21</v>
+      </c>
+      <c r="NP17">
+        <v>24</v>
+      </c>
     </row>
-    <row r="18" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -68547,7 +69674,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:NI18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:NP18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -68614,50 +69741,78 @@
         <f t="shared" si="1"/>
         <v>3372</v>
       </c>
+      <c r="NJ18" s="6">
+        <f t="shared" si="1"/>
+        <v>3401</v>
+      </c>
+      <c r="NK18" s="6">
+        <f t="shared" si="1"/>
+        <v>3375</v>
+      </c>
+      <c r="NL18" s="6">
+        <f t="shared" si="1"/>
+        <v>3391</v>
+      </c>
+      <c r="NM18" s="6">
+        <f t="shared" si="1"/>
+        <v>3374</v>
+      </c>
+      <c r="NN18" s="6">
+        <f t="shared" si="1"/>
+        <v>3353</v>
+      </c>
+      <c r="NO18" s="6">
+        <f t="shared" si="1"/>
+        <v>3363</v>
+      </c>
+      <c r="NP18" s="6">
+        <f t="shared" si="1"/>
+        <v>3406</v>
+      </c>
     </row>
-    <row r="19" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -68677,12 +69832,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:NI34"/>
+  <dimension ref="A1:NP34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NB1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="A24" sqref="A24"/>
+      <selection pane="topRight" activeCell="NR15" sqref="NR15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68700,7 +69855,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -69820,8 +70975,29 @@
       <c r="NI1" s="8">
         <v>44306</v>
       </c>
+      <c r="NJ1" s="8">
+        <v>44307</v>
+      </c>
+      <c r="NK1" s="8">
+        <v>44308</v>
+      </c>
+      <c r="NL1" s="8">
+        <v>44309</v>
+      </c>
+      <c r="NM1" s="8">
+        <v>44310</v>
+      </c>
+      <c r="NN1" s="8">
+        <v>44311</v>
+      </c>
+      <c r="NO1" s="8">
+        <v>44312</v>
+      </c>
+      <c r="NP1" s="8">
+        <v>44313</v>
+      </c>
     </row>
-    <row r="2" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -71033,8 +72209,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI2-'UCI OCUPADA COVID'!NI2</f>
         <v>6</v>
       </c>
+      <c r="NJ2">
+        <f>+'UCI OCUPADA TOTAL'!NJ2-'UCI OCUPADA COVID'!NJ2</f>
+        <v>5</v>
+      </c>
+      <c r="NK2">
+        <f>+'UCI OCUPADA TOTAL'!NK2-'UCI OCUPADA COVID'!NK2</f>
+        <v>5</v>
+      </c>
+      <c r="NL2">
+        <f>+'UCI OCUPADA TOTAL'!NL2-'UCI OCUPADA COVID'!NL2</f>
+        <v>7</v>
+      </c>
+      <c r="NM2">
+        <f>+'UCI OCUPADA TOTAL'!NM2-'UCI OCUPADA COVID'!NM2</f>
+        <v>4</v>
+      </c>
+      <c r="NN2">
+        <f>+'UCI OCUPADA TOTAL'!NN2-'UCI OCUPADA COVID'!NN2</f>
+        <v>4</v>
+      </c>
+      <c r="NO2">
+        <f>+'UCI OCUPADA TOTAL'!NO2-'UCI OCUPADA COVID'!NO2</f>
+        <v>4</v>
+      </c>
+      <c r="NP2">
+        <f>+'UCI OCUPADA TOTAL'!NP2-'UCI OCUPADA COVID'!NP2</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -72246,8 +73450,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI3-'UCI OCUPADA COVID'!NI3</f>
         <v>2</v>
       </c>
+      <c r="NJ3">
+        <f>+'UCI OCUPADA TOTAL'!NJ3-'UCI OCUPADA COVID'!NJ3</f>
+        <v>2</v>
+      </c>
+      <c r="NK3">
+        <f>+'UCI OCUPADA TOTAL'!NK3-'UCI OCUPADA COVID'!NK3</f>
+        <v>3</v>
+      </c>
+      <c r="NL3">
+        <f>+'UCI OCUPADA TOTAL'!NL3-'UCI OCUPADA COVID'!NL3</f>
+        <v>2</v>
+      </c>
+      <c r="NM3">
+        <f>+'UCI OCUPADA TOTAL'!NM3-'UCI OCUPADA COVID'!NM3</f>
+        <v>2</v>
+      </c>
+      <c r="NN3">
+        <f>+'UCI OCUPADA TOTAL'!NN3-'UCI OCUPADA COVID'!NN3</f>
+        <v>2</v>
+      </c>
+      <c r="NO3">
+        <f>+'UCI OCUPADA TOTAL'!NO3-'UCI OCUPADA COVID'!NO3</f>
+        <v>2</v>
+      </c>
+      <c r="NP3">
+        <f>+'UCI OCUPADA TOTAL'!NP3-'UCI OCUPADA COVID'!NP3</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -73459,8 +74691,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI4-'UCI OCUPADA COVID'!NI4</f>
         <v>58</v>
       </c>
+      <c r="NJ4">
+        <f>+'UCI OCUPADA TOTAL'!NJ4-'UCI OCUPADA COVID'!NJ4</f>
+        <v>55</v>
+      </c>
+      <c r="NK4">
+        <f>+'UCI OCUPADA TOTAL'!NK4-'UCI OCUPADA COVID'!NK4</f>
+        <v>54</v>
+      </c>
+      <c r="NL4">
+        <f>+'UCI OCUPADA TOTAL'!NL4-'UCI OCUPADA COVID'!NL4</f>
+        <v>57</v>
+      </c>
+      <c r="NM4">
+        <f>+'UCI OCUPADA TOTAL'!NM4-'UCI OCUPADA COVID'!NM4</f>
+        <v>51</v>
+      </c>
+      <c r="NN4">
+        <f>+'UCI OCUPADA TOTAL'!NN4-'UCI OCUPADA COVID'!NN4</f>
+        <v>55</v>
+      </c>
+      <c r="NO4">
+        <f>+'UCI OCUPADA TOTAL'!NO4-'UCI OCUPADA COVID'!NO4</f>
+        <v>62</v>
+      </c>
+      <c r="NP4">
+        <f>+'UCI OCUPADA TOTAL'!NP4-'UCI OCUPADA COVID'!NP4</f>
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -74672,8 +75932,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI5-'UCI OCUPADA COVID'!NI5</f>
         <v>3</v>
       </c>
+      <c r="NJ5">
+        <f>+'UCI OCUPADA TOTAL'!NJ5-'UCI OCUPADA COVID'!NJ5</f>
+        <v>3</v>
+      </c>
+      <c r="NK5">
+        <f>+'UCI OCUPADA TOTAL'!NK5-'UCI OCUPADA COVID'!NK5</f>
+        <v>3</v>
+      </c>
+      <c r="NL5">
+        <f>+'UCI OCUPADA TOTAL'!NL5-'UCI OCUPADA COVID'!NL5</f>
+        <v>3</v>
+      </c>
+      <c r="NM5">
+        <f>+'UCI OCUPADA TOTAL'!NM5-'UCI OCUPADA COVID'!NM5</f>
+        <v>2</v>
+      </c>
+      <c r="NN5">
+        <f>+'UCI OCUPADA TOTAL'!NN5-'UCI OCUPADA COVID'!NN5</f>
+        <v>2</v>
+      </c>
+      <c r="NO5">
+        <f>+'UCI OCUPADA TOTAL'!NO5-'UCI OCUPADA COVID'!NO5</f>
+        <v>2</v>
+      </c>
+      <c r="NP5">
+        <f>+'UCI OCUPADA TOTAL'!NP5-'UCI OCUPADA COVID'!NP5</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -75885,8 +77173,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI6-'UCI OCUPADA COVID'!NI6</f>
         <v>37</v>
       </c>
+      <c r="NJ6">
+        <f>+'UCI OCUPADA TOTAL'!NJ6-'UCI OCUPADA COVID'!NJ6</f>
+        <v>30</v>
+      </c>
+      <c r="NK6">
+        <f>+'UCI OCUPADA TOTAL'!NK6-'UCI OCUPADA COVID'!NK6</f>
+        <v>27</v>
+      </c>
+      <c r="NL6">
+        <f>+'UCI OCUPADA TOTAL'!NL6-'UCI OCUPADA COVID'!NL6</f>
+        <v>28</v>
+      </c>
+      <c r="NM6">
+        <f>+'UCI OCUPADA TOTAL'!NM6-'UCI OCUPADA COVID'!NM6</f>
+        <v>30</v>
+      </c>
+      <c r="NN6">
+        <f>+'UCI OCUPADA TOTAL'!NN6-'UCI OCUPADA COVID'!NN6</f>
+        <v>28</v>
+      </c>
+      <c r="NO6">
+        <f>+'UCI OCUPADA TOTAL'!NO6-'UCI OCUPADA COVID'!NO6</f>
+        <v>30</v>
+      </c>
+      <c r="NP6">
+        <f>+'UCI OCUPADA TOTAL'!NP6-'UCI OCUPADA COVID'!NP6</f>
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -77098,8 +78414,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI7-'UCI OCUPADA COVID'!NI7</f>
         <v>49</v>
       </c>
+      <c r="NJ7">
+        <f>+'UCI OCUPADA TOTAL'!NJ7-'UCI OCUPADA COVID'!NJ7</f>
+        <v>53</v>
+      </c>
+      <c r="NK7">
+        <f>+'UCI OCUPADA TOTAL'!NK7-'UCI OCUPADA COVID'!NK7</f>
+        <v>46</v>
+      </c>
+      <c r="NL7">
+        <f>+'UCI OCUPADA TOTAL'!NL7-'UCI OCUPADA COVID'!NL7</f>
+        <v>47</v>
+      </c>
+      <c r="NM7">
+        <f>+'UCI OCUPADA TOTAL'!NM7-'UCI OCUPADA COVID'!NM7</f>
+        <v>49</v>
+      </c>
+      <c r="NN7">
+        <f>+'UCI OCUPADA TOTAL'!NN7-'UCI OCUPADA COVID'!NN7</f>
+        <v>64</v>
+      </c>
+      <c r="NO7">
+        <f>+'UCI OCUPADA TOTAL'!NO7-'UCI OCUPADA COVID'!NO7</f>
+        <v>60</v>
+      </c>
+      <c r="NP7">
+        <f>+'UCI OCUPADA TOTAL'!NP7-'UCI OCUPADA COVID'!NP7</f>
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -78311,8 +79655,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI8-'UCI OCUPADA COVID'!NI8</f>
         <v>489</v>
       </c>
+      <c r="NJ8">
+        <f>+'UCI OCUPADA TOTAL'!NJ8-'UCI OCUPADA COVID'!NJ8</f>
+        <v>463</v>
+      </c>
+      <c r="NK8">
+        <f>+'UCI OCUPADA TOTAL'!NK8-'UCI OCUPADA COVID'!NK8</f>
+        <v>533</v>
+      </c>
+      <c r="NL8">
+        <f>+'UCI OCUPADA TOTAL'!NL8-'UCI OCUPADA COVID'!NL8</f>
+        <v>523</v>
+      </c>
+      <c r="NM8">
+        <f>+'UCI OCUPADA TOTAL'!NM8-'UCI OCUPADA COVID'!NM8</f>
+        <v>531</v>
+      </c>
+      <c r="NN8">
+        <f>+'UCI OCUPADA TOTAL'!NN8-'UCI OCUPADA COVID'!NN8</f>
+        <v>537</v>
+      </c>
+      <c r="NO8">
+        <f>+'UCI OCUPADA TOTAL'!NO8-'UCI OCUPADA COVID'!NO8</f>
+        <v>550</v>
+      </c>
+      <c r="NP8">
+        <f>+'UCI OCUPADA TOTAL'!NP8-'UCI OCUPADA COVID'!NP8</f>
+        <v>521</v>
+      </c>
     </row>
-    <row r="9" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -79524,8 +80896,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI9-'UCI OCUPADA COVID'!NI9</f>
         <v>29</v>
       </c>
+      <c r="NJ9">
+        <f>+'UCI OCUPADA TOTAL'!NJ9-'UCI OCUPADA COVID'!NJ9</f>
+        <v>27</v>
+      </c>
+      <c r="NK9">
+        <f>+'UCI OCUPADA TOTAL'!NK9-'UCI OCUPADA COVID'!NK9</f>
+        <v>28</v>
+      </c>
+      <c r="NL9">
+        <f>+'UCI OCUPADA TOTAL'!NL9-'UCI OCUPADA COVID'!NL9</f>
+        <v>26</v>
+      </c>
+      <c r="NM9">
+        <f>+'UCI OCUPADA TOTAL'!NM9-'UCI OCUPADA COVID'!NM9</f>
+        <v>31</v>
+      </c>
+      <c r="NN9">
+        <f>+'UCI OCUPADA TOTAL'!NN9-'UCI OCUPADA COVID'!NN9</f>
+        <v>24</v>
+      </c>
+      <c r="NO9">
+        <f>+'UCI OCUPADA TOTAL'!NO9-'UCI OCUPADA COVID'!NO9</f>
+        <v>22</v>
+      </c>
+      <c r="NP9">
+        <f>+'UCI OCUPADA TOTAL'!NP9-'UCI OCUPADA COVID'!NP9</f>
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -80737,8 +82137,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI10-'UCI OCUPADA COVID'!NI10</f>
         <v>17</v>
       </c>
+      <c r="NJ10">
+        <f>+'UCI OCUPADA TOTAL'!NJ10-'UCI OCUPADA COVID'!NJ10</f>
+        <v>17</v>
+      </c>
+      <c r="NK10">
+        <f>+'UCI OCUPADA TOTAL'!NK10-'UCI OCUPADA COVID'!NK10</f>
+        <v>17</v>
+      </c>
+      <c r="NL10">
+        <f>+'UCI OCUPADA TOTAL'!NL10-'UCI OCUPADA COVID'!NL10</f>
+        <v>16</v>
+      </c>
+      <c r="NM10">
+        <f>+'UCI OCUPADA TOTAL'!NM10-'UCI OCUPADA COVID'!NM10</f>
+        <v>19</v>
+      </c>
+      <c r="NN10">
+        <f>+'UCI OCUPADA TOTAL'!NN10-'UCI OCUPADA COVID'!NN10</f>
+        <v>22</v>
+      </c>
+      <c r="NO10">
+        <f>+'UCI OCUPADA TOTAL'!NO10-'UCI OCUPADA COVID'!NO10</f>
+        <v>21</v>
+      </c>
+      <c r="NP10">
+        <f>+'UCI OCUPADA TOTAL'!NP10-'UCI OCUPADA COVID'!NP10</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -81950,8 +83378,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI11-'UCI OCUPADA COVID'!NI11</f>
         <v>16</v>
       </c>
+      <c r="NJ11">
+        <f>+'UCI OCUPADA TOTAL'!NJ11-'UCI OCUPADA COVID'!NJ11</f>
+        <v>17</v>
+      </c>
+      <c r="NK11">
+        <f>+'UCI OCUPADA TOTAL'!NK11-'UCI OCUPADA COVID'!NK11</f>
+        <v>14</v>
+      </c>
+      <c r="NL11">
+        <f>+'UCI OCUPADA TOTAL'!NL11-'UCI OCUPADA COVID'!NL11</f>
+        <v>15</v>
+      </c>
+      <c r="NM11">
+        <f>+'UCI OCUPADA TOTAL'!NM11-'UCI OCUPADA COVID'!NM11</f>
+        <v>16</v>
+      </c>
+      <c r="NN11">
+        <f>+'UCI OCUPADA TOTAL'!NN11-'UCI OCUPADA COVID'!NN11</f>
+        <v>16</v>
+      </c>
+      <c r="NO11">
+        <f>+'UCI OCUPADA TOTAL'!NO11-'UCI OCUPADA COVID'!NO11</f>
+        <v>15</v>
+      </c>
+      <c r="NP11">
+        <f>+'UCI OCUPADA TOTAL'!NP11-'UCI OCUPADA COVID'!NP11</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -83163,8 +84619,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI12-'UCI OCUPADA COVID'!NI12</f>
         <v>56</v>
       </c>
+      <c r="NJ12">
+        <f>+'UCI OCUPADA TOTAL'!NJ12-'UCI OCUPADA COVID'!NJ12</f>
+        <v>59</v>
+      </c>
+      <c r="NK12">
+        <f>+'UCI OCUPADA TOTAL'!NK12-'UCI OCUPADA COVID'!NK12</f>
+        <v>62</v>
+      </c>
+      <c r="NL12">
+        <f>+'UCI OCUPADA TOTAL'!NL12-'UCI OCUPADA COVID'!NL12</f>
+        <v>64</v>
+      </c>
+      <c r="NM12">
+        <f>+'UCI OCUPADA TOTAL'!NM12-'UCI OCUPADA COVID'!NM12</f>
+        <v>65</v>
+      </c>
+      <c r="NN12">
+        <f>+'UCI OCUPADA TOTAL'!NN12-'UCI OCUPADA COVID'!NN12</f>
+        <v>67</v>
+      </c>
+      <c r="NO12">
+        <f>+'UCI OCUPADA TOTAL'!NO12-'UCI OCUPADA COVID'!NO12</f>
+        <v>65</v>
+      </c>
+      <c r="NP12">
+        <f>+'UCI OCUPADA TOTAL'!NP12-'UCI OCUPADA COVID'!NP12</f>
+        <v>66</v>
+      </c>
     </row>
-    <row r="13" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -84376,8 +85860,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI13-'UCI OCUPADA COVID'!NI13</f>
         <v>22</v>
       </c>
+      <c r="NJ13">
+        <f>+'UCI OCUPADA TOTAL'!NJ13-'UCI OCUPADA COVID'!NJ13</f>
+        <v>21</v>
+      </c>
+      <c r="NK13">
+        <f>+'UCI OCUPADA TOTAL'!NK13-'UCI OCUPADA COVID'!NK13</f>
+        <v>19</v>
+      </c>
+      <c r="NL13">
+        <f>+'UCI OCUPADA TOTAL'!NL13-'UCI OCUPADA COVID'!NL13</f>
+        <v>24</v>
+      </c>
+      <c r="NM13">
+        <f>+'UCI OCUPADA TOTAL'!NM13-'UCI OCUPADA COVID'!NM13</f>
+        <v>23</v>
+      </c>
+      <c r="NN13">
+        <f>+'UCI OCUPADA TOTAL'!NN13-'UCI OCUPADA COVID'!NN13</f>
+        <v>20</v>
+      </c>
+      <c r="NO13">
+        <f>+'UCI OCUPADA TOTAL'!NO13-'UCI OCUPADA COVID'!NO13</f>
+        <v>26</v>
+      </c>
+      <c r="NP13">
+        <f>+'UCI OCUPADA TOTAL'!NP13-'UCI OCUPADA COVID'!NP13</f>
+        <v>27</v>
+      </c>
     </row>
-    <row r="14" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -85589,8 +87101,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI14-'UCI OCUPADA COVID'!NI14</f>
         <v>12</v>
       </c>
+      <c r="NJ14">
+        <f>+'UCI OCUPADA TOTAL'!NJ14-'UCI OCUPADA COVID'!NJ14</f>
+        <v>14</v>
+      </c>
+      <c r="NK14">
+        <f>+'UCI OCUPADA TOTAL'!NK14-'UCI OCUPADA COVID'!NK14</f>
+        <v>13</v>
+      </c>
+      <c r="NL14">
+        <f>+'UCI OCUPADA TOTAL'!NL14-'UCI OCUPADA COVID'!NL14</f>
+        <v>15</v>
+      </c>
+      <c r="NM14">
+        <f>+'UCI OCUPADA TOTAL'!NM14-'UCI OCUPADA COVID'!NM14</f>
+        <v>10</v>
+      </c>
+      <c r="NN14">
+        <f>+'UCI OCUPADA TOTAL'!NN14-'UCI OCUPADA COVID'!NN14</f>
+        <v>11</v>
+      </c>
+      <c r="NO14">
+        <f>+'UCI OCUPADA TOTAL'!NO14-'UCI OCUPADA COVID'!NO14</f>
+        <v>11</v>
+      </c>
+      <c r="NP14">
+        <f>+'UCI OCUPADA TOTAL'!NP14-'UCI OCUPADA COVID'!NP14</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="15" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -86802,8 +88342,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI15-'UCI OCUPADA COVID'!NI15</f>
         <v>28</v>
       </c>
+      <c r="NJ15">
+        <f>+'UCI OCUPADA TOTAL'!NJ15-'UCI OCUPADA COVID'!NJ15</f>
+        <v>27</v>
+      </c>
+      <c r="NK15">
+        <f>+'UCI OCUPADA TOTAL'!NK15-'UCI OCUPADA COVID'!NK15</f>
+        <v>30</v>
+      </c>
+      <c r="NL15">
+        <f>+'UCI OCUPADA TOTAL'!NL15-'UCI OCUPADA COVID'!NL15</f>
+        <v>28</v>
+      </c>
+      <c r="NM15">
+        <f>+'UCI OCUPADA TOTAL'!NM15-'UCI OCUPADA COVID'!NM15</f>
+        <v>32</v>
+      </c>
+      <c r="NN15">
+        <f>+'UCI OCUPADA TOTAL'!NN15-'UCI OCUPADA COVID'!NN15</f>
+        <v>36</v>
+      </c>
+      <c r="NO15">
+        <f>+'UCI OCUPADA TOTAL'!NO15-'UCI OCUPADA COVID'!NO15</f>
+        <v>34</v>
+      </c>
+      <c r="NP15">
+        <f>+'UCI OCUPADA TOTAL'!NP15-'UCI OCUPADA COVID'!NP15</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="16" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -88015,8 +89583,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI16-'UCI OCUPADA COVID'!NI16</f>
         <v>3</v>
       </c>
+      <c r="NJ16">
+        <f>+'UCI OCUPADA TOTAL'!NJ16-'UCI OCUPADA COVID'!NJ16</f>
+        <v>0</v>
+      </c>
+      <c r="NK16">
+        <f>+'UCI OCUPADA TOTAL'!NK16-'UCI OCUPADA COVID'!NK16</f>
+        <v>4</v>
+      </c>
+      <c r="NL16">
+        <f>+'UCI OCUPADA TOTAL'!NL16-'UCI OCUPADA COVID'!NL16</f>
+        <v>4</v>
+      </c>
+      <c r="NM16">
+        <f>+'UCI OCUPADA TOTAL'!NM16-'UCI OCUPADA COVID'!NM16</f>
+        <v>3</v>
+      </c>
+      <c r="NN16">
+        <f>+'UCI OCUPADA TOTAL'!NN16-'UCI OCUPADA COVID'!NN16</f>
+        <v>2</v>
+      </c>
+      <c r="NO16">
+        <f>+'UCI OCUPADA TOTAL'!NO16-'UCI OCUPADA COVID'!NO16</f>
+        <v>2</v>
+      </c>
+      <c r="NP16">
+        <f>+'UCI OCUPADA TOTAL'!NP16-'UCI OCUPADA COVID'!NP16</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -89228,8 +90824,36 @@
         <f>+'UCI OCUPADA TOTAL'!NI17-'UCI OCUPADA COVID'!NI17</f>
         <v>15</v>
       </c>
+      <c r="NJ17">
+        <f>+'UCI OCUPADA TOTAL'!NJ17-'UCI OCUPADA COVID'!NJ17</f>
+        <v>13</v>
+      </c>
+      <c r="NK17">
+        <f>+'UCI OCUPADA TOTAL'!NK17-'UCI OCUPADA COVID'!NK17</f>
+        <v>12</v>
+      </c>
+      <c r="NL17">
+        <f>+'UCI OCUPADA TOTAL'!NL17-'UCI OCUPADA COVID'!NL17</f>
+        <v>15</v>
+      </c>
+      <c r="NM17">
+        <f>+'UCI OCUPADA TOTAL'!NM17-'UCI OCUPADA COVID'!NM17</f>
+        <v>14</v>
+      </c>
+      <c r="NN17">
+        <f>+'UCI OCUPADA TOTAL'!NN17-'UCI OCUPADA COVID'!NN17</f>
+        <v>12</v>
+      </c>
+      <c r="NO17">
+        <f>+'UCI OCUPADA TOTAL'!NO17-'UCI OCUPADA COVID'!NO17</f>
+        <v>9</v>
+      </c>
+      <c r="NP17">
+        <f>+'UCI OCUPADA TOTAL'!NP17-'UCI OCUPADA COVID'!NP17</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -90441,48 +92065,76 @@
         <f>+'UCI OCUPADA TOTAL'!NI18-'UCI OCUPADA COVID'!NI18</f>
         <v>842</v>
       </c>
+      <c r="NJ18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NJ18-'UCI OCUPADA COVID'!NJ18</f>
+        <v>806</v>
+      </c>
+      <c r="NK18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NK18-'UCI OCUPADA COVID'!NK18</f>
+        <v>870</v>
+      </c>
+      <c r="NL18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NL18-'UCI OCUPADA COVID'!NL18</f>
+        <v>874</v>
+      </c>
+      <c r="NM18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NM18-'UCI OCUPADA COVID'!NM18</f>
+        <v>882</v>
+      </c>
+      <c r="NN18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NN18-'UCI OCUPADA COVID'!NN18</f>
+        <v>902</v>
+      </c>
+      <c r="NO18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NO18-'UCI OCUPADA COVID'!NO18</f>
+        <v>915</v>
+      </c>
+      <c r="NP18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NP18-'UCI OCUPADA COVID'!NP18</f>
+        <v>889</v>
+      </c>
     </row>
-    <row r="19" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:373" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Camas uci al 5 de mayo, 2021
Signed-off-by: MinCiencia GitHub Actions Bot <actions@github.com>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -145,9 +145,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -196,12 +198,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -236,8 +239,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Millares" xfId="3" builtinId="3"/>
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Millares [0] 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2905,10 +2910,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NP1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
+      <selection pane="topRight" activeCell="NQ18" sqref="NQ18:NW18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4071,8 +4076,29 @@
       <c r="NP1" s="8">
         <v>44313</v>
       </c>
+      <c r="NQ1" s="8">
+        <v>44314</v>
+      </c>
+      <c r="NR1" s="8">
+        <v>44315</v>
+      </c>
+      <c r="NS1" s="8">
+        <v>44316</v>
+      </c>
+      <c r="NT1" s="8">
+        <v>44317</v>
+      </c>
+      <c r="NU1" s="8">
+        <v>44318</v>
+      </c>
+      <c r="NV1" s="8">
+        <v>44319</v>
+      </c>
+      <c r="NW1" s="8">
+        <v>44320</v>
+      </c>
     </row>
-    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5213,8 +5239,29 @@
       <c r="NP2" s="11">
         <v>40</v>
       </c>
+      <c r="NQ2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NR2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NS2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NT2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NU2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NV2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NW2" s="11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6355,8 +6402,29 @@
       <c r="NP3" s="11">
         <v>62</v>
       </c>
+      <c r="NQ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NR3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NS3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NT3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NU3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NV3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NW3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7497,8 +7565,29 @@
       <c r="NP4" s="11">
         <v>172</v>
       </c>
+      <c r="NQ4" s="11">
+        <v>173</v>
+      </c>
+      <c r="NR4" s="11">
+        <v>173</v>
+      </c>
+      <c r="NS4" s="11">
+        <v>173</v>
+      </c>
+      <c r="NT4" s="11">
+        <v>170</v>
+      </c>
+      <c r="NU4" s="11">
+        <v>170</v>
+      </c>
+      <c r="NV4" s="11">
+        <v>170</v>
+      </c>
+      <c r="NW4" s="11">
+        <v>168</v>
+      </c>
     </row>
-    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -8639,8 +8728,29 @@
       <c r="NP5" s="11">
         <v>34</v>
       </c>
+      <c r="NQ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NR5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NS5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NT5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NU5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NV5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NW5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -9781,8 +9891,29 @@
       <c r="NP6" s="11">
         <v>144</v>
       </c>
+      <c r="NQ6" s="11">
+        <v>143</v>
+      </c>
+      <c r="NR6" s="11">
+        <v>142</v>
+      </c>
+      <c r="NS6" s="11">
+        <v>143</v>
+      </c>
+      <c r="NT6" s="11">
+        <v>140</v>
+      </c>
+      <c r="NU6" s="11">
+        <v>140</v>
+      </c>
+      <c r="NV6" s="11">
+        <v>140</v>
+      </c>
+      <c r="NW6" s="11">
+        <v>140</v>
+      </c>
     </row>
-    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -10923,8 +11054,29 @@
       <c r="NP7" s="11">
         <v>344</v>
       </c>
+      <c r="NQ7" s="11">
+        <v>345</v>
+      </c>
+      <c r="NR7" s="11">
+        <v>345</v>
+      </c>
+      <c r="NS7" s="11">
+        <v>345</v>
+      </c>
+      <c r="NT7" s="11">
+        <v>345</v>
+      </c>
+      <c r="NU7" s="11">
+        <v>345</v>
+      </c>
+      <c r="NV7" s="11">
+        <v>344</v>
+      </c>
+      <c r="NW7" s="11">
+        <v>345</v>
+      </c>
     </row>
-    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12065,8 +12217,29 @@
       <c r="NP8" s="11">
         <v>2590</v>
       </c>
+      <c r="NQ8" s="11">
+        <v>2592</v>
+      </c>
+      <c r="NR8" s="11">
+        <v>2599</v>
+      </c>
+      <c r="NS8" s="11">
+        <v>2611</v>
+      </c>
+      <c r="NT8" s="11">
+        <v>2622</v>
+      </c>
+      <c r="NU8" s="11">
+        <v>2620</v>
+      </c>
+      <c r="NV8" s="11">
+        <v>2619</v>
+      </c>
+      <c r="NW8" s="11">
+        <v>2619</v>
+      </c>
     </row>
-    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13207,8 +13380,29 @@
       <c r="NP9" s="11">
         <v>203</v>
       </c>
+      <c r="NQ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NR9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NS9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NT9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NU9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NV9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NW9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -14349,8 +14543,29 @@
       <c r="NP10" s="11">
         <v>166</v>
       </c>
+      <c r="NQ10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NR10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NS10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NT10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NU10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NV10" s="11">
+        <v>162</v>
+      </c>
+      <c r="NW10" s="11">
+        <v>162</v>
+      </c>
     </row>
-    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -15491,8 +15706,29 @@
       <c r="NP11" s="11">
         <v>73</v>
       </c>
+      <c r="NQ11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NR11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NS11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NT11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NU11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NV11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NW11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -16633,8 +16869,29 @@
       <c r="NP12" s="11">
         <v>315</v>
       </c>
+      <c r="NQ12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NR12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NS12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NT12" s="11">
+        <v>316</v>
+      </c>
+      <c r="NU12" s="11">
+        <v>316</v>
+      </c>
+      <c r="NV12" s="11">
+        <v>314</v>
+      </c>
+      <c r="NW12" s="11">
+        <v>314</v>
+      </c>
     </row>
-    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -17775,8 +18032,29 @@
       <c r="NP13" s="11">
         <v>145</v>
       </c>
+      <c r="NQ13" s="11">
+        <v>145</v>
+      </c>
+      <c r="NR13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NS13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NT13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NU13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NV13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NW13" s="11">
+        <v>145</v>
+      </c>
     </row>
-    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -18917,8 +19195,29 @@
       <c r="NP14" s="11">
         <v>43</v>
       </c>
+      <c r="NQ14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NR14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NS14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NT14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NU14" s="11">
+        <v>43</v>
+      </c>
+      <c r="NV14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NW14" s="11">
+        <v>46</v>
+      </c>
     </row>
-    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -20059,8 +20358,29 @@
       <c r="NP15" s="11">
         <v>129</v>
       </c>
+      <c r="NQ15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NR15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NS15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NT15" s="11">
+        <v>124</v>
+      </c>
+      <c r="NU15" s="11">
+        <v>128</v>
+      </c>
+      <c r="NV15" s="11">
+        <v>128</v>
+      </c>
+      <c r="NW15" s="11">
+        <v>128</v>
+      </c>
     </row>
-    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -21201,8 +21521,29 @@
       <c r="NP16" s="11">
         <v>10</v>
       </c>
+      <c r="NQ16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NR16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NS16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NT16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NU16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NV16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NW16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -22343,8 +22684,29 @@
       <c r="NP17" s="11">
         <v>42</v>
       </c>
+      <c r="NQ17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NR17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NS17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NT17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NU17" s="11">
+        <v>42</v>
+      </c>
+      <c r="NV17" s="11">
+        <v>41</v>
+      </c>
+      <c r="NW17" s="11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="18" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -23520,7 +23882,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:NP18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:NW18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -23591,9 +23953,37 @@
         <f t="shared" si="7"/>
         <v>4512</v>
       </c>
+      <c r="NQ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4518</v>
+      </c>
+      <c r="NR18" s="6">
+        <f t="shared" si="7"/>
+        <v>4525</v>
+      </c>
+      <c r="NS18" s="6">
+        <f t="shared" si="7"/>
+        <v>4538</v>
+      </c>
+      <c r="NT18" s="6">
+        <f t="shared" si="7"/>
+        <v>4539</v>
+      </c>
+      <c r="NU18" s="6">
+        <f t="shared" si="7"/>
+        <v>4541</v>
+      </c>
+      <c r="NV18" s="6">
+        <f t="shared" si="7"/>
+        <v>4535</v>
+      </c>
+      <c r="NW18" s="6">
+        <f t="shared" si="7"/>
+        <v>4536</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:380 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -23611,12 +24001,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NP36"/>
+  <dimension ref="A1:NW36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NO1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
+      <selection pane="topRight" activeCell="NW2" sqref="NW2:NW17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23636,7 +24026,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -24777,8 +25167,29 @@
       <c r="NP1" s="8">
         <v>44313</v>
       </c>
+      <c r="NQ1" s="8">
+        <v>44314</v>
+      </c>
+      <c r="NR1" s="8">
+        <v>44315</v>
+      </c>
+      <c r="NS1" s="8">
+        <v>44316</v>
+      </c>
+      <c r="NT1" s="8">
+        <v>44317</v>
+      </c>
+      <c r="NU1" s="8">
+        <v>44318</v>
+      </c>
+      <c r="NV1" s="8">
+        <v>44319</v>
+      </c>
+      <c r="NW1" s="8">
+        <v>44320</v>
+      </c>
     </row>
-    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -25919,8 +26330,29 @@
       <c r="NP2">
         <v>36</v>
       </c>
+      <c r="NQ2">
+        <v>38</v>
+      </c>
+      <c r="NR2">
+        <v>35</v>
+      </c>
+      <c r="NS2">
+        <v>36</v>
+      </c>
+      <c r="NT2">
+        <v>38</v>
+      </c>
+      <c r="NU2">
+        <v>38</v>
+      </c>
+      <c r="NV2">
+        <v>37</v>
+      </c>
+      <c r="NW2">
+        <v>37</v>
+      </c>
     </row>
-    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -27061,8 +27493,29 @@
       <c r="NP3">
         <v>60</v>
       </c>
+      <c r="NQ3">
+        <v>59</v>
+      </c>
+      <c r="NR3">
+        <v>58</v>
+      </c>
+      <c r="NS3">
+        <v>58</v>
+      </c>
+      <c r="NT3">
+        <v>57</v>
+      </c>
+      <c r="NU3">
+        <v>57</v>
+      </c>
+      <c r="NV3">
+        <v>58</v>
+      </c>
+      <c r="NW3">
+        <v>59</v>
+      </c>
     </row>
-    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -28203,8 +28656,29 @@
       <c r="NP4">
         <v>152</v>
       </c>
+      <c r="NQ4">
+        <v>163</v>
+      </c>
+      <c r="NR4">
+        <v>163</v>
+      </c>
+      <c r="NS4">
+        <v>161</v>
+      </c>
+      <c r="NT4">
+        <v>162</v>
+      </c>
+      <c r="NU4">
+        <v>159</v>
+      </c>
+      <c r="NV4">
+        <v>159</v>
+      </c>
+      <c r="NW4">
+        <v>160</v>
+      </c>
     </row>
-    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -29345,8 +29819,29 @@
       <c r="NP5">
         <v>28</v>
       </c>
+      <c r="NQ5">
+        <v>29</v>
+      </c>
+      <c r="NR5">
+        <v>30</v>
+      </c>
+      <c r="NS5">
+        <v>31</v>
+      </c>
+      <c r="NT5">
+        <v>29</v>
+      </c>
+      <c r="NU5">
+        <v>29</v>
+      </c>
+      <c r="NV5">
+        <v>29</v>
+      </c>
+      <c r="NW5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -30487,8 +30982,29 @@
       <c r="NP6">
         <v>135</v>
       </c>
+      <c r="NQ6">
+        <v>135</v>
+      </c>
+      <c r="NR6">
+        <v>130</v>
+      </c>
+      <c r="NS6">
+        <v>128</v>
+      </c>
+      <c r="NT6">
+        <v>131</v>
+      </c>
+      <c r="NU6">
+        <v>126</v>
+      </c>
+      <c r="NV6">
+        <v>127</v>
+      </c>
+      <c r="NW6">
+        <v>133</v>
+      </c>
     </row>
-    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -31629,8 +32145,29 @@
       <c r="NP7">
         <v>334</v>
       </c>
+      <c r="NQ7">
+        <v>335</v>
+      </c>
+      <c r="NR7">
+        <v>339</v>
+      </c>
+      <c r="NS7">
+        <v>332</v>
+      </c>
+      <c r="NT7">
+        <v>336</v>
+      </c>
+      <c r="NU7">
+        <v>332</v>
+      </c>
+      <c r="NV7">
+        <v>331</v>
+      </c>
+      <c r="NW7">
+        <v>329</v>
+      </c>
     </row>
-    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -32771,8 +33308,29 @@
       <c r="NP8">
         <v>2508</v>
       </c>
+      <c r="NQ8">
+        <v>2505</v>
+      </c>
+      <c r="NR8">
+        <v>2521</v>
+      </c>
+      <c r="NS8">
+        <v>2513</v>
+      </c>
+      <c r="NT8">
+        <v>2504</v>
+      </c>
+      <c r="NU8">
+        <v>2516</v>
+      </c>
+      <c r="NV8">
+        <v>2513</v>
+      </c>
+      <c r="NW8">
+        <v>2522</v>
+      </c>
     </row>
-    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -33913,8 +34471,29 @@
       <c r="NP9">
         <v>179</v>
       </c>
+      <c r="NQ9">
+        <v>180</v>
+      </c>
+      <c r="NR9">
+        <v>183</v>
+      </c>
+      <c r="NS9">
+        <v>189</v>
+      </c>
+      <c r="NT9">
+        <v>181</v>
+      </c>
+      <c r="NU9">
+        <v>178</v>
+      </c>
+      <c r="NV9">
+        <v>175</v>
+      </c>
+      <c r="NW9">
+        <v>171</v>
+      </c>
     </row>
-    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -35055,8 +35634,29 @@
       <c r="NP10">
         <v>158</v>
       </c>
+      <c r="NQ10">
+        <v>159</v>
+      </c>
+      <c r="NR10">
+        <v>158</v>
+      </c>
+      <c r="NS10">
+        <v>158</v>
+      </c>
+      <c r="NT10">
+        <v>161</v>
+      </c>
+      <c r="NU10">
+        <v>159</v>
+      </c>
+      <c r="NV10">
+        <v>155</v>
+      </c>
+      <c r="NW10">
+        <v>155</v>
+      </c>
     </row>
-    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -36197,8 +36797,29 @@
       <c r="NP11">
         <v>68</v>
       </c>
+      <c r="NQ11">
+        <v>67</v>
+      </c>
+      <c r="NR11">
+        <v>66</v>
+      </c>
+      <c r="NS11">
+        <v>67</v>
+      </c>
+      <c r="NT11">
+        <v>69</v>
+      </c>
+      <c r="NU11">
+        <v>66</v>
+      </c>
+      <c r="NV11">
+        <v>68</v>
+      </c>
+      <c r="NW11">
+        <v>69</v>
+      </c>
     </row>
-    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -37339,8 +37960,29 @@
       <c r="NP12">
         <v>292</v>
       </c>
+      <c r="NQ12">
+        <v>289</v>
+      </c>
+      <c r="NR12">
+        <v>285</v>
+      </c>
+      <c r="NS12">
+        <v>277</v>
+      </c>
+      <c r="NT12">
+        <v>286</v>
+      </c>
+      <c r="NU12">
+        <v>282</v>
+      </c>
+      <c r="NV12">
+        <v>291</v>
+      </c>
+      <c r="NW12">
+        <v>288</v>
+      </c>
     </row>
-    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -38481,8 +39123,29 @@
       <c r="NP13">
         <v>140</v>
       </c>
+      <c r="NQ13">
+        <v>141</v>
+      </c>
+      <c r="NR13">
+        <v>138</v>
+      </c>
+      <c r="NS13">
+        <v>140</v>
+      </c>
+      <c r="NT13">
+        <v>144</v>
+      </c>
+      <c r="NU13">
+        <v>142</v>
+      </c>
+      <c r="NV13">
+        <v>143</v>
+      </c>
+      <c r="NW13">
+        <v>139</v>
+      </c>
     </row>
-    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -39623,8 +40286,29 @@
       <c r="NP14">
         <v>41</v>
       </c>
+      <c r="NQ14">
+        <v>38</v>
+      </c>
+      <c r="NR14">
+        <v>42</v>
+      </c>
+      <c r="NS14">
+        <v>38</v>
+      </c>
+      <c r="NT14">
+        <v>41</v>
+      </c>
+      <c r="NU14">
+        <v>40</v>
+      </c>
+      <c r="NV14">
+        <v>42</v>
+      </c>
+      <c r="NW14">
+        <v>43</v>
+      </c>
     </row>
-    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -40765,8 +41449,29 @@
       <c r="NP15">
         <v>118</v>
       </c>
+      <c r="NQ15">
+        <v>123</v>
+      </c>
+      <c r="NR15">
+        <v>124</v>
+      </c>
+      <c r="NS15">
+        <v>115</v>
+      </c>
+      <c r="NT15">
+        <v>119</v>
+      </c>
+      <c r="NU15">
+        <v>116</v>
+      </c>
+      <c r="NV15">
+        <v>120</v>
+      </c>
+      <c r="NW15">
+        <v>120</v>
+      </c>
     </row>
-    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -41907,8 +42612,29 @@
       <c r="NP16">
         <v>10</v>
       </c>
+      <c r="NQ16">
+        <v>9</v>
+      </c>
+      <c r="NR16">
+        <v>8</v>
+      </c>
+      <c r="NS16">
+        <v>9</v>
+      </c>
+      <c r="NT16">
+        <v>9</v>
+      </c>
+      <c r="NU16">
+        <v>10</v>
+      </c>
+      <c r="NV16">
+        <v>10</v>
+      </c>
+      <c r="NW16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -43049,8 +43775,29 @@
       <c r="NP17">
         <v>36</v>
       </c>
+      <c r="NQ17">
+        <v>34</v>
+      </c>
+      <c r="NR17">
+        <v>35</v>
+      </c>
+      <c r="NS17">
+        <v>34</v>
+      </c>
+      <c r="NT17">
+        <v>34</v>
+      </c>
+      <c r="NU17">
+        <v>34</v>
+      </c>
+      <c r="NV17">
+        <v>37</v>
+      </c>
+      <c r="NW17">
+        <v>38</v>
+      </c>
     </row>
-    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -44142,7 +44889,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:NP18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:NW18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -44277,8 +45024,36 @@
         <f t="shared" si="1"/>
         <v>4295</v>
       </c>
+      <c r="NQ18" s="6">
+        <f t="shared" si="1"/>
+        <v>4304</v>
+      </c>
+      <c r="NR18" s="6">
+        <f t="shared" si="1"/>
+        <v>4315</v>
+      </c>
+      <c r="NS18" s="6">
+        <f t="shared" si="1"/>
+        <v>4286</v>
+      </c>
+      <c r="NT18" s="6">
+        <f t="shared" si="1"/>
+        <v>4301</v>
+      </c>
+      <c r="NU18" s="6">
+        <f t="shared" si="1"/>
+        <v>4284</v>
+      </c>
+      <c r="NV18" s="6">
+        <f t="shared" si="1"/>
+        <v>4295</v>
+      </c>
+      <c r="NW18" s="6">
+        <f t="shared" si="1"/>
+        <v>4305</v>
+      </c>
     </row>
-    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -44561,7 +45336,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -44844,7 +45619,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -45127,7 +45902,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -45410,7 +46185,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -45693,7 +46468,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -45976,7 +46751,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -46259,7 +47034,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -46542,7 +47317,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -46825,7 +47600,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -47108,7 +47883,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -47391,7 +48166,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -47674,7 +48449,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -49097,12 +49872,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NP34"/>
+  <dimension ref="A1:NW34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NM1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NL18" sqref="NL18"/>
+      <selection pane="topRight" activeCell="NQ18" sqref="NQ18:NW18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49123,7 +49898,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -50264,8 +51039,29 @@
       <c r="NP1" s="8">
         <v>44313</v>
       </c>
+      <c r="NQ1" s="8">
+        <v>44314</v>
+      </c>
+      <c r="NR1" s="8">
+        <v>44315</v>
+      </c>
+      <c r="NS1" s="8">
+        <v>44316</v>
+      </c>
+      <c r="NT1" s="8">
+        <v>44317</v>
+      </c>
+      <c r="NU1" s="8">
+        <v>44318</v>
+      </c>
+      <c r="NV1" s="8">
+        <v>44319</v>
+      </c>
+      <c r="NW1" s="8">
+        <v>44320</v>
+      </c>
     </row>
-    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -51406,8 +52202,29 @@
       <c r="NP2">
         <v>32</v>
       </c>
+      <c r="NQ2">
+        <v>31</v>
+      </c>
+      <c r="NR2">
+        <v>29</v>
+      </c>
+      <c r="NS2">
+        <v>31</v>
+      </c>
+      <c r="NT2">
+        <v>32</v>
+      </c>
+      <c r="NU2">
+        <v>32</v>
+      </c>
+      <c r="NV2">
+        <v>31</v>
+      </c>
+      <c r="NW2">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -52548,8 +53365,29 @@
       <c r="NP3">
         <v>58</v>
       </c>
+      <c r="NQ3">
+        <v>55</v>
+      </c>
+      <c r="NR3">
+        <v>55</v>
+      </c>
+      <c r="NS3">
+        <v>54</v>
+      </c>
+      <c r="NT3">
+        <v>56</v>
+      </c>
+      <c r="NU3">
+        <v>54</v>
+      </c>
+      <c r="NV3">
+        <v>54</v>
+      </c>
+      <c r="NW3">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -53690,8 +54528,29 @@
       <c r="NP4">
         <v>95</v>
       </c>
+      <c r="NQ4">
+        <v>103</v>
+      </c>
+      <c r="NR4">
+        <v>113</v>
+      </c>
+      <c r="NS4">
+        <v>103</v>
+      </c>
+      <c r="NT4">
+        <v>102</v>
+      </c>
+      <c r="NU4">
+        <v>104</v>
+      </c>
+      <c r="NV4">
+        <v>103</v>
+      </c>
+      <c r="NW4">
+        <v>105</v>
+      </c>
     </row>
-    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -54832,8 +55691,29 @@
       <c r="NP5">
         <v>25</v>
       </c>
+      <c r="NQ5">
+        <v>25</v>
+      </c>
+      <c r="NR5">
+        <v>26</v>
+      </c>
+      <c r="NS5">
+        <v>27</v>
+      </c>
+      <c r="NT5">
+        <v>25</v>
+      </c>
+      <c r="NU5">
+        <v>24</v>
+      </c>
+      <c r="NV5">
+        <v>22</v>
+      </c>
+      <c r="NW5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -55974,8 +56854,29 @@
       <c r="NP6">
         <v>106</v>
       </c>
+      <c r="NQ6">
+        <v>100</v>
+      </c>
+      <c r="NR6">
+        <v>104</v>
+      </c>
+      <c r="NS6">
+        <v>101</v>
+      </c>
+      <c r="NT6">
+        <v>102</v>
+      </c>
+      <c r="NU6">
+        <v>103</v>
+      </c>
+      <c r="NV6">
+        <v>102</v>
+      </c>
+      <c r="NW6">
+        <v>103</v>
+      </c>
     </row>
-    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -57116,8 +58017,29 @@
       <c r="NP7">
         <v>272</v>
       </c>
+      <c r="NQ7">
+        <v>273</v>
+      </c>
+      <c r="NR7">
+        <v>273</v>
+      </c>
+      <c r="NS7">
+        <v>272</v>
+      </c>
+      <c r="NT7">
+        <v>274</v>
+      </c>
+      <c r="NU7">
+        <v>266</v>
+      </c>
+      <c r="NV7">
+        <v>265</v>
+      </c>
+      <c r="NW7">
+        <v>266</v>
+      </c>
     </row>
-    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -58258,8 +59180,29 @@
       <c r="NP8">
         <v>1987</v>
       </c>
+      <c r="NQ8">
+        <v>1964</v>
+      </c>
+      <c r="NR8">
+        <v>1976</v>
+      </c>
+      <c r="NS8">
+        <v>1947</v>
+      </c>
+      <c r="NT8">
+        <v>1918</v>
+      </c>
+      <c r="NU8">
+        <v>1930</v>
+      </c>
+      <c r="NV8">
+        <v>1912</v>
+      </c>
+      <c r="NW8">
+        <v>1913</v>
+      </c>
     </row>
-    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -59400,8 +60343,29 @@
       <c r="NP9">
         <v>156</v>
       </c>
+      <c r="NQ9">
+        <v>157</v>
+      </c>
+      <c r="NR9">
+        <v>157</v>
+      </c>
+      <c r="NS9">
+        <v>155</v>
+      </c>
+      <c r="NT9">
+        <v>159</v>
+      </c>
+      <c r="NU9">
+        <v>151</v>
+      </c>
+      <c r="NV9">
+        <v>151</v>
+      </c>
+      <c r="NW9">
+        <v>149</v>
+      </c>
     </row>
-    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -60542,8 +61506,29 @@
       <c r="NP10">
         <v>136</v>
       </c>
+      <c r="NQ10">
+        <v>138</v>
+      </c>
+      <c r="NR10">
+        <v>139</v>
+      </c>
+      <c r="NS10">
+        <v>137</v>
+      </c>
+      <c r="NT10">
+        <v>140</v>
+      </c>
+      <c r="NU10">
+        <v>135</v>
+      </c>
+      <c r="NV10">
+        <v>136</v>
+      </c>
+      <c r="NW10">
+        <v>135</v>
+      </c>
     </row>
-    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -61684,8 +62669,29 @@
       <c r="NP11">
         <v>52</v>
       </c>
+      <c r="NQ11">
+        <v>51</v>
+      </c>
+      <c r="NR11">
+        <v>50</v>
+      </c>
+      <c r="NS11">
+        <v>51</v>
+      </c>
+      <c r="NT11">
+        <v>52</v>
+      </c>
+      <c r="NU11">
+        <v>49</v>
+      </c>
+      <c r="NV11">
+        <v>51</v>
+      </c>
+      <c r="NW11">
+        <v>53</v>
+      </c>
     </row>
-    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -62826,8 +63832,29 @@
       <c r="NP12">
         <v>226</v>
       </c>
+      <c r="NQ12">
+        <v>221</v>
+      </c>
+      <c r="NR12">
+        <v>213</v>
+      </c>
+      <c r="NS12">
+        <v>203</v>
+      </c>
+      <c r="NT12">
+        <v>212</v>
+      </c>
+      <c r="NU12">
+        <v>209</v>
+      </c>
+      <c r="NV12">
+        <v>214</v>
+      </c>
+      <c r="NW12">
+        <v>218</v>
+      </c>
     </row>
-    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -63968,8 +64995,29 @@
       <c r="NP13">
         <v>113</v>
       </c>
+      <c r="NQ13">
+        <v>112</v>
+      </c>
+      <c r="NR13">
+        <v>112</v>
+      </c>
+      <c r="NS13">
+        <v>116</v>
+      </c>
+      <c r="NT13">
+        <v>114</v>
+      </c>
+      <c r="NU13">
+        <v>115</v>
+      </c>
+      <c r="NV13">
+        <v>115</v>
+      </c>
+      <c r="NW13">
+        <v>106</v>
+      </c>
     </row>
-    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -65110,8 +66158,29 @@
       <c r="NP14">
         <v>29</v>
       </c>
+      <c r="NQ14">
+        <v>26</v>
+      </c>
+      <c r="NR14">
+        <v>30</v>
+      </c>
+      <c r="NS14">
+        <v>28</v>
+      </c>
+      <c r="NT14">
+        <v>31</v>
+      </c>
+      <c r="NU14">
+        <v>29</v>
+      </c>
+      <c r="NV14">
+        <v>31</v>
+      </c>
+      <c r="NW14">
+        <v>27</v>
+      </c>
     </row>
-    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -66252,8 +67321,29 @@
       <c r="NP15">
         <v>87</v>
       </c>
+      <c r="NQ15">
+        <v>88</v>
+      </c>
+      <c r="NR15">
+        <v>86</v>
+      </c>
+      <c r="NS15">
+        <v>87</v>
+      </c>
+      <c r="NT15">
+        <v>85</v>
+      </c>
+      <c r="NU15">
+        <v>85</v>
+      </c>
+      <c r="NV15">
+        <v>84</v>
+      </c>
+      <c r="NW15">
+        <v>83</v>
+      </c>
     </row>
-    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -67394,8 +68484,29 @@
       <c r="NP16">
         <v>8</v>
       </c>
+      <c r="NQ16">
+        <v>7</v>
+      </c>
+      <c r="NR16">
+        <v>6</v>
+      </c>
+      <c r="NS16">
+        <v>7</v>
+      </c>
+      <c r="NT16">
+        <v>7</v>
+      </c>
+      <c r="NU16">
+        <v>6</v>
+      </c>
+      <c r="NV16">
+        <v>6</v>
+      </c>
+      <c r="NW16">
+        <v>7</v>
+      </c>
     </row>
-    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -68536,8 +69647,29 @@
       <c r="NP17">
         <v>24</v>
       </c>
+      <c r="NQ17">
+        <v>25</v>
+      </c>
+      <c r="NR17">
+        <v>27</v>
+      </c>
+      <c r="NS17">
+        <v>26</v>
+      </c>
+      <c r="NT17">
+        <v>27</v>
+      </c>
+      <c r="NU17">
+        <v>26</v>
+      </c>
+      <c r="NV17">
+        <v>26</v>
+      </c>
+      <c r="NW17">
+        <v>28</v>
+      </c>
     </row>
-    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -69674,7 +70806,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:NP18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:NW18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -69769,50 +70901,78 @@
         <f t="shared" si="1"/>
         <v>3406</v>
       </c>
+      <c r="NQ18" s="6">
+        <f t="shared" si="1"/>
+        <v>3376</v>
+      </c>
+      <c r="NR18" s="6">
+        <f t="shared" si="1"/>
+        <v>3396</v>
+      </c>
+      <c r="NS18" s="6">
+        <f t="shared" si="1"/>
+        <v>3345</v>
+      </c>
+      <c r="NT18" s="6">
+        <f t="shared" si="1"/>
+        <v>3336</v>
+      </c>
+      <c r="NU18" s="6">
+        <f t="shared" si="1"/>
+        <v>3318</v>
+      </c>
+      <c r="NV18" s="6">
+        <f t="shared" si="1"/>
+        <v>3303</v>
+      </c>
+      <c r="NW18" s="6">
+        <f t="shared" si="1"/>
+        <v>3303</v>
+      </c>
     </row>
-    <row r="19" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -69832,12 +70992,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:NP34"/>
+  <dimension ref="A1:NW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NI1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NO1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="NR15" sqref="NR15"/>
+      <selection pane="topRight" activeCell="NY12" sqref="NY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69855,7 +71015,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -70996,8 +72156,29 @@
       <c r="NP1" s="8">
         <v>44313</v>
       </c>
+      <c r="NQ1" s="8">
+        <v>44314</v>
+      </c>
+      <c r="NR1" s="8">
+        <v>44315</v>
+      </c>
+      <c r="NS1" s="8">
+        <v>44316</v>
+      </c>
+      <c r="NT1" s="8">
+        <v>44317</v>
+      </c>
+      <c r="NU1" s="8">
+        <v>44318</v>
+      </c>
+      <c r="NV1" s="8">
+        <v>44319</v>
+      </c>
+      <c r="NW1" s="8">
+        <v>44320</v>
+      </c>
     </row>
-    <row r="2" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -72237,8 +73418,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP2-'UCI OCUPADA COVID'!NP2</f>
         <v>4</v>
       </c>
+      <c r="NQ2">
+        <f>+'UCI OCUPADA TOTAL'!NQ2-'UCI OCUPADA COVID'!NQ2</f>
+        <v>7</v>
+      </c>
+      <c r="NR2">
+        <f>+'UCI OCUPADA TOTAL'!NR2-'UCI OCUPADA COVID'!NR2</f>
+        <v>6</v>
+      </c>
+      <c r="NS2">
+        <f>+'UCI OCUPADA TOTAL'!NS2-'UCI OCUPADA COVID'!NS2</f>
+        <v>5</v>
+      </c>
+      <c r="NT2">
+        <f>+'UCI OCUPADA TOTAL'!NT2-'UCI OCUPADA COVID'!NT2</f>
+        <v>6</v>
+      </c>
+      <c r="NU2">
+        <f>+'UCI OCUPADA TOTAL'!NU2-'UCI OCUPADA COVID'!NU2</f>
+        <v>6</v>
+      </c>
+      <c r="NV2">
+        <f>+'UCI OCUPADA TOTAL'!NV2-'UCI OCUPADA COVID'!NV2</f>
+        <v>6</v>
+      </c>
+      <c r="NW2">
+        <f>+'UCI OCUPADA TOTAL'!NW2-'UCI OCUPADA COVID'!NW2</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -73478,8 +74687,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP3-'UCI OCUPADA COVID'!NP3</f>
         <v>2</v>
       </c>
+      <c r="NQ3">
+        <f>+'UCI OCUPADA TOTAL'!NQ3-'UCI OCUPADA COVID'!NQ3</f>
+        <v>4</v>
+      </c>
+      <c r="NR3">
+        <f>+'UCI OCUPADA TOTAL'!NR3-'UCI OCUPADA COVID'!NR3</f>
+        <v>3</v>
+      </c>
+      <c r="NS3">
+        <f>+'UCI OCUPADA TOTAL'!NS3-'UCI OCUPADA COVID'!NS3</f>
+        <v>4</v>
+      </c>
+      <c r="NT3">
+        <f>+'UCI OCUPADA TOTAL'!NT3-'UCI OCUPADA COVID'!NT3</f>
+        <v>1</v>
+      </c>
+      <c r="NU3">
+        <f>+'UCI OCUPADA TOTAL'!NU3-'UCI OCUPADA COVID'!NU3</f>
+        <v>3</v>
+      </c>
+      <c r="NV3">
+        <f>+'UCI OCUPADA TOTAL'!NV3-'UCI OCUPADA COVID'!NV3</f>
+        <v>4</v>
+      </c>
+      <c r="NW3">
+        <f>+'UCI OCUPADA TOTAL'!NW3-'UCI OCUPADA COVID'!NW3</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -74719,8 +75956,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP4-'UCI OCUPADA COVID'!NP4</f>
         <v>57</v>
       </c>
+      <c r="NQ4">
+        <f>+'UCI OCUPADA TOTAL'!NQ4-'UCI OCUPADA COVID'!NQ4</f>
+        <v>60</v>
+      </c>
+      <c r="NR4">
+        <f>+'UCI OCUPADA TOTAL'!NR4-'UCI OCUPADA COVID'!NR4</f>
+        <v>50</v>
+      </c>
+      <c r="NS4">
+        <f>+'UCI OCUPADA TOTAL'!NS4-'UCI OCUPADA COVID'!NS4</f>
+        <v>58</v>
+      </c>
+      <c r="NT4">
+        <f>+'UCI OCUPADA TOTAL'!NT4-'UCI OCUPADA COVID'!NT4</f>
+        <v>60</v>
+      </c>
+      <c r="NU4">
+        <f>+'UCI OCUPADA TOTAL'!NU4-'UCI OCUPADA COVID'!NU4</f>
+        <v>55</v>
+      </c>
+      <c r="NV4">
+        <f>+'UCI OCUPADA TOTAL'!NV4-'UCI OCUPADA COVID'!NV4</f>
+        <v>56</v>
+      </c>
+      <c r="NW4">
+        <f>+'UCI OCUPADA TOTAL'!NW4-'UCI OCUPADA COVID'!NW4</f>
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -75960,8 +77225,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP5-'UCI OCUPADA COVID'!NP5</f>
         <v>3</v>
       </c>
+      <c r="NQ5">
+        <f>+'UCI OCUPADA TOTAL'!NQ5-'UCI OCUPADA COVID'!NQ5</f>
+        <v>4</v>
+      </c>
+      <c r="NR5">
+        <f>+'UCI OCUPADA TOTAL'!NR5-'UCI OCUPADA COVID'!NR5</f>
+        <v>4</v>
+      </c>
+      <c r="NS5">
+        <f>+'UCI OCUPADA TOTAL'!NS5-'UCI OCUPADA COVID'!NS5</f>
+        <v>4</v>
+      </c>
+      <c r="NT5">
+        <f>+'UCI OCUPADA TOTAL'!NT5-'UCI OCUPADA COVID'!NT5</f>
+        <v>4</v>
+      </c>
+      <c r="NU5">
+        <f>+'UCI OCUPADA TOTAL'!NU5-'UCI OCUPADA COVID'!NU5</f>
+        <v>5</v>
+      </c>
+      <c r="NV5">
+        <f>+'UCI OCUPADA TOTAL'!NV5-'UCI OCUPADA COVID'!NV5</f>
+        <v>7</v>
+      </c>
+      <c r="NW5">
+        <f>+'UCI OCUPADA TOTAL'!NW5-'UCI OCUPADA COVID'!NW5</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -77201,8 +78494,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP6-'UCI OCUPADA COVID'!NP6</f>
         <v>29</v>
       </c>
+      <c r="NQ6">
+        <f>+'UCI OCUPADA TOTAL'!NQ6-'UCI OCUPADA COVID'!NQ6</f>
+        <v>35</v>
+      </c>
+      <c r="NR6">
+        <f>+'UCI OCUPADA TOTAL'!NR6-'UCI OCUPADA COVID'!NR6</f>
+        <v>26</v>
+      </c>
+      <c r="NS6">
+        <f>+'UCI OCUPADA TOTAL'!NS6-'UCI OCUPADA COVID'!NS6</f>
+        <v>27</v>
+      </c>
+      <c r="NT6">
+        <f>+'UCI OCUPADA TOTAL'!NT6-'UCI OCUPADA COVID'!NT6</f>
+        <v>29</v>
+      </c>
+      <c r="NU6">
+        <f>+'UCI OCUPADA TOTAL'!NU6-'UCI OCUPADA COVID'!NU6</f>
+        <v>23</v>
+      </c>
+      <c r="NV6">
+        <f>+'UCI OCUPADA TOTAL'!NV6-'UCI OCUPADA COVID'!NV6</f>
+        <v>25</v>
+      </c>
+      <c r="NW6">
+        <f>+'UCI OCUPADA TOTAL'!NW6-'UCI OCUPADA COVID'!NW6</f>
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -78442,8 +79763,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP7-'UCI OCUPADA COVID'!NP7</f>
         <v>62</v>
       </c>
+      <c r="NQ7">
+        <f>+'UCI OCUPADA TOTAL'!NQ7-'UCI OCUPADA COVID'!NQ7</f>
+        <v>62</v>
+      </c>
+      <c r="NR7">
+        <f>+'UCI OCUPADA TOTAL'!NR7-'UCI OCUPADA COVID'!NR7</f>
+        <v>66</v>
+      </c>
+      <c r="NS7">
+        <f>+'UCI OCUPADA TOTAL'!NS7-'UCI OCUPADA COVID'!NS7</f>
+        <v>60</v>
+      </c>
+      <c r="NT7">
+        <f>+'UCI OCUPADA TOTAL'!NT7-'UCI OCUPADA COVID'!NT7</f>
+        <v>62</v>
+      </c>
+      <c r="NU7">
+        <f>+'UCI OCUPADA TOTAL'!NU7-'UCI OCUPADA COVID'!NU7</f>
+        <v>66</v>
+      </c>
+      <c r="NV7">
+        <f>+'UCI OCUPADA TOTAL'!NV7-'UCI OCUPADA COVID'!NV7</f>
+        <v>66</v>
+      </c>
+      <c r="NW7">
+        <f>+'UCI OCUPADA TOTAL'!NW7-'UCI OCUPADA COVID'!NW7</f>
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -79683,8 +81032,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP8-'UCI OCUPADA COVID'!NP8</f>
         <v>521</v>
       </c>
+      <c r="NQ8">
+        <f>+'UCI OCUPADA TOTAL'!NQ8-'UCI OCUPADA COVID'!NQ8</f>
+        <v>541</v>
+      </c>
+      <c r="NR8">
+        <f>+'UCI OCUPADA TOTAL'!NR8-'UCI OCUPADA COVID'!NR8</f>
+        <v>545</v>
+      </c>
+      <c r="NS8">
+        <f>+'UCI OCUPADA TOTAL'!NS8-'UCI OCUPADA COVID'!NS8</f>
+        <v>566</v>
+      </c>
+      <c r="NT8">
+        <f>+'UCI OCUPADA TOTAL'!NT8-'UCI OCUPADA COVID'!NT8</f>
+        <v>586</v>
+      </c>
+      <c r="NU8">
+        <f>+'UCI OCUPADA TOTAL'!NU8-'UCI OCUPADA COVID'!NU8</f>
+        <v>586</v>
+      </c>
+      <c r="NV8">
+        <f>+'UCI OCUPADA TOTAL'!NV8-'UCI OCUPADA COVID'!NV8</f>
+        <v>601</v>
+      </c>
+      <c r="NW8">
+        <f>+'UCI OCUPADA TOTAL'!NW8-'UCI OCUPADA COVID'!NW8</f>
+        <v>609</v>
+      </c>
     </row>
-    <row r="9" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -80924,8 +82301,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP9-'UCI OCUPADA COVID'!NP9</f>
         <v>23</v>
       </c>
+      <c r="NQ9">
+        <f>+'UCI OCUPADA TOTAL'!NQ9-'UCI OCUPADA COVID'!NQ9</f>
+        <v>23</v>
+      </c>
+      <c r="NR9">
+        <f>+'UCI OCUPADA TOTAL'!NR9-'UCI OCUPADA COVID'!NR9</f>
+        <v>26</v>
+      </c>
+      <c r="NS9">
+        <f>+'UCI OCUPADA TOTAL'!NS9-'UCI OCUPADA COVID'!NS9</f>
+        <v>34</v>
+      </c>
+      <c r="NT9">
+        <f>+'UCI OCUPADA TOTAL'!NT9-'UCI OCUPADA COVID'!NT9</f>
+        <v>22</v>
+      </c>
+      <c r="NU9">
+        <f>+'UCI OCUPADA TOTAL'!NU9-'UCI OCUPADA COVID'!NU9</f>
+        <v>27</v>
+      </c>
+      <c r="NV9">
+        <f>+'UCI OCUPADA TOTAL'!NV9-'UCI OCUPADA COVID'!NV9</f>
+        <v>24</v>
+      </c>
+      <c r="NW9">
+        <f>+'UCI OCUPADA TOTAL'!NW9-'UCI OCUPADA COVID'!NW9</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -82165,8 +83570,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP10-'UCI OCUPADA COVID'!NP10</f>
         <v>22</v>
       </c>
+      <c r="NQ10">
+        <f>+'UCI OCUPADA TOTAL'!NQ10-'UCI OCUPADA COVID'!NQ10</f>
+        <v>21</v>
+      </c>
+      <c r="NR10">
+        <f>+'UCI OCUPADA TOTAL'!NR10-'UCI OCUPADA COVID'!NR10</f>
+        <v>19</v>
+      </c>
+      <c r="NS10">
+        <f>+'UCI OCUPADA TOTAL'!NS10-'UCI OCUPADA COVID'!NS10</f>
+        <v>21</v>
+      </c>
+      <c r="NT10">
+        <f>+'UCI OCUPADA TOTAL'!NT10-'UCI OCUPADA COVID'!NT10</f>
+        <v>21</v>
+      </c>
+      <c r="NU10">
+        <f>+'UCI OCUPADA TOTAL'!NU10-'UCI OCUPADA COVID'!NU10</f>
+        <v>24</v>
+      </c>
+      <c r="NV10">
+        <f>+'UCI OCUPADA TOTAL'!NV10-'UCI OCUPADA COVID'!NV10</f>
+        <v>19</v>
+      </c>
+      <c r="NW10">
+        <f>+'UCI OCUPADA TOTAL'!NW10-'UCI OCUPADA COVID'!NW10</f>
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -83406,8 +84839,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP11-'UCI OCUPADA COVID'!NP11</f>
         <v>16</v>
       </c>
+      <c r="NQ11">
+        <f>+'UCI OCUPADA TOTAL'!NQ11-'UCI OCUPADA COVID'!NQ11</f>
+        <v>16</v>
+      </c>
+      <c r="NR11">
+        <f>+'UCI OCUPADA TOTAL'!NR11-'UCI OCUPADA COVID'!NR11</f>
+        <v>16</v>
+      </c>
+      <c r="NS11">
+        <f>+'UCI OCUPADA TOTAL'!NS11-'UCI OCUPADA COVID'!NS11</f>
+        <v>16</v>
+      </c>
+      <c r="NT11">
+        <f>+'UCI OCUPADA TOTAL'!NT11-'UCI OCUPADA COVID'!NT11</f>
+        <v>17</v>
+      </c>
+      <c r="NU11">
+        <f>+'UCI OCUPADA TOTAL'!NU11-'UCI OCUPADA COVID'!NU11</f>
+        <v>17</v>
+      </c>
+      <c r="NV11">
+        <f>+'UCI OCUPADA TOTAL'!NV11-'UCI OCUPADA COVID'!NV11</f>
+        <v>17</v>
+      </c>
+      <c r="NW11">
+        <f>+'UCI OCUPADA TOTAL'!NW11-'UCI OCUPADA COVID'!NW11</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -84647,8 +86108,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP12-'UCI OCUPADA COVID'!NP12</f>
         <v>66</v>
       </c>
+      <c r="NQ12">
+        <f>+'UCI OCUPADA TOTAL'!NQ12-'UCI OCUPADA COVID'!NQ12</f>
+        <v>68</v>
+      </c>
+      <c r="NR12">
+        <f>+'UCI OCUPADA TOTAL'!NR12-'UCI OCUPADA COVID'!NR12</f>
+        <v>72</v>
+      </c>
+      <c r="NS12">
+        <f>+'UCI OCUPADA TOTAL'!NS12-'UCI OCUPADA COVID'!NS12</f>
+        <v>74</v>
+      </c>
+      <c r="NT12">
+        <f>+'UCI OCUPADA TOTAL'!NT12-'UCI OCUPADA COVID'!NT12</f>
+        <v>74</v>
+      </c>
+      <c r="NU12">
+        <f>+'UCI OCUPADA TOTAL'!NU12-'UCI OCUPADA COVID'!NU12</f>
+        <v>73</v>
+      </c>
+      <c r="NV12">
+        <f>+'UCI OCUPADA TOTAL'!NV12-'UCI OCUPADA COVID'!NV12</f>
+        <v>77</v>
+      </c>
+      <c r="NW12">
+        <f>+'UCI OCUPADA TOTAL'!NW12-'UCI OCUPADA COVID'!NW12</f>
+        <v>70</v>
+      </c>
     </row>
-    <row r="13" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -85888,8 +87377,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP13-'UCI OCUPADA COVID'!NP13</f>
         <v>27</v>
       </c>
+      <c r="NQ13">
+        <f>+'UCI OCUPADA TOTAL'!NQ13-'UCI OCUPADA COVID'!NQ13</f>
+        <v>29</v>
+      </c>
+      <c r="NR13">
+        <f>+'UCI OCUPADA TOTAL'!NR13-'UCI OCUPADA COVID'!NR13</f>
+        <v>26</v>
+      </c>
+      <c r="NS13">
+        <f>+'UCI OCUPADA TOTAL'!NS13-'UCI OCUPADA COVID'!NS13</f>
+        <v>24</v>
+      </c>
+      <c r="NT13">
+        <f>+'UCI OCUPADA TOTAL'!NT13-'UCI OCUPADA COVID'!NT13</f>
+        <v>30</v>
+      </c>
+      <c r="NU13">
+        <f>+'UCI OCUPADA TOTAL'!NU13-'UCI OCUPADA COVID'!NU13</f>
+        <v>27</v>
+      </c>
+      <c r="NV13">
+        <f>+'UCI OCUPADA TOTAL'!NV13-'UCI OCUPADA COVID'!NV13</f>
+        <v>28</v>
+      </c>
+      <c r="NW13">
+        <f>+'UCI OCUPADA TOTAL'!NW13-'UCI OCUPADA COVID'!NW13</f>
+        <v>33</v>
+      </c>
     </row>
-    <row r="14" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -87129,8 +88646,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP14-'UCI OCUPADA COVID'!NP14</f>
         <v>12</v>
       </c>
+      <c r="NQ14">
+        <f>+'UCI OCUPADA TOTAL'!NQ14-'UCI OCUPADA COVID'!NQ14</f>
+        <v>12</v>
+      </c>
+      <c r="NR14">
+        <f>+'UCI OCUPADA TOTAL'!NR14-'UCI OCUPADA COVID'!NR14</f>
+        <v>12</v>
+      </c>
+      <c r="NS14">
+        <f>+'UCI OCUPADA TOTAL'!NS14-'UCI OCUPADA COVID'!NS14</f>
+        <v>10</v>
+      </c>
+      <c r="NT14">
+        <f>+'UCI OCUPADA TOTAL'!NT14-'UCI OCUPADA COVID'!NT14</f>
+        <v>10</v>
+      </c>
+      <c r="NU14">
+        <f>+'UCI OCUPADA TOTAL'!NU14-'UCI OCUPADA COVID'!NU14</f>
+        <v>11</v>
+      </c>
+      <c r="NV14">
+        <f>+'UCI OCUPADA TOTAL'!NV14-'UCI OCUPADA COVID'!NV14</f>
+        <v>11</v>
+      </c>
+      <c r="NW14">
+        <f>+'UCI OCUPADA TOTAL'!NW14-'UCI OCUPADA COVID'!NW14</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="15" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -88370,8 +89915,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP15-'UCI OCUPADA COVID'!NP15</f>
         <v>31</v>
       </c>
+      <c r="NQ15">
+        <f>+'UCI OCUPADA TOTAL'!NQ15-'UCI OCUPADA COVID'!NQ15</f>
+        <v>35</v>
+      </c>
+      <c r="NR15">
+        <f>+'UCI OCUPADA TOTAL'!NR15-'UCI OCUPADA COVID'!NR15</f>
+        <v>38</v>
+      </c>
+      <c r="NS15">
+        <f>+'UCI OCUPADA TOTAL'!NS15-'UCI OCUPADA COVID'!NS15</f>
+        <v>28</v>
+      </c>
+      <c r="NT15">
+        <f>+'UCI OCUPADA TOTAL'!NT15-'UCI OCUPADA COVID'!NT15</f>
+        <v>34</v>
+      </c>
+      <c r="NU15">
+        <f>+'UCI OCUPADA TOTAL'!NU15-'UCI OCUPADA COVID'!NU15</f>
+        <v>31</v>
+      </c>
+      <c r="NV15">
+        <f>+'UCI OCUPADA TOTAL'!NV15-'UCI OCUPADA COVID'!NV15</f>
+        <v>36</v>
+      </c>
+      <c r="NW15">
+        <f>+'UCI OCUPADA TOTAL'!NW15-'UCI OCUPADA COVID'!NW15</f>
+        <v>37</v>
+      </c>
     </row>
-    <row r="16" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -89611,8 +91184,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP16-'UCI OCUPADA COVID'!NP16</f>
         <v>2</v>
       </c>
+      <c r="NQ16">
+        <f>+'UCI OCUPADA TOTAL'!NQ16-'UCI OCUPADA COVID'!NQ16</f>
+        <v>2</v>
+      </c>
+      <c r="NR16">
+        <f>+'UCI OCUPADA TOTAL'!NR16-'UCI OCUPADA COVID'!NR16</f>
+        <v>2</v>
+      </c>
+      <c r="NS16">
+        <f>+'UCI OCUPADA TOTAL'!NS16-'UCI OCUPADA COVID'!NS16</f>
+        <v>2</v>
+      </c>
+      <c r="NT16">
+        <f>+'UCI OCUPADA TOTAL'!NT16-'UCI OCUPADA COVID'!NT16</f>
+        <v>2</v>
+      </c>
+      <c r="NU16">
+        <f>+'UCI OCUPADA TOTAL'!NU16-'UCI OCUPADA COVID'!NU16</f>
+        <v>4</v>
+      </c>
+      <c r="NV16">
+        <f>+'UCI OCUPADA TOTAL'!NV16-'UCI OCUPADA COVID'!NV16</f>
+        <v>4</v>
+      </c>
+      <c r="NW16">
+        <f>+'UCI OCUPADA TOTAL'!NW16-'UCI OCUPADA COVID'!NW16</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -90852,8 +92453,36 @@
         <f>+'UCI OCUPADA TOTAL'!NP17-'UCI OCUPADA COVID'!NP17</f>
         <v>12</v>
       </c>
+      <c r="NQ17">
+        <f>+'UCI OCUPADA TOTAL'!NQ17-'UCI OCUPADA COVID'!NQ17</f>
+        <v>9</v>
+      </c>
+      <c r="NR17">
+        <f>+'UCI OCUPADA TOTAL'!NR17-'UCI OCUPADA COVID'!NR17</f>
+        <v>8</v>
+      </c>
+      <c r="NS17">
+        <f>+'UCI OCUPADA TOTAL'!NS17-'UCI OCUPADA COVID'!NS17</f>
+        <v>8</v>
+      </c>
+      <c r="NT17">
+        <f>+'UCI OCUPADA TOTAL'!NT17-'UCI OCUPADA COVID'!NT17</f>
+        <v>7</v>
+      </c>
+      <c r="NU17">
+        <f>+'UCI OCUPADA TOTAL'!NU17-'UCI OCUPADA COVID'!NU17</f>
+        <v>8</v>
+      </c>
+      <c r="NV17">
+        <f>+'UCI OCUPADA TOTAL'!NV17-'UCI OCUPADA COVID'!NV17</f>
+        <v>11</v>
+      </c>
+      <c r="NW17">
+        <f>+'UCI OCUPADA TOTAL'!NW17-'UCI OCUPADA COVID'!NW17</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="18" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -92093,48 +93722,76 @@
         <f>+'UCI OCUPADA TOTAL'!NP18-'UCI OCUPADA COVID'!NP18</f>
         <v>889</v>
       </c>
+      <c r="NQ18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NQ18-'UCI OCUPADA COVID'!NQ18</f>
+        <v>928</v>
+      </c>
+      <c r="NR18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NR18-'UCI OCUPADA COVID'!NR18</f>
+        <v>919</v>
+      </c>
+      <c r="NS18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NS18-'UCI OCUPADA COVID'!NS18</f>
+        <v>941</v>
+      </c>
+      <c r="NT18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NT18-'UCI OCUPADA COVID'!NT18</f>
+        <v>965</v>
+      </c>
+      <c r="NU18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NU18-'UCI OCUPADA COVID'!NU18</f>
+        <v>966</v>
+      </c>
+      <c r="NV18" s="7">
+        <f>+'UCI OCUPADA TOTAL'!NV18-'UCI OCUPADA COVID'!NV18</f>
+        <v>992</v>
+      </c>
+      <c r="NW18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!NW18-'UCI OCUPADA COVID'!NW18</f>
+        <v>1002</v>
+      </c>
     </row>
-    <row r="19" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:380" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
camas UCI, martes 11 de mayo 2021
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -149,7 +149,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -239,7 +239,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="3" builtinId="3"/>
@@ -2910,10 +2910,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NP1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NU1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NQ18" sqref="NQ18:NW18"/>
+      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4097,8 +4097,29 @@
       <c r="NW1" s="8">
         <v>44320</v>
       </c>
+      <c r="NX1" s="8">
+        <v>44321</v>
+      </c>
+      <c r="NY1" s="8">
+        <v>44322</v>
+      </c>
+      <c r="NZ1" s="8">
+        <v>44323</v>
+      </c>
+      <c r="OA1" s="8">
+        <v>44324</v>
+      </c>
+      <c r="OB1" s="8">
+        <v>44325</v>
+      </c>
+      <c r="OC1" s="8">
+        <v>44326</v>
+      </c>
+      <c r="OD1" s="8">
+        <v>44327</v>
+      </c>
     </row>
-    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5260,8 +5281,29 @@
       <c r="NW2" s="11">
         <v>40</v>
       </c>
+      <c r="NX2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NY2" s="11">
+        <v>40</v>
+      </c>
+      <c r="NZ2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OA2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OB2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OC2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OD2" s="11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6423,8 +6465,29 @@
       <c r="NW3" s="11">
         <v>62</v>
       </c>
+      <c r="NX3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NY3" s="11">
+        <v>62</v>
+      </c>
+      <c r="NZ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OA3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OB3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OC3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OD3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7586,8 +7649,29 @@
       <c r="NW4" s="11">
         <v>168</v>
       </c>
+      <c r="NX4" s="11">
+        <v>165</v>
+      </c>
+      <c r="NY4" s="11">
+        <v>166</v>
+      </c>
+      <c r="NZ4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OA4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OB4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OC4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OD4" s="11">
+        <v>165</v>
+      </c>
     </row>
-    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -8749,8 +8833,29 @@
       <c r="NW5" s="11">
         <v>34</v>
       </c>
+      <c r="NX5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NY5" s="11">
+        <v>34</v>
+      </c>
+      <c r="NZ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OA5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OB5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OC5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OD5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -9912,8 +10017,29 @@
       <c r="NW6" s="11">
         <v>140</v>
       </c>
+      <c r="NX6" s="11">
+        <v>140</v>
+      </c>
+      <c r="NY6" s="11">
+        <v>140</v>
+      </c>
+      <c r="NZ6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OA6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OB6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OC6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OD6" s="11">
+        <v>140</v>
+      </c>
     </row>
-    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -11075,8 +11201,29 @@
       <c r="NW7" s="11">
         <v>345</v>
       </c>
+      <c r="NX7" s="11">
+        <v>343</v>
+      </c>
+      <c r="NY7" s="11">
+        <v>343</v>
+      </c>
+      <c r="NZ7" s="11">
+        <v>342</v>
+      </c>
+      <c r="OA7" s="11">
+        <v>342</v>
+      </c>
+      <c r="OB7" s="11">
+        <v>342</v>
+      </c>
+      <c r="OC7" s="11">
+        <v>342</v>
+      </c>
+      <c r="OD7" s="11">
+        <v>342</v>
+      </c>
     </row>
-    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12238,8 +12385,29 @@
       <c r="NW8" s="11">
         <v>2619</v>
       </c>
+      <c r="NX8" s="11">
+        <v>2621</v>
+      </c>
+      <c r="NY8" s="11">
+        <v>2621</v>
+      </c>
+      <c r="NZ8" s="11">
+        <v>2621</v>
+      </c>
+      <c r="OA8" s="11">
+        <v>2615</v>
+      </c>
+      <c r="OB8" s="11">
+        <v>2611</v>
+      </c>
+      <c r="OC8" s="11">
+        <v>2608</v>
+      </c>
+      <c r="OD8" s="11">
+        <v>2607</v>
+      </c>
     </row>
-    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13401,8 +13569,29 @@
       <c r="NW9" s="11">
         <v>206</v>
       </c>
+      <c r="NX9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NY9" s="11">
+        <v>206</v>
+      </c>
+      <c r="NZ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OA9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OB9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OC9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OD9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -14564,8 +14753,29 @@
       <c r="NW10" s="11">
         <v>162</v>
       </c>
+      <c r="NX10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NY10" s="11">
+        <v>166</v>
+      </c>
+      <c r="NZ10" s="11">
+        <v>166</v>
+      </c>
+      <c r="OA10" s="11">
+        <v>166</v>
+      </c>
+      <c r="OB10" s="11">
+        <v>166</v>
+      </c>
+      <c r="OC10" s="11">
+        <v>166</v>
+      </c>
+      <c r="OD10" s="11">
+        <v>166</v>
+      </c>
     </row>
-    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -15727,8 +15937,29 @@
       <c r="NW11" s="11">
         <v>73</v>
       </c>
+      <c r="NX11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NY11" s="11">
+        <v>73</v>
+      </c>
+      <c r="NZ11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OA11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OB11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OC11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OD11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -16890,8 +17121,29 @@
       <c r="NW12" s="11">
         <v>314</v>
       </c>
+      <c r="NX12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NY12" s="11">
+        <v>315</v>
+      </c>
+      <c r="NZ12" s="11">
+        <v>317</v>
+      </c>
+      <c r="OA12" s="11">
+        <v>317</v>
+      </c>
+      <c r="OB12" s="11">
+        <v>317</v>
+      </c>
+      <c r="OC12" s="11">
+        <v>317</v>
+      </c>
+      <c r="OD12" s="11">
+        <v>316</v>
+      </c>
     </row>
-    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -18053,8 +18305,29 @@
       <c r="NW13" s="11">
         <v>145</v>
       </c>
+      <c r="NX13" s="11">
+        <v>146</v>
+      </c>
+      <c r="NY13" s="11">
+        <v>148</v>
+      </c>
+      <c r="NZ13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OA13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OB13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OC13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OD13" s="11">
+        <v>151</v>
+      </c>
     </row>
-    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -19216,8 +19489,29 @@
       <c r="NW14" s="11">
         <v>46</v>
       </c>
+      <c r="NX14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NY14" s="11">
+        <v>46</v>
+      </c>
+      <c r="NZ14" s="11">
+        <v>46</v>
+      </c>
+      <c r="OA14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OB14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OC14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OD14" s="11">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -20379,8 +20673,29 @@
       <c r="NW15" s="11">
         <v>128</v>
       </c>
+      <c r="NX15" s="11">
+        <v>128</v>
+      </c>
+      <c r="NY15" s="11">
+        <v>129</v>
+      </c>
+      <c r="NZ15" s="11">
+        <v>129</v>
+      </c>
+      <c r="OA15" s="11">
+        <v>128</v>
+      </c>
+      <c r="OB15" s="11">
+        <v>128</v>
+      </c>
+      <c r="OC15" s="11">
+        <v>128</v>
+      </c>
+      <c r="OD15" s="11">
+        <v>128</v>
+      </c>
     </row>
-    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -21542,8 +21857,29 @@
       <c r="NW16" s="11">
         <v>10</v>
       </c>
+      <c r="NX16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NY16" s="11">
+        <v>10</v>
+      </c>
+      <c r="NZ16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OA16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OB16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OC16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OD16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -22705,8 +23041,29 @@
       <c r="NW17" s="11">
         <v>44</v>
       </c>
+      <c r="NX17" s="11">
+        <v>44</v>
+      </c>
+      <c r="NY17" s="11">
+        <v>44</v>
+      </c>
+      <c r="NZ17" s="11">
+        <v>44</v>
+      </c>
+      <c r="OA17" s="11">
+        <v>44</v>
+      </c>
+      <c r="OB17" s="11">
+        <v>44</v>
+      </c>
+      <c r="OC17" s="11">
+        <v>43</v>
+      </c>
+      <c r="OD17" s="11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="18" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -23882,7 +24239,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:NW18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:OD18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -23981,9 +24338,37 @@
         <f t="shared" si="7"/>
         <v>4536</v>
       </c>
+      <c r="NX18" s="6">
+        <f t="shared" si="7"/>
+        <v>4539</v>
+      </c>
+      <c r="NY18" s="6">
+        <f t="shared" si="7"/>
+        <v>4543</v>
+      </c>
+      <c r="NZ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4544</v>
+      </c>
+      <c r="OA18" s="6">
+        <f t="shared" si="7"/>
+        <v>4532</v>
+      </c>
+      <c r="OB18" s="6">
+        <f t="shared" si="7"/>
+        <v>4527</v>
+      </c>
+      <c r="OC18" s="6">
+        <f t="shared" si="7"/>
+        <v>4523</v>
+      </c>
+      <c r="OD18" s="6">
+        <f t="shared" si="7"/>
+        <v>4525</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:387 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -24001,12 +24386,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NW36"/>
+  <dimension ref="A1:OD36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NO1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NW2" sqref="NW2:NW17"/>
+      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24026,7 +24411,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -25188,8 +25573,29 @@
       <c r="NW1" s="8">
         <v>44320</v>
       </c>
+      <c r="NX1" s="8">
+        <v>44321</v>
+      </c>
+      <c r="NY1" s="8">
+        <v>44322</v>
+      </c>
+      <c r="NZ1" s="8">
+        <v>44323</v>
+      </c>
+      <c r="OA1" s="8">
+        <v>44324</v>
+      </c>
+      <c r="OB1" s="8">
+        <v>44325</v>
+      </c>
+      <c r="OC1" s="8">
+        <v>44326</v>
+      </c>
+      <c r="OD1" s="8">
+        <v>44327</v>
+      </c>
     </row>
-    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -26351,8 +26757,29 @@
       <c r="NW2">
         <v>37</v>
       </c>
+      <c r="NX2">
+        <v>35</v>
+      </c>
+      <c r="NY2">
+        <v>38</v>
+      </c>
+      <c r="NZ2">
+        <v>35</v>
+      </c>
+      <c r="OA2">
+        <v>35</v>
+      </c>
+      <c r="OB2">
+        <v>37</v>
+      </c>
+      <c r="OC2">
+        <v>38</v>
+      </c>
+      <c r="OD2">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -27514,8 +27941,29 @@
       <c r="NW3">
         <v>59</v>
       </c>
+      <c r="NX3">
+        <v>59</v>
+      </c>
+      <c r="NY3">
+        <v>60</v>
+      </c>
+      <c r="NZ3">
+        <v>55</v>
+      </c>
+      <c r="OA3">
+        <v>56</v>
+      </c>
+      <c r="OB3">
+        <v>56</v>
+      </c>
+      <c r="OC3">
+        <v>53</v>
+      </c>
+      <c r="OD3">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -28677,8 +29125,29 @@
       <c r="NW4">
         <v>160</v>
       </c>
+      <c r="NX4">
+        <v>156</v>
+      </c>
+      <c r="NY4">
+        <v>155</v>
+      </c>
+      <c r="NZ4">
+        <v>146</v>
+      </c>
+      <c r="OA4">
+        <v>148</v>
+      </c>
+      <c r="OB4">
+        <v>144</v>
+      </c>
+      <c r="OC4">
+        <v>149</v>
+      </c>
+      <c r="OD4">
+        <v>149</v>
+      </c>
     </row>
-    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -29840,8 +30309,29 @@
       <c r="NW5">
         <v>32</v>
       </c>
+      <c r="NX5">
+        <v>30</v>
+      </c>
+      <c r="NY5">
+        <v>30</v>
+      </c>
+      <c r="NZ5">
+        <v>31</v>
+      </c>
+      <c r="OA5">
+        <v>30</v>
+      </c>
+      <c r="OB5">
+        <v>27</v>
+      </c>
+      <c r="OC5">
+        <v>30</v>
+      </c>
+      <c r="OD5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -31003,8 +31493,29 @@
       <c r="NW6">
         <v>133</v>
       </c>
+      <c r="NX6">
+        <v>125</v>
+      </c>
+      <c r="NY6">
+        <v>126</v>
+      </c>
+      <c r="NZ6">
+        <v>127</v>
+      </c>
+      <c r="OA6">
+        <v>127</v>
+      </c>
+      <c r="OB6">
+        <v>132</v>
+      </c>
+      <c r="OC6">
+        <v>127</v>
+      </c>
+      <c r="OD6">
+        <v>126</v>
+      </c>
     </row>
-    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -32166,8 +32677,29 @@
       <c r="NW7">
         <v>329</v>
       </c>
+      <c r="NX7">
+        <v>334</v>
+      </c>
+      <c r="NY7">
+        <v>329</v>
+      </c>
+      <c r="NZ7">
+        <v>329</v>
+      </c>
+      <c r="OA7">
+        <v>327</v>
+      </c>
+      <c r="OB7">
+        <v>328</v>
+      </c>
+      <c r="OC7">
+        <v>330</v>
+      </c>
+      <c r="OD7">
+        <v>328</v>
+      </c>
     </row>
-    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -33329,8 +33861,29 @@
       <c r="NW8">
         <v>2522</v>
       </c>
+      <c r="NX8">
+        <v>2526</v>
+      </c>
+      <c r="NY8">
+        <v>2505</v>
+      </c>
+      <c r="NZ8">
+        <v>2500</v>
+      </c>
+      <c r="OA8">
+        <v>2498</v>
+      </c>
+      <c r="OB8">
+        <v>2486</v>
+      </c>
+      <c r="OC8">
+        <v>2488</v>
+      </c>
+      <c r="OD8">
+        <v>2498</v>
+      </c>
     </row>
-    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -34492,8 +35045,29 @@
       <c r="NW9">
         <v>171</v>
       </c>
+      <c r="NX9">
+        <v>170</v>
+      </c>
+      <c r="NY9">
+        <v>165</v>
+      </c>
+      <c r="NZ9">
+        <v>167</v>
+      </c>
+      <c r="OA9">
+        <v>166</v>
+      </c>
+      <c r="OB9">
+        <v>167</v>
+      </c>
+      <c r="OC9">
+        <v>170</v>
+      </c>
+      <c r="OD9">
+        <v>164</v>
+      </c>
     </row>
-    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -35655,8 +36229,29 @@
       <c r="NW10">
         <v>155</v>
       </c>
+      <c r="NX10">
+        <v>153</v>
+      </c>
+      <c r="NY10">
+        <v>159</v>
+      </c>
+      <c r="NZ10">
+        <v>161</v>
+      </c>
+      <c r="OA10">
+        <v>155</v>
+      </c>
+      <c r="OB10">
+        <v>160</v>
+      </c>
+      <c r="OC10">
+        <v>161</v>
+      </c>
+      <c r="OD10">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -36818,8 +37413,29 @@
       <c r="NW11">
         <v>69</v>
       </c>
+      <c r="NX11">
+        <v>68</v>
+      </c>
+      <c r="NY11">
+        <v>69</v>
+      </c>
+      <c r="NZ11">
+        <v>67</v>
+      </c>
+      <c r="OA11">
+        <v>66</v>
+      </c>
+      <c r="OB11">
+        <v>66</v>
+      </c>
+      <c r="OC11">
+        <v>61</v>
+      </c>
+      <c r="OD11">
+        <v>59</v>
+      </c>
     </row>
-    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -37981,8 +38597,29 @@
       <c r="NW12">
         <v>288</v>
       </c>
+      <c r="NX12">
+        <v>286</v>
+      </c>
+      <c r="NY12">
+        <v>283</v>
+      </c>
+      <c r="NZ12">
+        <v>286</v>
+      </c>
+      <c r="OA12">
+        <v>278</v>
+      </c>
+      <c r="OB12">
+        <v>288</v>
+      </c>
+      <c r="OC12">
+        <v>284</v>
+      </c>
+      <c r="OD12">
+        <v>280</v>
+      </c>
     </row>
-    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -39144,8 +39781,29 @@
       <c r="NW13">
         <v>139</v>
       </c>
+      <c r="NX13">
+        <v>135</v>
+      </c>
+      <c r="NY13">
+        <v>135</v>
+      </c>
+      <c r="NZ13">
+        <v>142</v>
+      </c>
+      <c r="OA13">
+        <v>142</v>
+      </c>
+      <c r="OB13">
+        <v>139</v>
+      </c>
+      <c r="OC13">
+        <v>141</v>
+      </c>
+      <c r="OD13">
+        <v>142</v>
+      </c>
     </row>
-    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -40307,8 +40965,29 @@
       <c r="NW14">
         <v>43</v>
       </c>
+      <c r="NX14">
+        <v>43</v>
+      </c>
+      <c r="NY14">
+        <v>40</v>
+      </c>
+      <c r="NZ14">
+        <v>43</v>
+      </c>
+      <c r="OA14">
+        <v>38</v>
+      </c>
+      <c r="OB14">
+        <v>37</v>
+      </c>
+      <c r="OC14">
+        <v>37</v>
+      </c>
+      <c r="OD14">
+        <v>34</v>
+      </c>
     </row>
-    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -41470,8 +42149,29 @@
       <c r="NW15">
         <v>120</v>
       </c>
+      <c r="NX15">
+        <v>118</v>
+      </c>
+      <c r="NY15">
+        <v>121</v>
+      </c>
+      <c r="NZ15">
+        <v>118</v>
+      </c>
+      <c r="OA15">
+        <v>111</v>
+      </c>
+      <c r="OB15">
+        <v>113</v>
+      </c>
+      <c r="OC15">
+        <v>110</v>
+      </c>
+      <c r="OD15">
+        <v>112</v>
+      </c>
     </row>
-    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -42633,8 +43333,29 @@
       <c r="NW16">
         <v>10</v>
       </c>
+      <c r="NX16">
+        <v>9</v>
+      </c>
+      <c r="NY16">
+        <v>10</v>
+      </c>
+      <c r="NZ16">
+        <v>8</v>
+      </c>
+      <c r="OA16">
+        <v>7</v>
+      </c>
+      <c r="OB16">
+        <v>7</v>
+      </c>
+      <c r="OC16">
+        <v>8</v>
+      </c>
+      <c r="OD16">
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -43796,8 +44517,29 @@
       <c r="NW17">
         <v>38</v>
       </c>
+      <c r="NX17">
+        <v>39</v>
+      </c>
+      <c r="NY17">
+        <v>35</v>
+      </c>
+      <c r="NZ17">
+        <v>35</v>
+      </c>
+      <c r="OA17">
+        <v>37</v>
+      </c>
+      <c r="OB17">
+        <v>36</v>
+      </c>
+      <c r="OC17">
+        <v>37</v>
+      </c>
+      <c r="OD17">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -44889,7 +45631,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:NW18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:OD18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -45052,8 +45794,36 @@
         <f t="shared" si="1"/>
         <v>4305</v>
       </c>
+      <c r="NX18" s="6">
+        <f t="shared" si="1"/>
+        <v>4286</v>
+      </c>
+      <c r="NY18" s="6">
+        <f t="shared" si="1"/>
+        <v>4260</v>
+      </c>
+      <c r="NZ18" s="6">
+        <f t="shared" si="1"/>
+        <v>4250</v>
+      </c>
+      <c r="OA18" s="6">
+        <f t="shared" si="1"/>
+        <v>4221</v>
+      </c>
+      <c r="OB18" s="6">
+        <f t="shared" si="1"/>
+        <v>4223</v>
+      </c>
+      <c r="OC18" s="6">
+        <f t="shared" si="1"/>
+        <v>4224</v>
+      </c>
+      <c r="OD18" s="6">
+        <f t="shared" si="1"/>
+        <v>4212</v>
+      </c>
     </row>
-    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -45336,7 +46106,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -45619,7 +46389,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -45902,7 +46672,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -46185,7 +46955,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -46468,7 +47238,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -46751,7 +47521,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -47034,7 +47804,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -47317,7 +48087,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -47600,7 +48370,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -47883,7 +48653,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -48166,7 +48936,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -48449,7 +49219,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -49872,12 +50642,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:NW34"/>
+  <dimension ref="A1:OD34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NM1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NQ18" sqref="NQ18:NW18"/>
+      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49898,7 +50668,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -51060,8 +51830,29 @@
       <c r="NW1" s="8">
         <v>44320</v>
       </c>
+      <c r="NX1" s="8">
+        <v>44321</v>
+      </c>
+      <c r="NY1" s="8">
+        <v>44322</v>
+      </c>
+      <c r="NZ1" s="8">
+        <v>44323</v>
+      </c>
+      <c r="OA1" s="8">
+        <v>44324</v>
+      </c>
+      <c r="OB1" s="8">
+        <v>44325</v>
+      </c>
+      <c r="OC1" s="8">
+        <v>44326</v>
+      </c>
+      <c r="OD1" s="8">
+        <v>44327</v>
+      </c>
     </row>
-    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -52223,8 +53014,29 @@
       <c r="NW2">
         <v>31</v>
       </c>
+      <c r="NX2">
+        <v>28</v>
+      </c>
+      <c r="NY2">
+        <v>30</v>
+      </c>
+      <c r="NZ2">
+        <v>30</v>
+      </c>
+      <c r="OA2">
+        <v>29</v>
+      </c>
+      <c r="OB2">
+        <v>31</v>
+      </c>
+      <c r="OC2">
+        <v>33</v>
+      </c>
+      <c r="OD2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -53386,8 +54198,29 @@
       <c r="NW3">
         <v>55</v>
       </c>
+      <c r="NX3">
+        <v>56</v>
+      </c>
+      <c r="NY3">
+        <v>57</v>
+      </c>
+      <c r="NZ3">
+        <v>54</v>
+      </c>
+      <c r="OA3">
+        <v>54</v>
+      </c>
+      <c r="OB3">
+        <v>54</v>
+      </c>
+      <c r="OC3">
+        <v>51</v>
+      </c>
+      <c r="OD3">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -54549,8 +55382,29 @@
       <c r="NW4">
         <v>105</v>
       </c>
+      <c r="NX4">
+        <v>101</v>
+      </c>
+      <c r="NY4">
+        <v>93</v>
+      </c>
+      <c r="NZ4">
+        <v>93</v>
+      </c>
+      <c r="OA4">
+        <v>90</v>
+      </c>
+      <c r="OB4">
+        <v>89</v>
+      </c>
+      <c r="OC4">
+        <v>88</v>
+      </c>
+      <c r="OD4">
+        <v>92</v>
+      </c>
     </row>
-    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -55712,8 +56566,29 @@
       <c r="NW5">
         <v>24</v>
       </c>
+      <c r="NX5">
+        <v>22</v>
+      </c>
+      <c r="NY5">
+        <v>20</v>
+      </c>
+      <c r="NZ5">
+        <v>20</v>
+      </c>
+      <c r="OA5">
+        <v>20</v>
+      </c>
+      <c r="OB5">
+        <v>18</v>
+      </c>
+      <c r="OC5">
+        <v>19</v>
+      </c>
+      <c r="OD5">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -56875,8 +57750,29 @@
       <c r="NW6">
         <v>103</v>
       </c>
+      <c r="NX6">
+        <v>95</v>
+      </c>
+      <c r="NY6">
+        <v>97</v>
+      </c>
+      <c r="NZ6">
+        <v>96</v>
+      </c>
+      <c r="OA6">
+        <v>97</v>
+      </c>
+      <c r="OB6">
+        <v>100</v>
+      </c>
+      <c r="OC6">
+        <v>98</v>
+      </c>
+      <c r="OD6">
+        <v>95</v>
+      </c>
     </row>
-    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -58038,8 +58934,29 @@
       <c r="NW7">
         <v>266</v>
       </c>
+      <c r="NX7">
+        <v>263</v>
+      </c>
+      <c r="NY7">
+        <v>256</v>
+      </c>
+      <c r="NZ7">
+        <v>250</v>
+      </c>
+      <c r="OA7">
+        <v>249</v>
+      </c>
+      <c r="OB7">
+        <v>244</v>
+      </c>
+      <c r="OC7">
+        <v>248</v>
+      </c>
+      <c r="OD7">
+        <v>245</v>
+      </c>
     </row>
-    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -59201,8 +60118,29 @@
       <c r="NW8">
         <v>1913</v>
       </c>
+      <c r="NX8">
+        <v>1898</v>
+      </c>
+      <c r="NY8">
+        <v>1851</v>
+      </c>
+      <c r="NZ8">
+        <v>1850</v>
+      </c>
+      <c r="OA8">
+        <v>1842</v>
+      </c>
+      <c r="OB8">
+        <v>1840</v>
+      </c>
+      <c r="OC8">
+        <v>1835</v>
+      </c>
+      <c r="OD8">
+        <v>1834</v>
+      </c>
     </row>
-    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -60364,8 +61302,29 @@
       <c r="NW9">
         <v>149</v>
       </c>
+      <c r="NX9">
+        <v>149</v>
+      </c>
+      <c r="NY9">
+        <v>140</v>
+      </c>
+      <c r="NZ9">
+        <v>136</v>
+      </c>
+      <c r="OA9">
+        <v>135</v>
+      </c>
+      <c r="OB9">
+        <v>136</v>
+      </c>
+      <c r="OC9">
+        <v>131</v>
+      </c>
+      <c r="OD9">
+        <v>122</v>
+      </c>
     </row>
-    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -61527,8 +62486,29 @@
       <c r="NW10">
         <v>135</v>
       </c>
+      <c r="NX10">
+        <v>135</v>
+      </c>
+      <c r="NY10">
+        <v>137</v>
+      </c>
+      <c r="NZ10">
+        <v>137</v>
+      </c>
+      <c r="OA10">
+        <v>134</v>
+      </c>
+      <c r="OB10">
+        <v>137</v>
+      </c>
+      <c r="OC10">
+        <v>137</v>
+      </c>
+      <c r="OD10">
+        <v>134</v>
+      </c>
     </row>
-    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -62690,8 +63670,29 @@
       <c r="NW11">
         <v>53</v>
       </c>
+      <c r="NX11">
+        <v>52</v>
+      </c>
+      <c r="NY11">
+        <v>52</v>
+      </c>
+      <c r="NZ11">
+        <v>52</v>
+      </c>
+      <c r="OA11">
+        <v>51</v>
+      </c>
+      <c r="OB11">
+        <v>49</v>
+      </c>
+      <c r="OC11">
+        <v>46</v>
+      </c>
+      <c r="OD11">
+        <v>45</v>
+      </c>
     </row>
-    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -63853,8 +64854,29 @@
       <c r="NW12">
         <v>218</v>
       </c>
+      <c r="NX12">
+        <v>210</v>
+      </c>
+      <c r="NY12">
+        <v>205</v>
+      </c>
+      <c r="NZ12">
+        <v>204</v>
+      </c>
+      <c r="OA12">
+        <v>197</v>
+      </c>
+      <c r="OB12">
+        <v>200</v>
+      </c>
+      <c r="OC12">
+        <v>199</v>
+      </c>
+      <c r="OD12">
+        <v>195</v>
+      </c>
     </row>
-    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -65016,8 +66038,29 @@
       <c r="NW13">
         <v>106</v>
       </c>
+      <c r="NX13">
+        <v>106</v>
+      </c>
+      <c r="NY13">
+        <v>107</v>
+      </c>
+      <c r="NZ13">
+        <v>110</v>
+      </c>
+      <c r="OA13">
+        <v>106</v>
+      </c>
+      <c r="OB13">
+        <v>110</v>
+      </c>
+      <c r="OC13">
+        <v>115</v>
+      </c>
+      <c r="OD13">
+        <v>109</v>
+      </c>
     </row>
-    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -66179,8 +67222,29 @@
       <c r="NW14">
         <v>27</v>
       </c>
+      <c r="NX14">
+        <v>23</v>
+      </c>
+      <c r="NY14">
+        <v>23</v>
+      </c>
+      <c r="NZ14">
+        <v>25</v>
+      </c>
+      <c r="OA14">
+        <v>24</v>
+      </c>
+      <c r="OB14">
+        <v>25</v>
+      </c>
+      <c r="OC14">
+        <v>23</v>
+      </c>
+      <c r="OD14">
+        <v>22</v>
+      </c>
     </row>
-    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -67342,8 +68406,29 @@
       <c r="NW15">
         <v>83</v>
       </c>
+      <c r="NX15">
+        <v>84</v>
+      </c>
+      <c r="NY15">
+        <v>83</v>
+      </c>
+      <c r="NZ15">
+        <v>82</v>
+      </c>
+      <c r="OA15">
+        <v>77</v>
+      </c>
+      <c r="OB15">
+        <v>82</v>
+      </c>
+      <c r="OC15">
+        <v>82</v>
+      </c>
+      <c r="OD15">
+        <v>77</v>
+      </c>
     </row>
-    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -68505,8 +69590,29 @@
       <c r="NW16">
         <v>7</v>
       </c>
+      <c r="NX16">
+        <v>7</v>
+      </c>
+      <c r="NY16">
+        <v>7</v>
+      </c>
+      <c r="NZ16">
+        <v>6</v>
+      </c>
+      <c r="OA16">
+        <v>5</v>
+      </c>
+      <c r="OB16">
+        <v>5</v>
+      </c>
+      <c r="OC16">
+        <v>5</v>
+      </c>
+      <c r="OD16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -69668,8 +70774,29 @@
       <c r="NW17">
         <v>28</v>
       </c>
+      <c r="NX17">
+        <v>31</v>
+      </c>
+      <c r="NY17">
+        <v>30</v>
+      </c>
+      <c r="NZ17">
+        <v>31</v>
+      </c>
+      <c r="OA17">
+        <v>28</v>
+      </c>
+      <c r="OB17">
+        <v>27</v>
+      </c>
+      <c r="OC17">
+        <v>27</v>
+      </c>
+      <c r="OD17">
+        <v>25</v>
+      </c>
     </row>
-    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -70806,7 +71933,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:NW18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:OD18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -70929,50 +72056,78 @@
         <f t="shared" si="1"/>
         <v>3303</v>
       </c>
+      <c r="NX18" s="6">
+        <f t="shared" si="1"/>
+        <v>3260</v>
+      </c>
+      <c r="NY18" s="6">
+        <f t="shared" si="1"/>
+        <v>3188</v>
+      </c>
+      <c r="NZ18" s="6">
+        <f t="shared" si="1"/>
+        <v>3176</v>
+      </c>
+      <c r="OA18" s="6">
+        <f t="shared" si="1"/>
+        <v>3138</v>
+      </c>
+      <c r="OB18" s="6">
+        <f t="shared" si="1"/>
+        <v>3147</v>
+      </c>
+      <c r="OC18" s="6">
+        <f t="shared" si="1"/>
+        <v>3137</v>
+      </c>
+      <c r="OD18" s="6">
+        <f t="shared" si="1"/>
+        <v>3102</v>
+      </c>
     </row>
-    <row r="19" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -70992,12 +72147,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:NW34"/>
+  <dimension ref="A1:OD34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NO1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="NY12" sqref="NY12"/>
+      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71015,7 +72170,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -72177,8 +73332,29 @@
       <c r="NW1" s="8">
         <v>44320</v>
       </c>
+      <c r="NX1" s="8">
+        <v>44321</v>
+      </c>
+      <c r="NY1" s="8">
+        <v>44322</v>
+      </c>
+      <c r="NZ1" s="8">
+        <v>44323</v>
+      </c>
+      <c r="OA1" s="8">
+        <v>44324</v>
+      </c>
+      <c r="OB1" s="8">
+        <v>44325</v>
+      </c>
+      <c r="OC1" s="8">
+        <v>44326</v>
+      </c>
+      <c r="OD1" s="8">
+        <v>44327</v>
+      </c>
     </row>
-    <row r="2" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -73446,8 +74622,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW2-'UCI OCUPADA COVID'!NW2</f>
         <v>6</v>
       </c>
+      <c r="NX2">
+        <f>+'UCI OCUPADA TOTAL'!NX2-'UCI OCUPADA COVID'!NX2</f>
+        <v>7</v>
+      </c>
+      <c r="NY2">
+        <f>+'UCI OCUPADA TOTAL'!NY2-'UCI OCUPADA COVID'!NY2</f>
+        <v>8</v>
+      </c>
+      <c r="NZ2">
+        <f>+'UCI OCUPADA TOTAL'!NZ2-'UCI OCUPADA COVID'!NZ2</f>
+        <v>5</v>
+      </c>
+      <c r="OA2">
+        <f>+'UCI OCUPADA TOTAL'!OA2-'UCI OCUPADA COVID'!OA2</f>
+        <v>6</v>
+      </c>
+      <c r="OB2">
+        <f>+'UCI OCUPADA TOTAL'!OB2-'UCI OCUPADA COVID'!OB2</f>
+        <v>6</v>
+      </c>
+      <c r="OC2">
+        <f>+'UCI OCUPADA TOTAL'!OC2-'UCI OCUPADA COVID'!OC2</f>
+        <v>5</v>
+      </c>
+      <c r="OD2">
+        <f>+'UCI OCUPADA TOTAL'!OD2-'UCI OCUPADA COVID'!OD2</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -74715,8 +75919,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW3-'UCI OCUPADA COVID'!NW3</f>
         <v>4</v>
       </c>
+      <c r="NX3">
+        <f>+'UCI OCUPADA TOTAL'!NX3-'UCI OCUPADA COVID'!NX3</f>
+        <v>3</v>
+      </c>
+      <c r="NY3">
+        <f>+'UCI OCUPADA TOTAL'!NY3-'UCI OCUPADA COVID'!NY3</f>
+        <v>3</v>
+      </c>
+      <c r="NZ3">
+        <f>+'UCI OCUPADA TOTAL'!NZ3-'UCI OCUPADA COVID'!NZ3</f>
+        <v>1</v>
+      </c>
+      <c r="OA3">
+        <f>+'UCI OCUPADA TOTAL'!OA3-'UCI OCUPADA COVID'!OA3</f>
+        <v>2</v>
+      </c>
+      <c r="OB3">
+        <f>+'UCI OCUPADA TOTAL'!OB3-'UCI OCUPADA COVID'!OB3</f>
+        <v>2</v>
+      </c>
+      <c r="OC3">
+        <f>+'UCI OCUPADA TOTAL'!OC3-'UCI OCUPADA COVID'!OC3</f>
+        <v>2</v>
+      </c>
+      <c r="OD3">
+        <f>+'UCI OCUPADA TOTAL'!OD3-'UCI OCUPADA COVID'!OD3</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -75984,8 +77216,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW4-'UCI OCUPADA COVID'!NW4</f>
         <v>55</v>
       </c>
+      <c r="NX4">
+        <f>+'UCI OCUPADA TOTAL'!NX4-'UCI OCUPADA COVID'!NX4</f>
+        <v>55</v>
+      </c>
+      <c r="NY4">
+        <f>+'UCI OCUPADA TOTAL'!NY4-'UCI OCUPADA COVID'!NY4</f>
+        <v>62</v>
+      </c>
+      <c r="NZ4">
+        <f>+'UCI OCUPADA TOTAL'!NZ4-'UCI OCUPADA COVID'!NZ4</f>
+        <v>53</v>
+      </c>
+      <c r="OA4">
+        <f>+'UCI OCUPADA TOTAL'!OA4-'UCI OCUPADA COVID'!OA4</f>
+        <v>58</v>
+      </c>
+      <c r="OB4">
+        <f>+'UCI OCUPADA TOTAL'!OB4-'UCI OCUPADA COVID'!OB4</f>
+        <v>55</v>
+      </c>
+      <c r="OC4">
+        <f>+'UCI OCUPADA TOTAL'!OC4-'UCI OCUPADA COVID'!OC4</f>
+        <v>61</v>
+      </c>
+      <c r="OD4">
+        <f>+'UCI OCUPADA TOTAL'!OD4-'UCI OCUPADA COVID'!OD4</f>
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -77253,8 +78513,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW5-'UCI OCUPADA COVID'!NW5</f>
         <v>8</v>
       </c>
+      <c r="NX5">
+        <f>+'UCI OCUPADA TOTAL'!NX5-'UCI OCUPADA COVID'!NX5</f>
+        <v>8</v>
+      </c>
+      <c r="NY5">
+        <f>+'UCI OCUPADA TOTAL'!NY5-'UCI OCUPADA COVID'!NY5</f>
+        <v>10</v>
+      </c>
+      <c r="NZ5">
+        <f>+'UCI OCUPADA TOTAL'!NZ5-'UCI OCUPADA COVID'!NZ5</f>
+        <v>11</v>
+      </c>
+      <c r="OA5">
+        <f>+'UCI OCUPADA TOTAL'!OA5-'UCI OCUPADA COVID'!OA5</f>
+        <v>10</v>
+      </c>
+      <c r="OB5">
+        <f>+'UCI OCUPADA TOTAL'!OB5-'UCI OCUPADA COVID'!OB5</f>
+        <v>9</v>
+      </c>
+      <c r="OC5">
+        <f>+'UCI OCUPADA TOTAL'!OC5-'UCI OCUPADA COVID'!OC5</f>
+        <v>11</v>
+      </c>
+      <c r="OD5">
+        <f>+'UCI OCUPADA TOTAL'!OD5-'UCI OCUPADA COVID'!OD5</f>
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -78522,8 +79810,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW6-'UCI OCUPADA COVID'!NW6</f>
         <v>30</v>
       </c>
+      <c r="NX6">
+        <f>+'UCI OCUPADA TOTAL'!NX6-'UCI OCUPADA COVID'!NX6</f>
+        <v>30</v>
+      </c>
+      <c r="NY6">
+        <f>+'UCI OCUPADA TOTAL'!NY6-'UCI OCUPADA COVID'!NY6</f>
+        <v>29</v>
+      </c>
+      <c r="NZ6">
+        <f>+'UCI OCUPADA TOTAL'!NZ6-'UCI OCUPADA COVID'!NZ6</f>
+        <v>31</v>
+      </c>
+      <c r="OA6">
+        <f>+'UCI OCUPADA TOTAL'!OA6-'UCI OCUPADA COVID'!OA6</f>
+        <v>30</v>
+      </c>
+      <c r="OB6">
+        <f>+'UCI OCUPADA TOTAL'!OB6-'UCI OCUPADA COVID'!OB6</f>
+        <v>32</v>
+      </c>
+      <c r="OC6">
+        <f>+'UCI OCUPADA TOTAL'!OC6-'UCI OCUPADA COVID'!OC6</f>
+        <v>29</v>
+      </c>
+      <c r="OD6">
+        <f>+'UCI OCUPADA TOTAL'!OD6-'UCI OCUPADA COVID'!OD6</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -79791,8 +81107,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW7-'UCI OCUPADA COVID'!NW7</f>
         <v>63</v>
       </c>
+      <c r="NX7">
+        <f>+'UCI OCUPADA TOTAL'!NX7-'UCI OCUPADA COVID'!NX7</f>
+        <v>71</v>
+      </c>
+      <c r="NY7">
+        <f>+'UCI OCUPADA TOTAL'!NY7-'UCI OCUPADA COVID'!NY7</f>
+        <v>73</v>
+      </c>
+      <c r="NZ7">
+        <f>+'UCI OCUPADA TOTAL'!NZ7-'UCI OCUPADA COVID'!NZ7</f>
+        <v>79</v>
+      </c>
+      <c r="OA7">
+        <f>+'UCI OCUPADA TOTAL'!OA7-'UCI OCUPADA COVID'!OA7</f>
+        <v>78</v>
+      </c>
+      <c r="OB7">
+        <f>+'UCI OCUPADA TOTAL'!OB7-'UCI OCUPADA COVID'!OB7</f>
+        <v>84</v>
+      </c>
+      <c r="OC7">
+        <f>+'UCI OCUPADA TOTAL'!OC7-'UCI OCUPADA COVID'!OC7</f>
+        <v>82</v>
+      </c>
+      <c r="OD7">
+        <f>+'UCI OCUPADA TOTAL'!OD7-'UCI OCUPADA COVID'!OD7</f>
+        <v>83</v>
+      </c>
     </row>
-    <row r="8" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -81060,8 +82404,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW8-'UCI OCUPADA COVID'!NW8</f>
         <v>609</v>
       </c>
+      <c r="NX8">
+        <f>+'UCI OCUPADA TOTAL'!NX8-'UCI OCUPADA COVID'!NX8</f>
+        <v>628</v>
+      </c>
+      <c r="NY8">
+        <f>+'UCI OCUPADA TOTAL'!NY8-'UCI OCUPADA COVID'!NY8</f>
+        <v>654</v>
+      </c>
+      <c r="NZ8">
+        <f>+'UCI OCUPADA TOTAL'!NZ8-'UCI OCUPADA COVID'!NZ8</f>
+        <v>650</v>
+      </c>
+      <c r="OA8">
+        <f>+'UCI OCUPADA TOTAL'!OA8-'UCI OCUPADA COVID'!OA8</f>
+        <v>656</v>
+      </c>
+      <c r="OB8">
+        <f>+'UCI OCUPADA TOTAL'!OB8-'UCI OCUPADA COVID'!OB8</f>
+        <v>646</v>
+      </c>
+      <c r="OC8">
+        <f>+'UCI OCUPADA TOTAL'!OC8-'UCI OCUPADA COVID'!OC8</f>
+        <v>653</v>
+      </c>
+      <c r="OD8">
+        <f>+'UCI OCUPADA TOTAL'!OD8-'UCI OCUPADA COVID'!OD8</f>
+        <v>664</v>
+      </c>
     </row>
-    <row r="9" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -82329,8 +83701,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW9-'UCI OCUPADA COVID'!NW9</f>
         <v>22</v>
       </c>
+      <c r="NX9">
+        <f>+'UCI OCUPADA TOTAL'!NX9-'UCI OCUPADA COVID'!NX9</f>
+        <v>21</v>
+      </c>
+      <c r="NY9">
+        <f>+'UCI OCUPADA TOTAL'!NY9-'UCI OCUPADA COVID'!NY9</f>
+        <v>25</v>
+      </c>
+      <c r="NZ9">
+        <f>+'UCI OCUPADA TOTAL'!NZ9-'UCI OCUPADA COVID'!NZ9</f>
+        <v>31</v>
+      </c>
+      <c r="OA9">
+        <f>+'UCI OCUPADA TOTAL'!OA9-'UCI OCUPADA COVID'!OA9</f>
+        <v>31</v>
+      </c>
+      <c r="OB9">
+        <f>+'UCI OCUPADA TOTAL'!OB9-'UCI OCUPADA COVID'!OB9</f>
+        <v>31</v>
+      </c>
+      <c r="OC9">
+        <f>+'UCI OCUPADA TOTAL'!OC9-'UCI OCUPADA COVID'!OC9</f>
+        <v>39</v>
+      </c>
+      <c r="OD9">
+        <f>+'UCI OCUPADA TOTAL'!OD9-'UCI OCUPADA COVID'!OD9</f>
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -83598,8 +84998,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW10-'UCI OCUPADA COVID'!NW10</f>
         <v>20</v>
       </c>
+      <c r="NX10">
+        <f>+'UCI OCUPADA TOTAL'!NX10-'UCI OCUPADA COVID'!NX10</f>
+        <v>18</v>
+      </c>
+      <c r="NY10">
+        <f>+'UCI OCUPADA TOTAL'!NY10-'UCI OCUPADA COVID'!NY10</f>
+        <v>22</v>
+      </c>
+      <c r="NZ10">
+        <f>+'UCI OCUPADA TOTAL'!NZ10-'UCI OCUPADA COVID'!NZ10</f>
+        <v>24</v>
+      </c>
+      <c r="OA10">
+        <f>+'UCI OCUPADA TOTAL'!OA10-'UCI OCUPADA COVID'!OA10</f>
+        <v>21</v>
+      </c>
+      <c r="OB10">
+        <f>+'UCI OCUPADA TOTAL'!OB10-'UCI OCUPADA COVID'!OB10</f>
+        <v>23</v>
+      </c>
+      <c r="OC10">
+        <f>+'UCI OCUPADA TOTAL'!OC10-'UCI OCUPADA COVID'!OC10</f>
+        <v>24</v>
+      </c>
+      <c r="OD10">
+        <f>+'UCI OCUPADA TOTAL'!OD10-'UCI OCUPADA COVID'!OD10</f>
+        <v>24</v>
+      </c>
     </row>
-    <row r="11" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -84867,8 +86295,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW11-'UCI OCUPADA COVID'!NW11</f>
         <v>16</v>
       </c>
+      <c r="NX11">
+        <f>+'UCI OCUPADA TOTAL'!NX11-'UCI OCUPADA COVID'!NX11</f>
+        <v>16</v>
+      </c>
+      <c r="NY11">
+        <f>+'UCI OCUPADA TOTAL'!NY11-'UCI OCUPADA COVID'!NY11</f>
+        <v>17</v>
+      </c>
+      <c r="NZ11">
+        <f>+'UCI OCUPADA TOTAL'!NZ11-'UCI OCUPADA COVID'!NZ11</f>
+        <v>15</v>
+      </c>
+      <c r="OA11">
+        <f>+'UCI OCUPADA TOTAL'!OA11-'UCI OCUPADA COVID'!OA11</f>
+        <v>15</v>
+      </c>
+      <c r="OB11">
+        <f>+'UCI OCUPADA TOTAL'!OB11-'UCI OCUPADA COVID'!OB11</f>
+        <v>17</v>
+      </c>
+      <c r="OC11">
+        <f>+'UCI OCUPADA TOTAL'!OC11-'UCI OCUPADA COVID'!OC11</f>
+        <v>15</v>
+      </c>
+      <c r="OD11">
+        <f>+'UCI OCUPADA TOTAL'!OD11-'UCI OCUPADA COVID'!OD11</f>
+        <v>14</v>
+      </c>
     </row>
-    <row r="12" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -86136,8 +87592,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW12-'UCI OCUPADA COVID'!NW12</f>
         <v>70</v>
       </c>
+      <c r="NX12">
+        <f>+'UCI OCUPADA TOTAL'!NX12-'UCI OCUPADA COVID'!NX12</f>
+        <v>76</v>
+      </c>
+      <c r="NY12">
+        <f>+'UCI OCUPADA TOTAL'!NY12-'UCI OCUPADA COVID'!NY12</f>
+        <v>78</v>
+      </c>
+      <c r="NZ12">
+        <f>+'UCI OCUPADA TOTAL'!NZ12-'UCI OCUPADA COVID'!NZ12</f>
+        <v>82</v>
+      </c>
+      <c r="OA12">
+        <f>+'UCI OCUPADA TOTAL'!OA12-'UCI OCUPADA COVID'!OA12</f>
+        <v>81</v>
+      </c>
+      <c r="OB12">
+        <f>+'UCI OCUPADA TOTAL'!OB12-'UCI OCUPADA COVID'!OB12</f>
+        <v>88</v>
+      </c>
+      <c r="OC12">
+        <f>+'UCI OCUPADA TOTAL'!OC12-'UCI OCUPADA COVID'!OC12</f>
+        <v>85</v>
+      </c>
+      <c r="OD12">
+        <f>+'UCI OCUPADA TOTAL'!OD12-'UCI OCUPADA COVID'!OD12</f>
+        <v>85</v>
+      </c>
     </row>
-    <row r="13" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -87405,8 +88889,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW13-'UCI OCUPADA COVID'!NW13</f>
         <v>33</v>
       </c>
+      <c r="NX13">
+        <f>+'UCI OCUPADA TOTAL'!NX13-'UCI OCUPADA COVID'!NX13</f>
+        <v>29</v>
+      </c>
+      <c r="NY13">
+        <f>+'UCI OCUPADA TOTAL'!NY13-'UCI OCUPADA COVID'!NY13</f>
+        <v>28</v>
+      </c>
+      <c r="NZ13">
+        <f>+'UCI OCUPADA TOTAL'!NZ13-'UCI OCUPADA COVID'!NZ13</f>
+        <v>32</v>
+      </c>
+      <c r="OA13">
+        <f>+'UCI OCUPADA TOTAL'!OA13-'UCI OCUPADA COVID'!OA13</f>
+        <v>36</v>
+      </c>
+      <c r="OB13">
+        <f>+'UCI OCUPADA TOTAL'!OB13-'UCI OCUPADA COVID'!OB13</f>
+        <v>29</v>
+      </c>
+      <c r="OC13">
+        <f>+'UCI OCUPADA TOTAL'!OC13-'UCI OCUPADA COVID'!OC13</f>
+        <v>26</v>
+      </c>
+      <c r="OD13">
+        <f>+'UCI OCUPADA TOTAL'!OD13-'UCI OCUPADA COVID'!OD13</f>
+        <v>33</v>
+      </c>
     </row>
-    <row r="14" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -88674,8 +90186,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW14-'UCI OCUPADA COVID'!NW14</f>
         <v>16</v>
       </c>
+      <c r="NX14">
+        <f>+'UCI OCUPADA TOTAL'!NX14-'UCI OCUPADA COVID'!NX14</f>
+        <v>20</v>
+      </c>
+      <c r="NY14">
+        <f>+'UCI OCUPADA TOTAL'!NY14-'UCI OCUPADA COVID'!NY14</f>
+        <v>17</v>
+      </c>
+      <c r="NZ14">
+        <f>+'UCI OCUPADA TOTAL'!NZ14-'UCI OCUPADA COVID'!NZ14</f>
+        <v>18</v>
+      </c>
+      <c r="OA14">
+        <f>+'UCI OCUPADA TOTAL'!OA14-'UCI OCUPADA COVID'!OA14</f>
+        <v>14</v>
+      </c>
+      <c r="OB14">
+        <f>+'UCI OCUPADA TOTAL'!OB14-'UCI OCUPADA COVID'!OB14</f>
+        <v>12</v>
+      </c>
+      <c r="OC14">
+        <f>+'UCI OCUPADA TOTAL'!OC14-'UCI OCUPADA COVID'!OC14</f>
+        <v>14</v>
+      </c>
+      <c r="OD14">
+        <f>+'UCI OCUPADA TOTAL'!OD14-'UCI OCUPADA COVID'!OD14</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="15" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -89943,8 +91483,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW15-'UCI OCUPADA COVID'!NW15</f>
         <v>37</v>
       </c>
+      <c r="NX15">
+        <f>+'UCI OCUPADA TOTAL'!NX15-'UCI OCUPADA COVID'!NX15</f>
+        <v>34</v>
+      </c>
+      <c r="NY15">
+        <f>+'UCI OCUPADA TOTAL'!NY15-'UCI OCUPADA COVID'!NY15</f>
+        <v>38</v>
+      </c>
+      <c r="NZ15">
+        <f>+'UCI OCUPADA TOTAL'!NZ15-'UCI OCUPADA COVID'!NZ15</f>
+        <v>36</v>
+      </c>
+      <c r="OA15">
+        <f>+'UCI OCUPADA TOTAL'!OA15-'UCI OCUPADA COVID'!OA15</f>
+        <v>34</v>
+      </c>
+      <c r="OB15">
+        <f>+'UCI OCUPADA TOTAL'!OB15-'UCI OCUPADA COVID'!OB15</f>
+        <v>31</v>
+      </c>
+      <c r="OC15">
+        <f>+'UCI OCUPADA TOTAL'!OC15-'UCI OCUPADA COVID'!OC15</f>
+        <v>28</v>
+      </c>
+      <c r="OD15">
+        <f>+'UCI OCUPADA TOTAL'!OD15-'UCI OCUPADA COVID'!OD15</f>
+        <v>35</v>
+      </c>
     </row>
-    <row r="16" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -91212,8 +92780,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW16-'UCI OCUPADA COVID'!NW16</f>
         <v>3</v>
       </c>
+      <c r="NX16">
+        <f>+'UCI OCUPADA TOTAL'!NX16-'UCI OCUPADA COVID'!NX16</f>
+        <v>2</v>
+      </c>
+      <c r="NY16">
+        <f>+'UCI OCUPADA TOTAL'!NY16-'UCI OCUPADA COVID'!NY16</f>
+        <v>3</v>
+      </c>
+      <c r="NZ16">
+        <f>+'UCI OCUPADA TOTAL'!NZ16-'UCI OCUPADA COVID'!NZ16</f>
+        <v>2</v>
+      </c>
+      <c r="OA16">
+        <f>+'UCI OCUPADA TOTAL'!OA16-'UCI OCUPADA COVID'!OA16</f>
+        <v>2</v>
+      </c>
+      <c r="OB16">
+        <f>+'UCI OCUPADA TOTAL'!OB16-'UCI OCUPADA COVID'!OB16</f>
+        <v>2</v>
+      </c>
+      <c r="OC16">
+        <f>+'UCI OCUPADA TOTAL'!OC16-'UCI OCUPADA COVID'!OC16</f>
+        <v>3</v>
+      </c>
+      <c r="OD16">
+        <f>+'UCI OCUPADA TOTAL'!OD16-'UCI OCUPADA COVID'!OD16</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -92481,8 +94077,36 @@
         <f>+'UCI OCUPADA TOTAL'!NW17-'UCI OCUPADA COVID'!NW17</f>
         <v>10</v>
       </c>
+      <c r="NX17">
+        <f>+'UCI OCUPADA TOTAL'!NX17-'UCI OCUPADA COVID'!NX17</f>
+        <v>8</v>
+      </c>
+      <c r="NY17">
+        <f>+'UCI OCUPADA TOTAL'!NY17-'UCI OCUPADA COVID'!NY17</f>
+        <v>5</v>
+      </c>
+      <c r="NZ17">
+        <f>+'UCI OCUPADA TOTAL'!NZ17-'UCI OCUPADA COVID'!NZ17</f>
+        <v>4</v>
+      </c>
+      <c r="OA17">
+        <f>+'UCI OCUPADA TOTAL'!OA17-'UCI OCUPADA COVID'!OA17</f>
+        <v>9</v>
+      </c>
+      <c r="OB17">
+        <f>+'UCI OCUPADA TOTAL'!OB17-'UCI OCUPADA COVID'!OB17</f>
+        <v>9</v>
+      </c>
+      <c r="OC17">
+        <f>+'UCI OCUPADA TOTAL'!OC17-'UCI OCUPADA COVID'!OC17</f>
+        <v>10</v>
+      </c>
+      <c r="OD17">
+        <f>+'UCI OCUPADA TOTAL'!OD17-'UCI OCUPADA COVID'!OD17</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -93750,48 +95374,76 @@
         <f>+'UCI OCUPADA TOTAL'!NW18-'UCI OCUPADA COVID'!NW18</f>
         <v>1002</v>
       </c>
+      <c r="NX18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!NX18-'UCI OCUPADA COVID'!NX18</f>
+        <v>1026</v>
+      </c>
+      <c r="NY18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!NY18-'UCI OCUPADA COVID'!NY18</f>
+        <v>1072</v>
+      </c>
+      <c r="NZ18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!NZ18-'UCI OCUPADA COVID'!NZ18</f>
+        <v>1074</v>
+      </c>
+      <c r="OA18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OA18-'UCI OCUPADA COVID'!OA18</f>
+        <v>1083</v>
+      </c>
+      <c r="OB18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OB18-'UCI OCUPADA COVID'!OB18</f>
+        <v>1076</v>
+      </c>
+      <c r="OC18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OC18-'UCI OCUPADA COVID'!OC18</f>
+        <v>1087</v>
+      </c>
+      <c r="OD18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OD18-'UCI OCUPADA COVID'!OD18</f>
+        <v>1110</v>
+      </c>
     </row>
-    <row r="19" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:387" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reporte diario, miércoles 19 de mayo de 2021
Signed-off-by: MinCiencia GitHub Actions Bot <actions@github.com>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -2910,10 +2910,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NU1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="OB1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
+      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4118,8 +4118,29 @@
       <c r="OD1" s="8">
         <v>44327</v>
       </c>
+      <c r="OE1" s="8">
+        <v>44328</v>
+      </c>
+      <c r="OF1" s="8">
+        <v>44329</v>
+      </c>
+      <c r="OG1" s="8">
+        <v>44330</v>
+      </c>
+      <c r="OH1" s="8">
+        <v>44331</v>
+      </c>
+      <c r="OI1" s="8">
+        <v>44332</v>
+      </c>
+      <c r="OJ1" s="8">
+        <v>44333</v>
+      </c>
+      <c r="OK1" s="8">
+        <v>44334</v>
+      </c>
     </row>
-    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5302,8 +5323,29 @@
       <c r="OD2" s="11">
         <v>40</v>
       </c>
+      <c r="OE2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OF2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OG2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OH2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OI2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OJ2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OK2" s="11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6486,8 +6528,29 @@
       <c r="OD3" s="11">
         <v>62</v>
       </c>
+      <c r="OE3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OF3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OG3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OH3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OI3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OJ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OK3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7670,8 +7733,29 @@
       <c r="OD4" s="11">
         <v>165</v>
       </c>
+      <c r="OE4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OF4" s="11">
+        <v>161</v>
+      </c>
+      <c r="OG4" s="11">
+        <v>161</v>
+      </c>
+      <c r="OH4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OI4" s="11">
+        <v>166</v>
+      </c>
+      <c r="OJ4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OK4" s="11">
+        <v>163</v>
+      </c>
     </row>
-    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -8854,8 +8938,29 @@
       <c r="OD5" s="11">
         <v>34</v>
       </c>
+      <c r="OE5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OF5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OG5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OH5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OI5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OJ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OK5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10038,8 +10143,29 @@
       <c r="OD6" s="11">
         <v>140</v>
       </c>
+      <c r="OE6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OF6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OG6" s="11">
+        <v>140</v>
+      </c>
+      <c r="OH6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OI6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OJ6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OK6" s="11">
+        <v>134</v>
+      </c>
     </row>
-    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -11222,8 +11348,29 @@
       <c r="OD7" s="11">
         <v>342</v>
       </c>
+      <c r="OE7" s="11">
+        <v>340</v>
+      </c>
+      <c r="OF7" s="11">
+        <v>340</v>
+      </c>
+      <c r="OG7" s="11">
+        <v>338</v>
+      </c>
+      <c r="OH7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OI7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OJ7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OK7" s="11">
+        <v>334</v>
+      </c>
     </row>
-    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12406,8 +12553,29 @@
       <c r="OD8" s="11">
         <v>2607</v>
       </c>
+      <c r="OE8" s="11">
+        <v>2602</v>
+      </c>
+      <c r="OF8" s="11">
+        <v>2598</v>
+      </c>
+      <c r="OG8" s="11">
+        <v>2597</v>
+      </c>
+      <c r="OH8" s="11">
+        <v>2595</v>
+      </c>
+      <c r="OI8" s="11">
+        <v>2595</v>
+      </c>
+      <c r="OJ8" s="11">
+        <v>2594</v>
+      </c>
+      <c r="OK8" s="11">
+        <v>2593</v>
+      </c>
     </row>
-    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13590,8 +13758,29 @@
       <c r="OD9" s="11">
         <v>206</v>
       </c>
+      <c r="OE9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OF9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OG9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OH9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OI9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OJ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OK9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -14774,8 +14963,29 @@
       <c r="OD10" s="11">
         <v>166</v>
       </c>
+      <c r="OE10" s="11">
+        <v>157</v>
+      </c>
+      <c r="OF10" s="11">
+        <v>163</v>
+      </c>
+      <c r="OG10" s="11">
+        <v>162</v>
+      </c>
+      <c r="OH10" s="11">
+        <v>162</v>
+      </c>
+      <c r="OI10" s="11">
+        <v>156</v>
+      </c>
+      <c r="OJ10" s="11">
+        <v>162</v>
+      </c>
+      <c r="OK10" s="11">
+        <v>162</v>
+      </c>
     </row>
-    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -15958,8 +16168,29 @@
       <c r="OD11" s="11">
         <v>73</v>
       </c>
+      <c r="OE11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OF11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OG11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OH11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OI11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OJ11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OK11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -17142,8 +17373,29 @@
       <c r="OD12" s="11">
         <v>316</v>
       </c>
+      <c r="OE12" s="11">
+        <v>316</v>
+      </c>
+      <c r="OF12" s="11">
+        <v>316</v>
+      </c>
+      <c r="OG12" s="11">
+        <v>311</v>
+      </c>
+      <c r="OH12" s="11">
+        <v>311</v>
+      </c>
+      <c r="OI12" s="11">
+        <v>310</v>
+      </c>
+      <c r="OJ12" s="11">
+        <v>310</v>
+      </c>
+      <c r="OK12" s="11">
+        <v>310</v>
+      </c>
     </row>
-    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -18326,8 +18578,29 @@
       <c r="OD13" s="11">
         <v>151</v>
       </c>
+      <c r="OE13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OF13" s="11">
+        <v>149</v>
+      </c>
+      <c r="OG13" s="11">
+        <v>148</v>
+      </c>
+      <c r="OH13" s="11">
+        <v>145</v>
+      </c>
+      <c r="OI13" s="11">
+        <v>145</v>
+      </c>
+      <c r="OJ13" s="11">
+        <v>145</v>
+      </c>
+      <c r="OK13" s="11">
+        <v>145</v>
+      </c>
     </row>
-    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -19510,8 +19783,29 @@
       <c r="OD14" s="11">
         <v>41</v>
       </c>
+      <c r="OE14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OF14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OG14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OH14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OI14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OJ14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OK14" s="11">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -20694,8 +20988,29 @@
       <c r="OD15" s="11">
         <v>128</v>
       </c>
+      <c r="OE15" s="11">
+        <v>128</v>
+      </c>
+      <c r="OF15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OG15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OH15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OI15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OJ15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OK15" s="11">
+        <v>126</v>
+      </c>
     </row>
-    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -21878,8 +22193,29 @@
       <c r="OD16" s="11">
         <v>10</v>
       </c>
+      <c r="OE16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OF16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OG16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OH16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OI16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OJ16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OK16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -23062,8 +23398,29 @@
       <c r="OD17" s="11">
         <v>44</v>
       </c>
+      <c r="OE17" s="11">
+        <v>43</v>
+      </c>
+      <c r="OF17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OG17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OH17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OI17" s="11">
+        <v>48</v>
+      </c>
+      <c r="OJ17" s="11">
+        <v>48</v>
+      </c>
+      <c r="OK17" s="11">
+        <v>48</v>
+      </c>
     </row>
-    <row r="18" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -24239,7 +24596,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:OD18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:OK18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -24366,9 +24723,37 @@
         <f t="shared" si="7"/>
         <v>4525</v>
       </c>
+      <c r="OE18" s="6">
+        <f t="shared" si="7"/>
+        <v>4505</v>
+      </c>
+      <c r="OF18" s="6">
+        <f t="shared" si="7"/>
+        <v>4506</v>
+      </c>
+      <c r="OG18" s="6">
+        <f t="shared" si="7"/>
+        <v>4496</v>
+      </c>
+      <c r="OH18" s="6">
+        <f t="shared" si="7"/>
+        <v>4484</v>
+      </c>
+      <c r="OI18" s="6">
+        <f t="shared" si="7"/>
+        <v>4480</v>
+      </c>
+      <c r="OJ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4483</v>
+      </c>
+      <c r="OK18" s="6">
+        <f t="shared" si="7"/>
+        <v>4481</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:394 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -24386,12 +24771,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OD36"/>
+  <dimension ref="A1:OK36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OB1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
+      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24411,7 +24796,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -25594,8 +25979,29 @@
       <c r="OD1" s="8">
         <v>44327</v>
       </c>
+      <c r="OE1" s="8">
+        <v>44328</v>
+      </c>
+      <c r="OF1" s="8">
+        <v>44329</v>
+      </c>
+      <c r="OG1" s="8">
+        <v>44330</v>
+      </c>
+      <c r="OH1" s="8">
+        <v>44331</v>
+      </c>
+      <c r="OI1" s="8">
+        <v>44332</v>
+      </c>
+      <c r="OJ1" s="8">
+        <v>44333</v>
+      </c>
+      <c r="OK1" s="8">
+        <v>44334</v>
+      </c>
     </row>
-    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -26778,8 +27184,29 @@
       <c r="OD2">
         <v>36</v>
       </c>
+      <c r="OE2">
+        <v>37</v>
+      </c>
+      <c r="OF2">
+        <v>34</v>
+      </c>
+      <c r="OG2">
+        <v>34</v>
+      </c>
+      <c r="OH2">
+        <v>34</v>
+      </c>
+      <c r="OI2">
+        <v>33</v>
+      </c>
+      <c r="OJ2">
+        <v>35</v>
+      </c>
+      <c r="OK2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -27962,8 +28389,29 @@
       <c r="OD3">
         <v>56</v>
       </c>
+      <c r="OE3">
+        <v>54</v>
+      </c>
+      <c r="OF3">
+        <v>50</v>
+      </c>
+      <c r="OG3">
+        <v>53</v>
+      </c>
+      <c r="OH3">
+        <v>51</v>
+      </c>
+      <c r="OI3">
+        <v>49</v>
+      </c>
+      <c r="OJ3">
+        <v>54</v>
+      </c>
+      <c r="OK3">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -29146,8 +29594,29 @@
       <c r="OD4">
         <v>149</v>
       </c>
+      <c r="OE4">
+        <v>142</v>
+      </c>
+      <c r="OF4">
+        <v>150</v>
+      </c>
+      <c r="OG4">
+        <v>140</v>
+      </c>
+      <c r="OH4">
+        <v>155</v>
+      </c>
+      <c r="OI4">
+        <v>153</v>
+      </c>
+      <c r="OJ4">
+        <v>154</v>
+      </c>
+      <c r="OK4">
+        <v>152</v>
+      </c>
     </row>
-    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -30330,8 +30799,29 @@
       <c r="OD5">
         <v>30</v>
       </c>
+      <c r="OE5">
+        <v>32</v>
+      </c>
+      <c r="OF5">
+        <v>31</v>
+      </c>
+      <c r="OG5">
+        <v>31</v>
+      </c>
+      <c r="OH5">
+        <v>29</v>
+      </c>
+      <c r="OI5">
+        <v>29</v>
+      </c>
+      <c r="OJ5">
+        <v>28</v>
+      </c>
+      <c r="OK5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -31514,8 +32004,29 @@
       <c r="OD6">
         <v>126</v>
       </c>
+      <c r="OE6">
+        <v>122</v>
+      </c>
+      <c r="OF6">
+        <v>125</v>
+      </c>
+      <c r="OG6">
+        <v>122</v>
+      </c>
+      <c r="OH6">
+        <v>124</v>
+      </c>
+      <c r="OI6">
+        <v>121</v>
+      </c>
+      <c r="OJ6">
+        <v>125</v>
+      </c>
+      <c r="OK6">
+        <v>125</v>
+      </c>
     </row>
-    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -32698,8 +33209,29 @@
       <c r="OD7">
         <v>328</v>
       </c>
+      <c r="OE7">
+        <v>313</v>
+      </c>
+      <c r="OF7">
+        <v>320</v>
+      </c>
+      <c r="OG7">
+        <v>322</v>
+      </c>
+      <c r="OH7">
+        <v>318</v>
+      </c>
+      <c r="OI7">
+        <v>320</v>
+      </c>
+      <c r="OJ7">
+        <v>321</v>
+      </c>
+      <c r="OK7">
+        <v>314</v>
+      </c>
     </row>
-    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -33882,8 +34414,29 @@
       <c r="OD8">
         <v>2498</v>
       </c>
+      <c r="OE8">
+        <v>2476</v>
+      </c>
+      <c r="OF8">
+        <v>2447</v>
+      </c>
+      <c r="OG8">
+        <v>2473</v>
+      </c>
+      <c r="OH8">
+        <v>2462</v>
+      </c>
+      <c r="OI8">
+        <v>2470</v>
+      </c>
+      <c r="OJ8">
+        <v>2471</v>
+      </c>
+      <c r="OK8">
+        <v>2488</v>
+      </c>
     </row>
-    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -35066,8 +35619,29 @@
       <c r="OD9">
         <v>164</v>
       </c>
+      <c r="OE9">
+        <v>160</v>
+      </c>
+      <c r="OF9">
+        <v>159</v>
+      </c>
+      <c r="OG9">
+        <v>164</v>
+      </c>
+      <c r="OH9">
+        <v>164</v>
+      </c>
+      <c r="OI9">
+        <v>157</v>
+      </c>
+      <c r="OJ9">
+        <v>162</v>
+      </c>
+      <c r="OK9">
+        <v>162</v>
+      </c>
     </row>
-    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -36250,8 +36824,29 @@
       <c r="OD10">
         <v>158</v>
       </c>
+      <c r="OE10">
+        <v>148</v>
+      </c>
+      <c r="OF10">
+        <v>145</v>
+      </c>
+      <c r="OG10">
+        <v>146</v>
+      </c>
+      <c r="OH10">
+        <v>137</v>
+      </c>
+      <c r="OI10">
+        <v>133</v>
+      </c>
+      <c r="OJ10">
+        <v>132</v>
+      </c>
+      <c r="OK10">
+        <v>132</v>
+      </c>
     </row>
-    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -37434,8 +38029,29 @@
       <c r="OD11">
         <v>59</v>
       </c>
+      <c r="OE11">
+        <v>57</v>
+      </c>
+      <c r="OF11">
+        <v>59</v>
+      </c>
+      <c r="OG11">
+        <v>56</v>
+      </c>
+      <c r="OH11">
+        <v>56</v>
+      </c>
+      <c r="OI11">
+        <v>60</v>
+      </c>
+      <c r="OJ11">
+        <v>60</v>
+      </c>
+      <c r="OK11">
+        <v>61</v>
+      </c>
     </row>
-    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -38618,8 +39234,29 @@
       <c r="OD12">
         <v>280</v>
       </c>
+      <c r="OE12">
+        <v>284</v>
+      </c>
+      <c r="OF12">
+        <v>282</v>
+      </c>
+      <c r="OG12">
+        <v>281</v>
+      </c>
+      <c r="OH12">
+        <v>271</v>
+      </c>
+      <c r="OI12">
+        <v>274</v>
+      </c>
+      <c r="OJ12">
+        <v>273</v>
+      </c>
+      <c r="OK12">
+        <v>275</v>
+      </c>
     </row>
-    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -39802,8 +40439,29 @@
       <c r="OD13">
         <v>142</v>
       </c>
+      <c r="OE13">
+        <v>143</v>
+      </c>
+      <c r="OF13">
+        <v>138</v>
+      </c>
+      <c r="OG13">
+        <v>139</v>
+      </c>
+      <c r="OH13">
+        <v>139</v>
+      </c>
+      <c r="OI13">
+        <v>134</v>
+      </c>
+      <c r="OJ13">
+        <v>138</v>
+      </c>
+      <c r="OK13">
+        <v>133</v>
+      </c>
     </row>
-    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -40986,8 +41644,29 @@
       <c r="OD14">
         <v>34</v>
       </c>
+      <c r="OE14">
+        <v>34</v>
+      </c>
+      <c r="OF14">
+        <v>39</v>
+      </c>
+      <c r="OG14">
+        <v>38</v>
+      </c>
+      <c r="OH14">
+        <v>39</v>
+      </c>
+      <c r="OI14">
+        <v>38</v>
+      </c>
+      <c r="OJ14">
+        <v>39</v>
+      </c>
+      <c r="OK14">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -42170,8 +42849,29 @@
       <c r="OD15">
         <v>112</v>
       </c>
+      <c r="OE15">
+        <v>112</v>
+      </c>
+      <c r="OF15">
+        <v>112</v>
+      </c>
+      <c r="OG15">
+        <v>118</v>
+      </c>
+      <c r="OH15">
+        <v>117</v>
+      </c>
+      <c r="OI15">
+        <v>117</v>
+      </c>
+      <c r="OJ15">
+        <v>118</v>
+      </c>
+      <c r="OK15">
+        <v>117</v>
+      </c>
     </row>
-    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -43354,8 +44054,29 @@
       <c r="OD16">
         <v>6</v>
       </c>
+      <c r="OE16">
+        <v>8</v>
+      </c>
+      <c r="OF16">
+        <v>8</v>
+      </c>
+      <c r="OG16">
+        <v>10</v>
+      </c>
+      <c r="OH16">
+        <v>10</v>
+      </c>
+      <c r="OI16">
+        <v>9</v>
+      </c>
+      <c r="OJ16">
+        <v>9</v>
+      </c>
+      <c r="OK16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -44538,8 +45259,29 @@
       <c r="OD17">
         <v>34</v>
       </c>
+      <c r="OE17">
+        <v>36</v>
+      </c>
+      <c r="OF17">
+        <v>39</v>
+      </c>
+      <c r="OG17">
+        <v>37</v>
+      </c>
+      <c r="OH17">
+        <v>41</v>
+      </c>
+      <c r="OI17">
+        <v>42</v>
+      </c>
+      <c r="OJ17">
+        <v>41</v>
+      </c>
+      <c r="OK17">
+        <v>37</v>
+      </c>
     </row>
-    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -45631,7 +46373,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:OD18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:OK18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -45822,8 +46564,36 @@
         <f t="shared" si="1"/>
         <v>4212</v>
       </c>
+      <c r="OE18" s="6">
+        <f t="shared" si="1"/>
+        <v>4158</v>
+      </c>
+      <c r="OF18" s="6">
+        <f t="shared" si="1"/>
+        <v>4138</v>
+      </c>
+      <c r="OG18" s="6">
+        <f t="shared" si="1"/>
+        <v>4164</v>
+      </c>
+      <c r="OH18" s="6">
+        <f t="shared" si="1"/>
+        <v>4147</v>
+      </c>
+      <c r="OI18" s="6">
+        <f t="shared" si="1"/>
+        <v>4139</v>
+      </c>
+      <c r="OJ18" s="6">
+        <f t="shared" si="1"/>
+        <v>4160</v>
+      </c>
+      <c r="OK18" s="6">
+        <f t="shared" si="1"/>
+        <v>4166</v>
+      </c>
     </row>
-    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -46106,7 +46876,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -46389,7 +47159,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -46672,7 +47442,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -46955,7 +47725,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -47238,7 +48008,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -47521,7 +48291,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -47804,7 +48574,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -48087,7 +48857,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -48370,7 +49140,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -48653,7 +49423,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -48936,7 +49706,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -49219,7 +49989,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -50642,12 +51412,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OD34"/>
+  <dimension ref="A1:OK34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OC1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
+      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50668,7 +51438,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -51851,8 +52621,29 @@
       <c r="OD1" s="8">
         <v>44327</v>
       </c>
+      <c r="OE1" s="8">
+        <v>44328</v>
+      </c>
+      <c r="OF1" s="8">
+        <v>44329</v>
+      </c>
+      <c r="OG1" s="8">
+        <v>44330</v>
+      </c>
+      <c r="OH1" s="8">
+        <v>44331</v>
+      </c>
+      <c r="OI1" s="8">
+        <v>44332</v>
+      </c>
+      <c r="OJ1" s="8">
+        <v>44333</v>
+      </c>
+      <c r="OK1" s="8">
+        <v>44334</v>
+      </c>
     </row>
-    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -53035,8 +53826,29 @@
       <c r="OD2">
         <v>30</v>
       </c>
+      <c r="OE2">
+        <v>29</v>
+      </c>
+      <c r="OF2">
+        <v>28</v>
+      </c>
+      <c r="OG2">
+        <v>28</v>
+      </c>
+      <c r="OH2">
+        <v>26</v>
+      </c>
+      <c r="OI2">
+        <v>24</v>
+      </c>
+      <c r="OJ2">
+        <v>27</v>
+      </c>
+      <c r="OK2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -54219,8 +55031,29 @@
       <c r="OD3">
         <v>53</v>
       </c>
+      <c r="OE3">
+        <v>50</v>
+      </c>
+      <c r="OF3">
+        <v>47</v>
+      </c>
+      <c r="OG3">
+        <v>51</v>
+      </c>
+      <c r="OH3">
+        <v>49</v>
+      </c>
+      <c r="OI3">
+        <v>48</v>
+      </c>
+      <c r="OJ3">
+        <v>48</v>
+      </c>
+      <c r="OK3">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -55403,8 +56236,29 @@
       <c r="OD4">
         <v>92</v>
       </c>
+      <c r="OE4">
+        <v>90</v>
+      </c>
+      <c r="OF4">
+        <v>86</v>
+      </c>
+      <c r="OG4">
+        <v>84</v>
+      </c>
+      <c r="OH4">
+        <v>88</v>
+      </c>
+      <c r="OI4">
+        <v>88</v>
+      </c>
+      <c r="OJ4">
+        <v>90</v>
+      </c>
+      <c r="OK4">
+        <v>92</v>
+      </c>
     </row>
-    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -56587,8 +57441,29 @@
       <c r="OD5">
         <v>19</v>
       </c>
+      <c r="OE5">
+        <v>23</v>
+      </c>
+      <c r="OF5">
+        <v>20</v>
+      </c>
+      <c r="OG5">
+        <v>22</v>
+      </c>
+      <c r="OH5">
+        <v>20</v>
+      </c>
+      <c r="OI5">
+        <v>23</v>
+      </c>
+      <c r="OJ5">
+        <v>23</v>
+      </c>
+      <c r="OK5">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -57771,8 +58646,29 @@
       <c r="OD6">
         <v>95</v>
       </c>
+      <c r="OE6">
+        <v>89</v>
+      </c>
+      <c r="OF6">
+        <v>91</v>
+      </c>
+      <c r="OG6">
+        <v>92</v>
+      </c>
+      <c r="OH6">
+        <v>92</v>
+      </c>
+      <c r="OI6">
+        <v>91</v>
+      </c>
+      <c r="OJ6">
+        <v>93</v>
+      </c>
+      <c r="OK6">
+        <v>94</v>
+      </c>
     </row>
-    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -58955,8 +59851,29 @@
       <c r="OD7">
         <v>245</v>
       </c>
+      <c r="OE7">
+        <v>234</v>
+      </c>
+      <c r="OF7">
+        <v>232</v>
+      </c>
+      <c r="OG7">
+        <v>220</v>
+      </c>
+      <c r="OH7">
+        <v>218</v>
+      </c>
+      <c r="OI7">
+        <v>225</v>
+      </c>
+      <c r="OJ7">
+        <v>225</v>
+      </c>
+      <c r="OK7">
+        <v>222</v>
+      </c>
     </row>
-    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -60139,8 +61056,29 @@
       <c r="OD8">
         <v>1834</v>
       </c>
+      <c r="OE8">
+        <v>1805</v>
+      </c>
+      <c r="OF8">
+        <v>1759</v>
+      </c>
+      <c r="OG8">
+        <v>1769</v>
+      </c>
+      <c r="OH8">
+        <v>1768</v>
+      </c>
+      <c r="OI8">
+        <v>1765</v>
+      </c>
+      <c r="OJ8">
+        <v>1772</v>
+      </c>
+      <c r="OK8">
+        <v>1787</v>
+      </c>
     </row>
-    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -61323,8 +62261,29 @@
       <c r="OD9">
         <v>122</v>
       </c>
+      <c r="OE9">
+        <v>123</v>
+      </c>
+      <c r="OF9">
+        <v>127</v>
+      </c>
+      <c r="OG9">
+        <v>120</v>
+      </c>
+      <c r="OH9">
+        <v>116</v>
+      </c>
+      <c r="OI9">
+        <v>117</v>
+      </c>
+      <c r="OJ9">
+        <v>118</v>
+      </c>
+      <c r="OK9">
+        <v>115</v>
+      </c>
     </row>
-    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -62507,8 +63466,29 @@
       <c r="OD10">
         <v>134</v>
       </c>
+      <c r="OE10">
+        <v>124</v>
+      </c>
+      <c r="OF10">
+        <v>121</v>
+      </c>
+      <c r="OG10">
+        <v>121</v>
+      </c>
+      <c r="OH10">
+        <v>113</v>
+      </c>
+      <c r="OI10">
+        <v>110</v>
+      </c>
+      <c r="OJ10">
+        <v>106</v>
+      </c>
+      <c r="OK10">
+        <v>107</v>
+      </c>
     </row>
-    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -63691,8 +64671,29 @@
       <c r="OD11">
         <v>45</v>
       </c>
+      <c r="OE11">
+        <v>42</v>
+      </c>
+      <c r="OF11">
+        <v>44</v>
+      </c>
+      <c r="OG11">
+        <v>44</v>
+      </c>
+      <c r="OH11">
+        <v>45</v>
+      </c>
+      <c r="OI11">
+        <v>47</v>
+      </c>
+      <c r="OJ11">
+        <v>48</v>
+      </c>
+      <c r="OK11">
+        <v>47</v>
+      </c>
     </row>
-    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -64875,8 +65876,29 @@
       <c r="OD12">
         <v>195</v>
       </c>
+      <c r="OE12">
+        <v>194</v>
+      </c>
+      <c r="OF12">
+        <v>190</v>
+      </c>
+      <c r="OG12">
+        <v>190</v>
+      </c>
+      <c r="OH12">
+        <v>181</v>
+      </c>
+      <c r="OI12">
+        <v>186</v>
+      </c>
+      <c r="OJ12">
+        <v>185</v>
+      </c>
+      <c r="OK12">
+        <v>185</v>
+      </c>
     </row>
-    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -66059,8 +67081,29 @@
       <c r="OD13">
         <v>109</v>
       </c>
+      <c r="OE13">
+        <v>110</v>
+      </c>
+      <c r="OF13">
+        <v>103</v>
+      </c>
+      <c r="OG13">
+        <v>108</v>
+      </c>
+      <c r="OH13">
+        <v>108</v>
+      </c>
+      <c r="OI13">
+        <v>103</v>
+      </c>
+      <c r="OJ13">
+        <v>104</v>
+      </c>
+      <c r="OK13">
+        <v>99</v>
+      </c>
     </row>
-    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -67243,8 +68286,29 @@
       <c r="OD14">
         <v>22</v>
       </c>
+      <c r="OE14">
+        <v>22</v>
+      </c>
+      <c r="OF14">
+        <v>24</v>
+      </c>
+      <c r="OG14">
+        <v>22</v>
+      </c>
+      <c r="OH14">
+        <v>22</v>
+      </c>
+      <c r="OI14">
+        <v>20</v>
+      </c>
+      <c r="OJ14">
+        <v>20</v>
+      </c>
+      <c r="OK14">
+        <v>22</v>
+      </c>
     </row>
-    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -68427,8 +69491,29 @@
       <c r="OD15">
         <v>77</v>
       </c>
+      <c r="OE15">
+        <v>70</v>
+      </c>
+      <c r="OF15">
+        <v>69</v>
+      </c>
+      <c r="OG15">
+        <v>70</v>
+      </c>
+      <c r="OH15">
+        <v>70</v>
+      </c>
+      <c r="OI15">
+        <v>71</v>
+      </c>
+      <c r="OJ15">
+        <v>74</v>
+      </c>
+      <c r="OK15">
+        <v>74</v>
+      </c>
     </row>
-    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -69611,8 +70696,29 @@
       <c r="OD16">
         <v>5</v>
       </c>
+      <c r="OE16">
+        <v>5</v>
+      </c>
+      <c r="OF16">
+        <v>5</v>
+      </c>
+      <c r="OG16">
+        <v>6</v>
+      </c>
+      <c r="OH16">
+        <v>6</v>
+      </c>
+      <c r="OI16">
+        <v>5</v>
+      </c>
+      <c r="OJ16">
+        <v>5</v>
+      </c>
+      <c r="OK16">
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -70795,8 +71901,29 @@
       <c r="OD17">
         <v>25</v>
       </c>
+      <c r="OE17">
+        <v>26</v>
+      </c>
+      <c r="OF17">
+        <v>30</v>
+      </c>
+      <c r="OG17">
+        <v>29</v>
+      </c>
+      <c r="OH17">
+        <v>31</v>
+      </c>
+      <c r="OI17">
+        <v>31</v>
+      </c>
+      <c r="OJ17">
+        <v>31</v>
+      </c>
+      <c r="OK17">
+        <v>29</v>
+      </c>
     </row>
-    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -71933,7 +73060,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:OD18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:OK18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -72084,50 +73211,78 @@
         <f t="shared" si="1"/>
         <v>3102</v>
       </c>
+      <c r="OE18" s="6">
+        <f t="shared" si="1"/>
+        <v>3036</v>
+      </c>
+      <c r="OF18" s="6">
+        <f t="shared" si="1"/>
+        <v>2976</v>
+      </c>
+      <c r="OG18" s="6">
+        <f t="shared" si="1"/>
+        <v>2976</v>
+      </c>
+      <c r="OH18" s="6">
+        <f t="shared" si="1"/>
+        <v>2953</v>
+      </c>
+      <c r="OI18" s="6">
+        <f t="shared" si="1"/>
+        <v>2954</v>
+      </c>
+      <c r="OJ18" s="6">
+        <f t="shared" si="1"/>
+        <v>2969</v>
+      </c>
+      <c r="OK18" s="6">
+        <f t="shared" si="1"/>
+        <v>2979</v>
+      </c>
     </row>
-    <row r="19" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -72147,12 +73302,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:OD34"/>
+  <dimension ref="A1:OK34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="NV1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="OA1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="NX2" sqref="NX2:OD18"/>
+      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72170,7 +73325,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -73353,8 +74508,29 @@
       <c r="OD1" s="8">
         <v>44327</v>
       </c>
+      <c r="OE1" s="8">
+        <v>44328</v>
+      </c>
+      <c r="OF1" s="8">
+        <v>44329</v>
+      </c>
+      <c r="OG1" s="8">
+        <v>44330</v>
+      </c>
+      <c r="OH1" s="8">
+        <v>44331</v>
+      </c>
+      <c r="OI1" s="8">
+        <v>44332</v>
+      </c>
+      <c r="OJ1" s="8">
+        <v>44333</v>
+      </c>
+      <c r="OK1" s="8">
+        <v>44334</v>
+      </c>
     </row>
-    <row r="2" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -74650,8 +75826,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD2-'UCI OCUPADA COVID'!OD2</f>
         <v>6</v>
       </c>
+      <c r="OE2">
+        <f>+'UCI OCUPADA TOTAL'!OE2-'UCI OCUPADA COVID'!OE2</f>
+        <v>8</v>
+      </c>
+      <c r="OF2">
+        <f>+'UCI OCUPADA TOTAL'!OF2-'UCI OCUPADA COVID'!OF2</f>
+        <v>6</v>
+      </c>
+      <c r="OG2">
+        <f>+'UCI OCUPADA TOTAL'!OG2-'UCI OCUPADA COVID'!OG2</f>
+        <v>6</v>
+      </c>
+      <c r="OH2">
+        <f>+'UCI OCUPADA TOTAL'!OH2-'UCI OCUPADA COVID'!OH2</f>
+        <v>8</v>
+      </c>
+      <c r="OI2">
+        <f>+'UCI OCUPADA TOTAL'!OI2-'UCI OCUPADA COVID'!OI2</f>
+        <v>9</v>
+      </c>
+      <c r="OJ2">
+        <f>+'UCI OCUPADA TOTAL'!OJ2-'UCI OCUPADA COVID'!OJ2</f>
+        <v>8</v>
+      </c>
+      <c r="OK2">
+        <f>+'UCI OCUPADA TOTAL'!OK2-'UCI OCUPADA COVID'!OK2</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -75947,8 +77151,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD3-'UCI OCUPADA COVID'!OD3</f>
         <v>3</v>
       </c>
+      <c r="OE3">
+        <f>+'UCI OCUPADA TOTAL'!OE3-'UCI OCUPADA COVID'!OE3</f>
+        <v>4</v>
+      </c>
+      <c r="OF3">
+        <f>+'UCI OCUPADA TOTAL'!OF3-'UCI OCUPADA COVID'!OF3</f>
+        <v>3</v>
+      </c>
+      <c r="OG3">
+        <f>+'UCI OCUPADA TOTAL'!OG3-'UCI OCUPADA COVID'!OG3</f>
+        <v>2</v>
+      </c>
+      <c r="OH3">
+        <f>+'UCI OCUPADA TOTAL'!OH3-'UCI OCUPADA COVID'!OH3</f>
+        <v>2</v>
+      </c>
+      <c r="OI3">
+        <f>+'UCI OCUPADA TOTAL'!OI3-'UCI OCUPADA COVID'!OI3</f>
+        <v>1</v>
+      </c>
+      <c r="OJ3">
+        <f>+'UCI OCUPADA TOTAL'!OJ3-'UCI OCUPADA COVID'!OJ3</f>
+        <v>6</v>
+      </c>
+      <c r="OK3">
+        <f>+'UCI OCUPADA TOTAL'!OK3-'UCI OCUPADA COVID'!OK3</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -77244,8 +78476,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD4-'UCI OCUPADA COVID'!OD4</f>
         <v>57</v>
       </c>
+      <c r="OE4">
+        <f>+'UCI OCUPADA TOTAL'!OE4-'UCI OCUPADA COVID'!OE4</f>
+        <v>52</v>
+      </c>
+      <c r="OF4">
+        <f>+'UCI OCUPADA TOTAL'!OF4-'UCI OCUPADA COVID'!OF4</f>
+        <v>64</v>
+      </c>
+      <c r="OG4">
+        <f>+'UCI OCUPADA TOTAL'!OG4-'UCI OCUPADA COVID'!OG4</f>
+        <v>56</v>
+      </c>
+      <c r="OH4">
+        <f>+'UCI OCUPADA TOTAL'!OH4-'UCI OCUPADA COVID'!OH4</f>
+        <v>67</v>
+      </c>
+      <c r="OI4">
+        <f>+'UCI OCUPADA TOTAL'!OI4-'UCI OCUPADA COVID'!OI4</f>
+        <v>65</v>
+      </c>
+      <c r="OJ4">
+        <f>+'UCI OCUPADA TOTAL'!OJ4-'UCI OCUPADA COVID'!OJ4</f>
+        <v>64</v>
+      </c>
+      <c r="OK4">
+        <f>+'UCI OCUPADA TOTAL'!OK4-'UCI OCUPADA COVID'!OK4</f>
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -78541,8 +79801,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD5-'UCI OCUPADA COVID'!OD5</f>
         <v>11</v>
       </c>
+      <c r="OE5">
+        <f>+'UCI OCUPADA TOTAL'!OE5-'UCI OCUPADA COVID'!OE5</f>
+        <v>9</v>
+      </c>
+      <c r="OF5">
+        <f>+'UCI OCUPADA TOTAL'!OF5-'UCI OCUPADA COVID'!OF5</f>
+        <v>11</v>
+      </c>
+      <c r="OG5">
+        <f>+'UCI OCUPADA TOTAL'!OG5-'UCI OCUPADA COVID'!OG5</f>
+        <v>9</v>
+      </c>
+      <c r="OH5">
+        <f>+'UCI OCUPADA TOTAL'!OH5-'UCI OCUPADA COVID'!OH5</f>
+        <v>9</v>
+      </c>
+      <c r="OI5">
+        <f>+'UCI OCUPADA TOTAL'!OI5-'UCI OCUPADA COVID'!OI5</f>
+        <v>6</v>
+      </c>
+      <c r="OJ5">
+        <f>+'UCI OCUPADA TOTAL'!OJ5-'UCI OCUPADA COVID'!OJ5</f>
+        <v>5</v>
+      </c>
+      <c r="OK5">
+        <f>+'UCI OCUPADA TOTAL'!OK5-'UCI OCUPADA COVID'!OK5</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -79838,8 +81126,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD6-'UCI OCUPADA COVID'!OD6</f>
         <v>31</v>
       </c>
+      <c r="OE6">
+        <f>+'UCI OCUPADA TOTAL'!OE6-'UCI OCUPADA COVID'!OE6</f>
+        <v>33</v>
+      </c>
+      <c r="OF6">
+        <f>+'UCI OCUPADA TOTAL'!OF6-'UCI OCUPADA COVID'!OF6</f>
+        <v>34</v>
+      </c>
+      <c r="OG6">
+        <f>+'UCI OCUPADA TOTAL'!OG6-'UCI OCUPADA COVID'!OG6</f>
+        <v>30</v>
+      </c>
+      <c r="OH6">
+        <f>+'UCI OCUPADA TOTAL'!OH6-'UCI OCUPADA COVID'!OH6</f>
+        <v>32</v>
+      </c>
+      <c r="OI6">
+        <f>+'UCI OCUPADA TOTAL'!OI6-'UCI OCUPADA COVID'!OI6</f>
+        <v>30</v>
+      </c>
+      <c r="OJ6">
+        <f>+'UCI OCUPADA TOTAL'!OJ6-'UCI OCUPADA COVID'!OJ6</f>
+        <v>32</v>
+      </c>
+      <c r="OK6">
+        <f>+'UCI OCUPADA TOTAL'!OK6-'UCI OCUPADA COVID'!OK6</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="7" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -81135,8 +82451,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD7-'UCI OCUPADA COVID'!OD7</f>
         <v>83</v>
       </c>
+      <c r="OE7">
+        <f>+'UCI OCUPADA TOTAL'!OE7-'UCI OCUPADA COVID'!OE7</f>
+        <v>79</v>
+      </c>
+      <c r="OF7">
+        <f>+'UCI OCUPADA TOTAL'!OF7-'UCI OCUPADA COVID'!OF7</f>
+        <v>88</v>
+      </c>
+      <c r="OG7">
+        <f>+'UCI OCUPADA TOTAL'!OG7-'UCI OCUPADA COVID'!OG7</f>
+        <v>102</v>
+      </c>
+      <c r="OH7">
+        <f>+'UCI OCUPADA TOTAL'!OH7-'UCI OCUPADA COVID'!OH7</f>
+        <v>100</v>
+      </c>
+      <c r="OI7">
+        <f>+'UCI OCUPADA TOTAL'!OI7-'UCI OCUPADA COVID'!OI7</f>
+        <v>95</v>
+      </c>
+      <c r="OJ7">
+        <f>+'UCI OCUPADA TOTAL'!OJ7-'UCI OCUPADA COVID'!OJ7</f>
+        <v>96</v>
+      </c>
+      <c r="OK7">
+        <f>+'UCI OCUPADA TOTAL'!OK7-'UCI OCUPADA COVID'!OK7</f>
+        <v>92</v>
+      </c>
     </row>
-    <row r="8" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -82432,8 +83776,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD8-'UCI OCUPADA COVID'!OD8</f>
         <v>664</v>
       </c>
+      <c r="OE8">
+        <f>+'UCI OCUPADA TOTAL'!OE8-'UCI OCUPADA COVID'!OE8</f>
+        <v>671</v>
+      </c>
+      <c r="OF8">
+        <f>+'UCI OCUPADA TOTAL'!OF8-'UCI OCUPADA COVID'!OF8</f>
+        <v>688</v>
+      </c>
+      <c r="OG8">
+        <f>+'UCI OCUPADA TOTAL'!OG8-'UCI OCUPADA COVID'!OG8</f>
+        <v>704</v>
+      </c>
+      <c r="OH8">
+        <f>+'UCI OCUPADA TOTAL'!OH8-'UCI OCUPADA COVID'!OH8</f>
+        <v>694</v>
+      </c>
+      <c r="OI8">
+        <f>+'UCI OCUPADA TOTAL'!OI8-'UCI OCUPADA COVID'!OI8</f>
+        <v>705</v>
+      </c>
+      <c r="OJ8">
+        <f>+'UCI OCUPADA TOTAL'!OJ8-'UCI OCUPADA COVID'!OJ8</f>
+        <v>699</v>
+      </c>
+      <c r="OK8">
+        <f>+'UCI OCUPADA TOTAL'!OK8-'UCI OCUPADA COVID'!OK8</f>
+        <v>701</v>
+      </c>
     </row>
-    <row r="9" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -83729,8 +85101,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD9-'UCI OCUPADA COVID'!OD9</f>
         <v>42</v>
       </c>
+      <c r="OE9">
+        <f>+'UCI OCUPADA TOTAL'!OE9-'UCI OCUPADA COVID'!OE9</f>
+        <v>37</v>
+      </c>
+      <c r="OF9">
+        <f>+'UCI OCUPADA TOTAL'!OF9-'UCI OCUPADA COVID'!OF9</f>
+        <v>32</v>
+      </c>
+      <c r="OG9">
+        <f>+'UCI OCUPADA TOTAL'!OG9-'UCI OCUPADA COVID'!OG9</f>
+        <v>44</v>
+      </c>
+      <c r="OH9">
+        <f>+'UCI OCUPADA TOTAL'!OH9-'UCI OCUPADA COVID'!OH9</f>
+        <v>48</v>
+      </c>
+      <c r="OI9">
+        <f>+'UCI OCUPADA TOTAL'!OI9-'UCI OCUPADA COVID'!OI9</f>
+        <v>40</v>
+      </c>
+      <c r="OJ9">
+        <f>+'UCI OCUPADA TOTAL'!OJ9-'UCI OCUPADA COVID'!OJ9</f>
+        <v>44</v>
+      </c>
+      <c r="OK9">
+        <f>+'UCI OCUPADA TOTAL'!OK9-'UCI OCUPADA COVID'!OK9</f>
+        <v>47</v>
+      </c>
     </row>
-    <row r="10" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -85026,8 +86426,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD10-'UCI OCUPADA COVID'!OD10</f>
         <v>24</v>
       </c>
+      <c r="OE10">
+        <f>+'UCI OCUPADA TOTAL'!OE10-'UCI OCUPADA COVID'!OE10</f>
+        <v>24</v>
+      </c>
+      <c r="OF10">
+        <f>+'UCI OCUPADA TOTAL'!OF10-'UCI OCUPADA COVID'!OF10</f>
+        <v>24</v>
+      </c>
+      <c r="OG10">
+        <f>+'UCI OCUPADA TOTAL'!OG10-'UCI OCUPADA COVID'!OG10</f>
+        <v>25</v>
+      </c>
+      <c r="OH10">
+        <f>+'UCI OCUPADA TOTAL'!OH10-'UCI OCUPADA COVID'!OH10</f>
+        <v>24</v>
+      </c>
+      <c r="OI10">
+        <f>+'UCI OCUPADA TOTAL'!OI10-'UCI OCUPADA COVID'!OI10</f>
+        <v>23</v>
+      </c>
+      <c r="OJ10">
+        <f>+'UCI OCUPADA TOTAL'!OJ10-'UCI OCUPADA COVID'!OJ10</f>
+        <v>26</v>
+      </c>
+      <c r="OK10">
+        <f>+'UCI OCUPADA TOTAL'!OK10-'UCI OCUPADA COVID'!OK10</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="11" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -86323,8 +87751,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD11-'UCI OCUPADA COVID'!OD11</f>
         <v>14</v>
       </c>
+      <c r="OE11">
+        <f>+'UCI OCUPADA TOTAL'!OE11-'UCI OCUPADA COVID'!OE11</f>
+        <v>15</v>
+      </c>
+      <c r="OF11">
+        <f>+'UCI OCUPADA TOTAL'!OF11-'UCI OCUPADA COVID'!OF11</f>
+        <v>15</v>
+      </c>
+      <c r="OG11">
+        <f>+'UCI OCUPADA TOTAL'!OG11-'UCI OCUPADA COVID'!OG11</f>
+        <v>12</v>
+      </c>
+      <c r="OH11">
+        <f>+'UCI OCUPADA TOTAL'!OH11-'UCI OCUPADA COVID'!OH11</f>
+        <v>11</v>
+      </c>
+      <c r="OI11">
+        <f>+'UCI OCUPADA TOTAL'!OI11-'UCI OCUPADA COVID'!OI11</f>
+        <v>13</v>
+      </c>
+      <c r="OJ11">
+        <f>+'UCI OCUPADA TOTAL'!OJ11-'UCI OCUPADA COVID'!OJ11</f>
+        <v>12</v>
+      </c>
+      <c r="OK11">
+        <f>+'UCI OCUPADA TOTAL'!OK11-'UCI OCUPADA COVID'!OK11</f>
+        <v>14</v>
+      </c>
     </row>
-    <row r="12" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -87620,8 +89076,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD12-'UCI OCUPADA COVID'!OD12</f>
         <v>85</v>
       </c>
+      <c r="OE12">
+        <f>+'UCI OCUPADA TOTAL'!OE12-'UCI OCUPADA COVID'!OE12</f>
+        <v>90</v>
+      </c>
+      <c r="OF12">
+        <f>+'UCI OCUPADA TOTAL'!OF12-'UCI OCUPADA COVID'!OF12</f>
+        <v>92</v>
+      </c>
+      <c r="OG12">
+        <f>+'UCI OCUPADA TOTAL'!OG12-'UCI OCUPADA COVID'!OG12</f>
+        <v>91</v>
+      </c>
+      <c r="OH12">
+        <f>+'UCI OCUPADA TOTAL'!OH12-'UCI OCUPADA COVID'!OH12</f>
+        <v>90</v>
+      </c>
+      <c r="OI12">
+        <f>+'UCI OCUPADA TOTAL'!OI12-'UCI OCUPADA COVID'!OI12</f>
+        <v>88</v>
+      </c>
+      <c r="OJ12">
+        <f>+'UCI OCUPADA TOTAL'!OJ12-'UCI OCUPADA COVID'!OJ12</f>
+        <v>88</v>
+      </c>
+      <c r="OK12">
+        <f>+'UCI OCUPADA TOTAL'!OK12-'UCI OCUPADA COVID'!OK12</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="13" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -88917,8 +90401,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD13-'UCI OCUPADA COVID'!OD13</f>
         <v>33</v>
       </c>
+      <c r="OE13">
+        <f>+'UCI OCUPADA TOTAL'!OE13-'UCI OCUPADA COVID'!OE13</f>
+        <v>33</v>
+      </c>
+      <c r="OF13">
+        <f>+'UCI OCUPADA TOTAL'!OF13-'UCI OCUPADA COVID'!OF13</f>
+        <v>35</v>
+      </c>
+      <c r="OG13">
+        <f>+'UCI OCUPADA TOTAL'!OG13-'UCI OCUPADA COVID'!OG13</f>
+        <v>31</v>
+      </c>
+      <c r="OH13">
+        <f>+'UCI OCUPADA TOTAL'!OH13-'UCI OCUPADA COVID'!OH13</f>
+        <v>31</v>
+      </c>
+      <c r="OI13">
+        <f>+'UCI OCUPADA TOTAL'!OI13-'UCI OCUPADA COVID'!OI13</f>
+        <v>31</v>
+      </c>
+      <c r="OJ13">
+        <f>+'UCI OCUPADA TOTAL'!OJ13-'UCI OCUPADA COVID'!OJ13</f>
+        <v>34</v>
+      </c>
+      <c r="OK13">
+        <f>+'UCI OCUPADA TOTAL'!OK13-'UCI OCUPADA COVID'!OK13</f>
+        <v>34</v>
+      </c>
     </row>
-    <row r="14" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -90214,8 +91726,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD14-'UCI OCUPADA COVID'!OD14</f>
         <v>12</v>
       </c>
+      <c r="OE14">
+        <f>+'UCI OCUPADA TOTAL'!OE14-'UCI OCUPADA COVID'!OE14</f>
+        <v>12</v>
+      </c>
+      <c r="OF14">
+        <f>+'UCI OCUPADA TOTAL'!OF14-'UCI OCUPADA COVID'!OF14</f>
+        <v>15</v>
+      </c>
+      <c r="OG14">
+        <f>+'UCI OCUPADA TOTAL'!OG14-'UCI OCUPADA COVID'!OG14</f>
+        <v>16</v>
+      </c>
+      <c r="OH14">
+        <f>+'UCI OCUPADA TOTAL'!OH14-'UCI OCUPADA COVID'!OH14</f>
+        <v>17</v>
+      </c>
+      <c r="OI14">
+        <f>+'UCI OCUPADA TOTAL'!OI14-'UCI OCUPADA COVID'!OI14</f>
+        <v>18</v>
+      </c>
+      <c r="OJ14">
+        <f>+'UCI OCUPADA TOTAL'!OJ14-'UCI OCUPADA COVID'!OJ14</f>
+        <v>19</v>
+      </c>
+      <c r="OK14">
+        <f>+'UCI OCUPADA TOTAL'!OK14-'UCI OCUPADA COVID'!OK14</f>
+        <v>18</v>
+      </c>
     </row>
-    <row r="15" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -91511,8 +93051,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD15-'UCI OCUPADA COVID'!OD15</f>
         <v>35</v>
       </c>
+      <c r="OE15">
+        <f>+'UCI OCUPADA TOTAL'!OE15-'UCI OCUPADA COVID'!OE15</f>
+        <v>42</v>
+      </c>
+      <c r="OF15">
+        <f>+'UCI OCUPADA TOTAL'!OF15-'UCI OCUPADA COVID'!OF15</f>
+        <v>43</v>
+      </c>
+      <c r="OG15">
+        <f>+'UCI OCUPADA TOTAL'!OG15-'UCI OCUPADA COVID'!OG15</f>
+        <v>48</v>
+      </c>
+      <c r="OH15">
+        <f>+'UCI OCUPADA TOTAL'!OH15-'UCI OCUPADA COVID'!OH15</f>
+        <v>47</v>
+      </c>
+      <c r="OI15">
+        <f>+'UCI OCUPADA TOTAL'!OI15-'UCI OCUPADA COVID'!OI15</f>
+        <v>46</v>
+      </c>
+      <c r="OJ15">
+        <f>+'UCI OCUPADA TOTAL'!OJ15-'UCI OCUPADA COVID'!OJ15</f>
+        <v>44</v>
+      </c>
+      <c r="OK15">
+        <f>+'UCI OCUPADA TOTAL'!OK15-'UCI OCUPADA COVID'!OK15</f>
+        <v>43</v>
+      </c>
     </row>
-    <row r="16" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -92808,8 +94376,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD16-'UCI OCUPADA COVID'!OD16</f>
         <v>1</v>
       </c>
+      <c r="OE16">
+        <f>+'UCI OCUPADA TOTAL'!OE16-'UCI OCUPADA COVID'!OE16</f>
+        <v>3</v>
+      </c>
+      <c r="OF16">
+        <f>+'UCI OCUPADA TOTAL'!OF16-'UCI OCUPADA COVID'!OF16</f>
+        <v>3</v>
+      </c>
+      <c r="OG16">
+        <f>+'UCI OCUPADA TOTAL'!OG16-'UCI OCUPADA COVID'!OG16</f>
+        <v>4</v>
+      </c>
+      <c r="OH16">
+        <f>+'UCI OCUPADA TOTAL'!OH16-'UCI OCUPADA COVID'!OH16</f>
+        <v>4</v>
+      </c>
+      <c r="OI16">
+        <f>+'UCI OCUPADA TOTAL'!OI16-'UCI OCUPADA COVID'!OI16</f>
+        <v>4</v>
+      </c>
+      <c r="OJ16">
+        <f>+'UCI OCUPADA TOTAL'!OJ16-'UCI OCUPADA COVID'!OJ16</f>
+        <v>4</v>
+      </c>
+      <c r="OK16">
+        <f>+'UCI OCUPADA TOTAL'!OK16-'UCI OCUPADA COVID'!OK16</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="17" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -94105,8 +95701,36 @@
         <f>+'UCI OCUPADA TOTAL'!OD17-'UCI OCUPADA COVID'!OD17</f>
         <v>9</v>
       </c>
+      <c r="OE17">
+        <f>+'UCI OCUPADA TOTAL'!OE17-'UCI OCUPADA COVID'!OE17</f>
+        <v>10</v>
+      </c>
+      <c r="OF17">
+        <f>+'UCI OCUPADA TOTAL'!OF17-'UCI OCUPADA COVID'!OF17</f>
+        <v>9</v>
+      </c>
+      <c r="OG17">
+        <f>+'UCI OCUPADA TOTAL'!OG17-'UCI OCUPADA COVID'!OG17</f>
+        <v>8</v>
+      </c>
+      <c r="OH17">
+        <f>+'UCI OCUPADA TOTAL'!OH17-'UCI OCUPADA COVID'!OH17</f>
+        <v>10</v>
+      </c>
+      <c r="OI17">
+        <f>+'UCI OCUPADA TOTAL'!OI17-'UCI OCUPADA COVID'!OI17</f>
+        <v>11</v>
+      </c>
+      <c r="OJ17">
+        <f>+'UCI OCUPADA TOTAL'!OJ17-'UCI OCUPADA COVID'!OJ17</f>
+        <v>10</v>
+      </c>
+      <c r="OK17">
+        <f>+'UCI OCUPADA TOTAL'!OK17-'UCI OCUPADA COVID'!OK17</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -95402,48 +97026,76 @@
         <f>+'UCI OCUPADA TOTAL'!OD18-'UCI OCUPADA COVID'!OD18</f>
         <v>1110</v>
       </c>
+      <c r="OE18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OE18-'UCI OCUPADA COVID'!OE18</f>
+        <v>1122</v>
+      </c>
+      <c r="OF18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OF18-'UCI OCUPADA COVID'!OF18</f>
+        <v>1162</v>
+      </c>
+      <c r="OG18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OG18-'UCI OCUPADA COVID'!OG18</f>
+        <v>1188</v>
+      </c>
+      <c r="OH18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OH18-'UCI OCUPADA COVID'!OH18</f>
+        <v>1194</v>
+      </c>
+      <c r="OI18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OI18-'UCI OCUPADA COVID'!OI18</f>
+        <v>1185</v>
+      </c>
+      <c r="OJ18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OJ18-'UCI OCUPADA COVID'!OJ18</f>
+        <v>1191</v>
+      </c>
+      <c r="OK18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OK18-'UCI OCUPADA COVID'!OK18</f>
+        <v>1187</v>
+      </c>
     </row>
-    <row r="19" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:394" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
camas uci, Mayo 25 2021
Signed-off-by: dna33 <Cruzado1982>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -2911,9 +2911,9 @@
   <dimension ref="A1:XFD20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OB1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
+      <selection pane="topRight" activeCell="OL1" sqref="OL1:OR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4139,8 +4139,29 @@
       <c r="OK1" s="8">
         <v>44334</v>
       </c>
+      <c r="OL1" s="8">
+        <v>44335</v>
+      </c>
+      <c r="OM1" s="8">
+        <v>44336</v>
+      </c>
+      <c r="ON1" s="8">
+        <v>44337</v>
+      </c>
+      <c r="OO1" s="8">
+        <v>44338</v>
+      </c>
+      <c r="OP1" s="8">
+        <v>44339</v>
+      </c>
+      <c r="OQ1" s="8">
+        <v>44340</v>
+      </c>
+      <c r="OR1" s="8">
+        <v>44341</v>
+      </c>
     </row>
-    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5344,8 +5365,29 @@
       <c r="OK2" s="11">
         <v>40</v>
       </c>
+      <c r="OL2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OM2" s="11">
+        <v>40</v>
+      </c>
+      <c r="ON2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OO2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OP2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OQ2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OR2" s="11">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6549,8 +6591,29 @@
       <c r="OK3" s="11">
         <v>62</v>
       </c>
+      <c r="OL3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OM3" s="11">
+        <v>62</v>
+      </c>
+      <c r="ON3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OO3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OP3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OQ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OR3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7754,8 +7817,29 @@
       <c r="OK4" s="11">
         <v>163</v>
       </c>
+      <c r="OL4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OM4" s="11">
+        <v>163</v>
+      </c>
+      <c r="ON4" s="11">
+        <v>163</v>
+      </c>
+      <c r="OO4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OP4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OQ4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OR4" s="11">
+        <v>164</v>
+      </c>
     </row>
-    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -8959,8 +9043,29 @@
       <c r="OK5" s="11">
         <v>34</v>
       </c>
+      <c r="OL5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OM5" s="11">
+        <v>34</v>
+      </c>
+      <c r="ON5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OO5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OP5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OQ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OR5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10164,8 +10269,29 @@
       <c r="OK6" s="11">
         <v>134</v>
       </c>
+      <c r="OL6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OM6" s="11">
+        <v>134</v>
+      </c>
+      <c r="ON6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OO6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OP6" s="11">
+        <v>133</v>
+      </c>
+      <c r="OQ6" s="11">
+        <v>133</v>
+      </c>
+      <c r="OR6" s="11">
+        <v>132</v>
+      </c>
     </row>
-    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -11369,8 +11495,29 @@
       <c r="OK7" s="11">
         <v>334</v>
       </c>
+      <c r="OL7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OM7" s="11">
+        <v>334</v>
+      </c>
+      <c r="ON7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OO7" s="11">
+        <v>334</v>
+      </c>
+      <c r="OP7" s="11">
+        <v>332</v>
+      </c>
+      <c r="OQ7" s="11">
+        <v>330</v>
+      </c>
+      <c r="OR7" s="11">
+        <v>329</v>
+      </c>
     </row>
-    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12574,8 +12721,29 @@
       <c r="OK8" s="11">
         <v>2593</v>
       </c>
+      <c r="OL8" s="11">
+        <v>2589</v>
+      </c>
+      <c r="OM8" s="11">
+        <v>2591</v>
+      </c>
+      <c r="ON8" s="11">
+        <v>2588</v>
+      </c>
+      <c r="OO8" s="11">
+        <v>2580</v>
+      </c>
+      <c r="OP8" s="11">
+        <v>2577</v>
+      </c>
+      <c r="OQ8" s="11">
+        <v>2576</v>
+      </c>
+      <c r="OR8" s="11">
+        <v>2577</v>
+      </c>
     </row>
-    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13779,8 +13947,29 @@
       <c r="OK9" s="11">
         <v>206</v>
       </c>
+      <c r="OL9" s="11">
+        <v>203</v>
+      </c>
+      <c r="OM9" s="11">
+        <v>206</v>
+      </c>
+      <c r="ON9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OO9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OP9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OQ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OR9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -14984,8 +15173,29 @@
       <c r="OK10" s="11">
         <v>162</v>
       </c>
+      <c r="OL10" s="11">
+        <v>142</v>
+      </c>
+      <c r="OM10" s="11">
+        <v>142</v>
+      </c>
+      <c r="ON10" s="11">
+        <v>147</v>
+      </c>
+      <c r="OO10" s="11">
+        <v>146</v>
+      </c>
+      <c r="OP10" s="11">
+        <v>137</v>
+      </c>
+      <c r="OQ10" s="11">
+        <v>138</v>
+      </c>
+      <c r="OR10" s="11">
+        <v>138</v>
+      </c>
     </row>
-    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -16189,8 +16399,29 @@
       <c r="OK11" s="11">
         <v>73</v>
       </c>
+      <c r="OL11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OM11" s="11">
+        <v>73</v>
+      </c>
+      <c r="ON11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OO11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OP11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OQ11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OR11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -17394,8 +17625,29 @@
       <c r="OK12" s="11">
         <v>310</v>
       </c>
+      <c r="OL12" s="11">
+        <v>310</v>
+      </c>
+      <c r="OM12" s="11">
+        <v>310</v>
+      </c>
+      <c r="ON12" s="11">
+        <v>304</v>
+      </c>
+      <c r="OO12" s="11">
+        <v>307</v>
+      </c>
+      <c r="OP12" s="11">
+        <v>307</v>
+      </c>
+      <c r="OQ12" s="11">
+        <v>307</v>
+      </c>
+      <c r="OR12" s="11">
+        <v>306</v>
+      </c>
     </row>
-    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -18599,8 +18851,29 @@
       <c r="OK13" s="11">
         <v>145</v>
       </c>
+      <c r="OL13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OM13" s="11">
+        <v>150</v>
+      </c>
+      <c r="ON13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OO13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OP13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OQ13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OR13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -19804,8 +20077,29 @@
       <c r="OK14" s="11">
         <v>41</v>
       </c>
+      <c r="OL14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OM14" s="11">
+        <v>41</v>
+      </c>
+      <c r="ON14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OO14" s="11">
+        <v>39</v>
+      </c>
+      <c r="OP14" s="11">
+        <v>39</v>
+      </c>
+      <c r="OQ14" s="11">
+        <v>39</v>
+      </c>
+      <c r="OR14" s="11">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -21009,8 +21303,29 @@
       <c r="OK15" s="11">
         <v>126</v>
       </c>
+      <c r="OL15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OM15" s="11">
+        <v>126</v>
+      </c>
+      <c r="ON15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OO15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OP15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OQ15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OR15" s="11">
+        <v>126</v>
+      </c>
     </row>
-    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -22214,8 +22529,29 @@
       <c r="OK16" s="11">
         <v>10</v>
       </c>
+      <c r="OL16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OM16" s="11">
+        <v>10</v>
+      </c>
+      <c r="ON16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OO16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OP16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OQ16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OR16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -23419,8 +23755,29 @@
       <c r="OK17" s="11">
         <v>48</v>
       </c>
+      <c r="OL17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OM17" s="11">
+        <v>47</v>
+      </c>
+      <c r="ON17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OO17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OP17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OQ17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OR17" s="11">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -24596,7 +24953,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:OK18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:OR18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -24751,9 +25108,37 @@
         <f t="shared" si="7"/>
         <v>4481</v>
       </c>
+      <c r="OL18" s="6">
+        <f t="shared" si="7"/>
+        <v>4459</v>
+      </c>
+      <c r="OM18" s="6">
+        <f t="shared" si="7"/>
+        <v>4463</v>
+      </c>
+      <c r="ON18" s="6">
+        <f t="shared" si="7"/>
+        <v>4459</v>
+      </c>
+      <c r="OO18" s="6">
+        <f t="shared" si="7"/>
+        <v>4453</v>
+      </c>
+      <c r="OP18" s="6">
+        <f t="shared" si="7"/>
+        <v>4438</v>
+      </c>
+      <c r="OQ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4435</v>
+      </c>
+      <c r="OR18" s="6">
+        <f t="shared" si="7"/>
+        <v>4435</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:401 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -24771,12 +25156,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OK36"/>
+  <dimension ref="A1:OR36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OB1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
+      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24796,7 +25181,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -26000,8 +26385,29 @@
       <c r="OK1" s="8">
         <v>44334</v>
       </c>
+      <c r="OL1" s="8">
+        <v>44335</v>
+      </c>
+      <c r="OM1" s="8">
+        <v>44336</v>
+      </c>
+      <c r="ON1" s="8">
+        <v>44337</v>
+      </c>
+      <c r="OO1" s="8">
+        <v>44338</v>
+      </c>
+      <c r="OP1" s="8">
+        <v>44339</v>
+      </c>
+      <c r="OQ1" s="8">
+        <v>44340</v>
+      </c>
+      <c r="OR1" s="8">
+        <v>44341</v>
+      </c>
     </row>
-    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -27205,8 +27611,29 @@
       <c r="OK2">
         <v>34</v>
       </c>
+      <c r="OL2">
+        <v>35</v>
+      </c>
+      <c r="OM2">
+        <v>34</v>
+      </c>
+      <c r="ON2">
+        <v>36</v>
+      </c>
+      <c r="OO2">
+        <v>35</v>
+      </c>
+      <c r="OP2">
+        <v>34</v>
+      </c>
+      <c r="OQ2">
+        <v>35</v>
+      </c>
+      <c r="OR2">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -28410,8 +28837,29 @@
       <c r="OK3">
         <v>56</v>
       </c>
+      <c r="OL3">
+        <v>54</v>
+      </c>
+      <c r="OM3">
+        <v>52</v>
+      </c>
+      <c r="ON3">
+        <v>52</v>
+      </c>
+      <c r="OO3">
+        <v>54</v>
+      </c>
+      <c r="OP3">
+        <v>54</v>
+      </c>
+      <c r="OQ3">
+        <v>59</v>
+      </c>
+      <c r="OR3">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -29615,8 +30063,29 @@
       <c r="OK4">
         <v>152</v>
       </c>
+      <c r="OL4">
+        <v>154</v>
+      </c>
+      <c r="OM4">
+        <v>154</v>
+      </c>
+      <c r="ON4">
+        <v>154</v>
+      </c>
+      <c r="OO4">
+        <v>152</v>
+      </c>
+      <c r="OP4">
+        <v>154</v>
+      </c>
+      <c r="OQ4">
+        <v>154</v>
+      </c>
+      <c r="OR4">
+        <v>155</v>
+      </c>
     </row>
-    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -30820,8 +31289,29 @@
       <c r="OK5">
         <v>30</v>
       </c>
+      <c r="OL5">
+        <v>30</v>
+      </c>
+      <c r="OM5">
+        <v>29</v>
+      </c>
+      <c r="ON5">
+        <v>29</v>
+      </c>
+      <c r="OO5">
+        <v>31</v>
+      </c>
+      <c r="OP5">
+        <v>30</v>
+      </c>
+      <c r="OQ5">
+        <v>28</v>
+      </c>
+      <c r="OR5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -32025,8 +32515,29 @@
       <c r="OK6">
         <v>125</v>
       </c>
+      <c r="OL6">
+        <v>131</v>
+      </c>
+      <c r="OM6">
+        <v>126</v>
+      </c>
+      <c r="ON6">
+        <v>124</v>
+      </c>
+      <c r="OO6">
+        <v>128</v>
+      </c>
+      <c r="OP6">
+        <v>130</v>
+      </c>
+      <c r="OQ6">
+        <v>130</v>
+      </c>
+      <c r="OR6">
+        <v>127</v>
+      </c>
     </row>
-    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -33230,8 +33741,29 @@
       <c r="OK7">
         <v>314</v>
       </c>
+      <c r="OL7">
+        <v>318</v>
+      </c>
+      <c r="OM7">
+        <v>310</v>
+      </c>
+      <c r="ON7">
+        <v>313</v>
+      </c>
+      <c r="OO7">
+        <v>313</v>
+      </c>
+      <c r="OP7">
+        <v>312</v>
+      </c>
+      <c r="OQ7">
+        <v>317</v>
+      </c>
+      <c r="OR7">
+        <v>321</v>
+      </c>
     </row>
-    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -34435,8 +34967,29 @@
       <c r="OK8">
         <v>2488</v>
       </c>
+      <c r="OL8">
+        <v>2478</v>
+      </c>
+      <c r="OM8">
+        <v>2483</v>
+      </c>
+      <c r="ON8">
+        <v>2487</v>
+      </c>
+      <c r="OO8">
+        <v>2489</v>
+      </c>
+      <c r="OP8">
+        <v>2508</v>
+      </c>
+      <c r="OQ8">
+        <v>2518</v>
+      </c>
+      <c r="OR8">
+        <v>2518</v>
+      </c>
     </row>
-    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -35640,8 +36193,29 @@
       <c r="OK9">
         <v>162</v>
       </c>
+      <c r="OL9">
+        <v>164</v>
+      </c>
+      <c r="OM9">
+        <v>167</v>
+      </c>
+      <c r="ON9">
+        <v>169</v>
+      </c>
+      <c r="OO9">
+        <v>164</v>
+      </c>
+      <c r="OP9">
+        <v>171</v>
+      </c>
+      <c r="OQ9">
+        <v>169</v>
+      </c>
+      <c r="OR9">
+        <v>175</v>
+      </c>
     </row>
-    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -36845,8 +37419,29 @@
       <c r="OK10">
         <v>132</v>
       </c>
+      <c r="OL10">
+        <v>126</v>
+      </c>
+      <c r="OM10">
+        <v>130</v>
+      </c>
+      <c r="ON10">
+        <v>131</v>
+      </c>
+      <c r="OO10">
+        <v>137</v>
+      </c>
+      <c r="OP10">
+        <v>133</v>
+      </c>
+      <c r="OQ10">
+        <v>135</v>
+      </c>
+      <c r="OR10">
+        <v>135</v>
+      </c>
     </row>
-    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -38050,8 +38645,29 @@
       <c r="OK11">
         <v>61</v>
       </c>
+      <c r="OL11">
+        <v>64</v>
+      </c>
+      <c r="OM11">
+        <v>58</v>
+      </c>
+      <c r="ON11">
+        <v>62</v>
+      </c>
+      <c r="OO11">
+        <v>61</v>
+      </c>
+      <c r="OP11">
+        <v>63</v>
+      </c>
+      <c r="OQ11">
+        <v>65</v>
+      </c>
+      <c r="OR11">
+        <v>69</v>
+      </c>
     </row>
-    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -39255,8 +39871,29 @@
       <c r="OK12">
         <v>275</v>
       </c>
+      <c r="OL12">
+        <v>279</v>
+      </c>
+      <c r="OM12">
+        <v>272</v>
+      </c>
+      <c r="ON12">
+        <v>272</v>
+      </c>
+      <c r="OO12">
+        <v>275</v>
+      </c>
+      <c r="OP12">
+        <v>269</v>
+      </c>
+      <c r="OQ12">
+        <v>273</v>
+      </c>
+      <c r="OR12">
+        <v>278</v>
+      </c>
     </row>
-    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -40460,8 +41097,29 @@
       <c r="OK13">
         <v>133</v>
       </c>
+      <c r="OL13">
+        <v>134</v>
+      </c>
+      <c r="OM13">
+        <v>132</v>
+      </c>
+      <c r="ON13">
+        <v>132</v>
+      </c>
+      <c r="OO13">
+        <v>133</v>
+      </c>
+      <c r="OP13">
+        <v>132</v>
+      </c>
+      <c r="OQ13">
+        <v>133</v>
+      </c>
+      <c r="OR13">
+        <v>141</v>
+      </c>
     </row>
-    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -41665,8 +42323,29 @@
       <c r="OK14">
         <v>40</v>
       </c>
+      <c r="OL14">
+        <v>40</v>
+      </c>
+      <c r="OM14">
+        <v>37</v>
+      </c>
+      <c r="ON14">
+        <v>34</v>
+      </c>
+      <c r="OO14">
+        <v>38</v>
+      </c>
+      <c r="OP14">
+        <v>37</v>
+      </c>
+      <c r="OQ14">
+        <v>38</v>
+      </c>
+      <c r="OR14">
+        <v>37</v>
+      </c>
     </row>
-    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -42870,8 +43549,29 @@
       <c r="OK15">
         <v>117</v>
       </c>
+      <c r="OL15">
+        <v>121</v>
+      </c>
+      <c r="OM15">
+        <v>120</v>
+      </c>
+      <c r="ON15">
+        <v>120</v>
+      </c>
+      <c r="OO15">
+        <v>118</v>
+      </c>
+      <c r="OP15">
+        <v>116</v>
+      </c>
+      <c r="OQ15">
+        <v>117</v>
+      </c>
+      <c r="OR15">
+        <v>123</v>
+      </c>
     </row>
-    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -44075,8 +44775,29 @@
       <c r="OK16">
         <v>10</v>
       </c>
+      <c r="OL16">
+        <v>10</v>
+      </c>
+      <c r="OM16">
+        <v>10</v>
+      </c>
+      <c r="ON16">
+        <v>10</v>
+      </c>
+      <c r="OO16">
+        <v>10</v>
+      </c>
+      <c r="OP16">
+        <v>10</v>
+      </c>
+      <c r="OQ16">
+        <v>10</v>
+      </c>
+      <c r="OR16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -45280,8 +46001,29 @@
       <c r="OK17">
         <v>37</v>
       </c>
+      <c r="OL17">
+        <v>39</v>
+      </c>
+      <c r="OM17">
+        <v>41</v>
+      </c>
+      <c r="ON17">
+        <v>43</v>
+      </c>
+      <c r="OO17">
+        <v>37</v>
+      </c>
+      <c r="OP17">
+        <v>37</v>
+      </c>
+      <c r="OQ17">
+        <v>36</v>
+      </c>
+      <c r="OR17">
+        <v>40</v>
+      </c>
     </row>
-    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -46373,7 +47115,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:OK18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:OR18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -46592,8 +47334,36 @@
         <f t="shared" si="1"/>
         <v>4166</v>
       </c>
+      <c r="OL18" s="6">
+        <f t="shared" si="1"/>
+        <v>4177</v>
+      </c>
+      <c r="OM18" s="6">
+        <f t="shared" si="1"/>
+        <v>4155</v>
+      </c>
+      <c r="ON18" s="6">
+        <f t="shared" si="1"/>
+        <v>4168</v>
+      </c>
+      <c r="OO18" s="6">
+        <f t="shared" si="1"/>
+        <v>4175</v>
+      </c>
+      <c r="OP18" s="6">
+        <f t="shared" si="1"/>
+        <v>4190</v>
+      </c>
+      <c r="OQ18" s="6">
+        <f t="shared" si="1"/>
+        <v>4217</v>
+      </c>
+      <c r="OR18" s="6">
+        <f t="shared" si="1"/>
+        <v>4254</v>
+      </c>
     </row>
-    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -46876,7 +47646,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -47159,7 +47929,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -47442,7 +48212,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -47725,7 +48495,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -48008,7 +48778,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -48291,7 +49061,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -48574,7 +49344,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -48857,7 +49627,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -49140,7 +49910,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -49423,7 +50193,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -49706,7 +50476,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -49989,7 +50759,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -51412,12 +52182,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OK34"/>
+  <dimension ref="A1:OR34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OC1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
+      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51438,7 +52208,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -52642,8 +53412,29 @@
       <c r="OK1" s="8">
         <v>44334</v>
       </c>
+      <c r="OL1" s="8">
+        <v>44335</v>
+      </c>
+      <c r="OM1" s="8">
+        <v>44336</v>
+      </c>
+      <c r="ON1" s="8">
+        <v>44337</v>
+      </c>
+      <c r="OO1" s="8">
+        <v>44338</v>
+      </c>
+      <c r="OP1" s="8">
+        <v>44339</v>
+      </c>
+      <c r="OQ1" s="8">
+        <v>44340</v>
+      </c>
+      <c r="OR1" s="8">
+        <v>44341</v>
+      </c>
     </row>
-    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -53847,8 +54638,29 @@
       <c r="OK2">
         <v>27</v>
       </c>
+      <c r="OL2">
+        <v>29</v>
+      </c>
+      <c r="OM2">
+        <v>29</v>
+      </c>
+      <c r="ON2">
+        <v>29</v>
+      </c>
+      <c r="OO2">
+        <v>30</v>
+      </c>
+      <c r="OP2">
+        <v>29</v>
+      </c>
+      <c r="OQ2">
+        <v>29</v>
+      </c>
+      <c r="OR2">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -55052,8 +55864,29 @@
       <c r="OK3">
         <v>52</v>
       </c>
+      <c r="OL3">
+        <v>49</v>
+      </c>
+      <c r="OM3">
+        <v>48</v>
+      </c>
+      <c r="ON3">
+        <v>48</v>
+      </c>
+      <c r="OO3">
+        <v>49</v>
+      </c>
+      <c r="OP3">
+        <v>51</v>
+      </c>
+      <c r="OQ3">
+        <v>54</v>
+      </c>
+      <c r="OR3">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -56257,8 +57090,29 @@
       <c r="OK4">
         <v>92</v>
       </c>
+      <c r="OL4">
+        <v>93</v>
+      </c>
+      <c r="OM4">
+        <v>94</v>
+      </c>
+      <c r="ON4">
+        <v>90</v>
+      </c>
+      <c r="OO4">
+        <v>92</v>
+      </c>
+      <c r="OP4">
+        <v>91</v>
+      </c>
+      <c r="OQ4">
+        <v>92</v>
+      </c>
+      <c r="OR4">
+        <v>93</v>
+      </c>
     </row>
-    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -57462,8 +58316,29 @@
       <c r="OK5">
         <v>22</v>
       </c>
+      <c r="OL5">
+        <v>24</v>
+      </c>
+      <c r="OM5">
+        <v>24</v>
+      </c>
+      <c r="ON5">
+        <v>25</v>
+      </c>
+      <c r="OO5">
+        <v>25</v>
+      </c>
+      <c r="OP5">
+        <v>24</v>
+      </c>
+      <c r="OQ5">
+        <v>23</v>
+      </c>
+      <c r="OR5">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -58667,8 +59542,29 @@
       <c r="OK6">
         <v>94</v>
       </c>
+      <c r="OL6">
+        <v>97</v>
+      </c>
+      <c r="OM6">
+        <v>94</v>
+      </c>
+      <c r="ON6">
+        <v>95</v>
+      </c>
+      <c r="OO6">
+        <v>94</v>
+      </c>
+      <c r="OP6">
+        <v>94</v>
+      </c>
+      <c r="OQ6">
+        <v>92</v>
+      </c>
+      <c r="OR6">
+        <v>92</v>
+      </c>
     </row>
-    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -59872,8 +60768,29 @@
       <c r="OK7">
         <v>222</v>
       </c>
+      <c r="OL7">
+        <v>226</v>
+      </c>
+      <c r="OM7">
+        <v>216</v>
+      </c>
+      <c r="ON7">
+        <v>224</v>
+      </c>
+      <c r="OO7">
+        <v>219</v>
+      </c>
+      <c r="OP7">
+        <v>214</v>
+      </c>
+      <c r="OQ7">
+        <v>211</v>
+      </c>
+      <c r="OR7">
+        <v>211</v>
+      </c>
     </row>
-    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -61077,8 +61994,29 @@
       <c r="OK8">
         <v>1787</v>
       </c>
+      <c r="OL8">
+        <v>1783</v>
+      </c>
+      <c r="OM8">
+        <v>1768</v>
+      </c>
+      <c r="ON8">
+        <v>1796</v>
+      </c>
+      <c r="OO8">
+        <v>1772</v>
+      </c>
+      <c r="OP8">
+        <v>1788</v>
+      </c>
+      <c r="OQ8">
+        <v>1832</v>
+      </c>
+      <c r="OR8">
+        <v>1805</v>
+      </c>
     </row>
-    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -62282,8 +63220,29 @@
       <c r="OK9">
         <v>115</v>
       </c>
+      <c r="OL9">
+        <v>114</v>
+      </c>
+      <c r="OM9">
+        <v>115</v>
+      </c>
+      <c r="ON9">
+        <v>125</v>
+      </c>
+      <c r="OO9">
+        <v>122</v>
+      </c>
+      <c r="OP9">
+        <v>121</v>
+      </c>
+      <c r="OQ9">
+        <v>128</v>
+      </c>
+      <c r="OR9">
+        <v>128</v>
+      </c>
     </row>
-    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -63487,8 +64446,29 @@
       <c r="OK10">
         <v>107</v>
       </c>
+      <c r="OL10">
+        <v>100</v>
+      </c>
+      <c r="OM10">
+        <v>99</v>
+      </c>
+      <c r="ON10">
+        <v>101</v>
+      </c>
+      <c r="OO10">
+        <v>103</v>
+      </c>
+      <c r="OP10">
+        <v>107</v>
+      </c>
+      <c r="OQ10">
+        <v>109</v>
+      </c>
+      <c r="OR10">
+        <v>109</v>
+      </c>
     </row>
-    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -64692,8 +65672,29 @@
       <c r="OK11">
         <v>47</v>
       </c>
+      <c r="OL11">
+        <v>50</v>
+      </c>
+      <c r="OM11">
+        <v>46</v>
+      </c>
+      <c r="ON11">
+        <v>49</v>
+      </c>
+      <c r="OO11">
+        <v>50</v>
+      </c>
+      <c r="OP11">
+        <v>50</v>
+      </c>
+      <c r="OQ11">
+        <v>51</v>
+      </c>
+      <c r="OR11">
+        <v>53</v>
+      </c>
     </row>
-    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -65897,8 +66898,29 @@
       <c r="OK12">
         <v>185</v>
       </c>
+      <c r="OL12">
+        <v>178</v>
+      </c>
+      <c r="OM12">
+        <v>176</v>
+      </c>
+      <c r="ON12">
+        <v>174</v>
+      </c>
+      <c r="OO12">
+        <v>178</v>
+      </c>
+      <c r="OP12">
+        <v>175</v>
+      </c>
+      <c r="OQ12">
+        <v>178</v>
+      </c>
+      <c r="OR12">
+        <v>184</v>
+      </c>
     </row>
-    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -67102,8 +68124,29 @@
       <c r="OK13">
         <v>99</v>
       </c>
+      <c r="OL13">
+        <v>97</v>
+      </c>
+      <c r="OM13">
+        <v>94</v>
+      </c>
+      <c r="ON13">
+        <v>93</v>
+      </c>
+      <c r="OO13">
+        <v>97</v>
+      </c>
+      <c r="OP13">
+        <v>96</v>
+      </c>
+      <c r="OQ13">
+        <v>99</v>
+      </c>
+      <c r="OR13">
+        <v>100</v>
+      </c>
     </row>
-    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -68307,8 +69350,29 @@
       <c r="OK14">
         <v>22</v>
       </c>
+      <c r="OL14">
+        <v>22</v>
+      </c>
+      <c r="OM14">
+        <v>18</v>
+      </c>
+      <c r="ON14">
+        <v>18</v>
+      </c>
+      <c r="OO14">
+        <v>22</v>
+      </c>
+      <c r="OP14">
+        <v>23</v>
+      </c>
+      <c r="OQ14">
+        <v>25</v>
+      </c>
+      <c r="OR14">
+        <v>24</v>
+      </c>
     </row>
-    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -69512,8 +70576,29 @@
       <c r="OK15">
         <v>74</v>
       </c>
+      <c r="OL15">
+        <v>73</v>
+      </c>
+      <c r="OM15">
+        <v>74</v>
+      </c>
+      <c r="ON15">
+        <v>82</v>
+      </c>
+      <c r="OO15">
+        <v>83</v>
+      </c>
+      <c r="OP15">
+        <v>80</v>
+      </c>
+      <c r="OQ15">
+        <v>79</v>
+      </c>
+      <c r="OR15">
+        <v>82</v>
+      </c>
     </row>
-    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -70717,8 +71802,29 @@
       <c r="OK16">
         <v>5</v>
       </c>
+      <c r="OL16">
+        <v>6</v>
+      </c>
+      <c r="OM16">
+        <v>9</v>
+      </c>
+      <c r="ON16">
+        <v>9</v>
+      </c>
+      <c r="OO16">
+        <v>10</v>
+      </c>
+      <c r="OP16">
+        <v>10</v>
+      </c>
+      <c r="OQ16">
+        <v>10</v>
+      </c>
+      <c r="OR16">
+        <v>9</v>
+      </c>
     </row>
-    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -71922,8 +73028,29 @@
       <c r="OK17">
         <v>29</v>
       </c>
+      <c r="OL17">
+        <v>31</v>
+      </c>
+      <c r="OM17">
+        <v>31</v>
+      </c>
+      <c r="ON17">
+        <v>33</v>
+      </c>
+      <c r="OO17">
+        <v>28</v>
+      </c>
+      <c r="OP17">
+        <v>27</v>
+      </c>
+      <c r="OQ17">
+        <v>25</v>
+      </c>
+      <c r="OR17">
+        <v>30</v>
+      </c>
     </row>
-    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -73060,7 +74187,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:OK18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:OR18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -73239,50 +74366,78 @@
         <f t="shared" si="1"/>
         <v>2979</v>
       </c>
+      <c r="OL18" s="6">
+        <f t="shared" si="1"/>
+        <v>2972</v>
+      </c>
+      <c r="OM18" s="6">
+        <f t="shared" si="1"/>
+        <v>2935</v>
+      </c>
+      <c r="ON18" s="6">
+        <f t="shared" si="1"/>
+        <v>2991</v>
+      </c>
+      <c r="OO18" s="6">
+        <f t="shared" si="1"/>
+        <v>2974</v>
+      </c>
+      <c r="OP18" s="6">
+        <f t="shared" si="1"/>
+        <v>2980</v>
+      </c>
+      <c r="OQ18" s="6">
+        <f t="shared" si="1"/>
+        <v>3037</v>
+      </c>
+      <c r="OR18" s="6">
+        <f t="shared" si="1"/>
+        <v>3026</v>
+      </c>
     </row>
-    <row r="19" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -73302,12 +74457,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:OK34"/>
+  <dimension ref="A1:OR34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OA1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="OE18" sqref="OE18:OK18"/>
+      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73325,7 +74480,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -74529,8 +75684,29 @@
       <c r="OK1" s="8">
         <v>44334</v>
       </c>
+      <c r="OL1" s="8">
+        <v>44335</v>
+      </c>
+      <c r="OM1" s="8">
+        <v>44336</v>
+      </c>
+      <c r="ON1" s="8">
+        <v>44337</v>
+      </c>
+      <c r="OO1" s="8">
+        <v>44338</v>
+      </c>
+      <c r="OP1" s="8">
+        <v>44339</v>
+      </c>
+      <c r="OQ1" s="8">
+        <v>44340</v>
+      </c>
+      <c r="OR1" s="8">
+        <v>44341</v>
+      </c>
     </row>
-    <row r="2" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -75854,8 +77030,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK2-'UCI OCUPADA COVID'!OK2</f>
         <v>7</v>
       </c>
+      <c r="OL2">
+        <f>+'UCI OCUPADA TOTAL'!OL2-'UCI OCUPADA COVID'!OL2</f>
+        <v>6</v>
+      </c>
+      <c r="OM2">
+        <f>+'UCI OCUPADA TOTAL'!OM2-'UCI OCUPADA COVID'!OM2</f>
+        <v>5</v>
+      </c>
+      <c r="ON2">
+        <f>+'UCI OCUPADA TOTAL'!ON2-'UCI OCUPADA COVID'!ON2</f>
+        <v>7</v>
+      </c>
+      <c r="OO2">
+        <f>+'UCI OCUPADA TOTAL'!OO2-'UCI OCUPADA COVID'!OO2</f>
+        <v>5</v>
+      </c>
+      <c r="OP2">
+        <f>+'UCI OCUPADA TOTAL'!OP2-'UCI OCUPADA COVID'!OP2</f>
+        <v>5</v>
+      </c>
+      <c r="OQ2">
+        <f>+'UCI OCUPADA TOTAL'!OQ2-'UCI OCUPADA COVID'!OQ2</f>
+        <v>6</v>
+      </c>
+      <c r="OR2">
+        <f>+'UCI OCUPADA TOTAL'!OR2-'UCI OCUPADA COVID'!OR2</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -77179,8 +78383,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK3-'UCI OCUPADA COVID'!OK3</f>
         <v>4</v>
       </c>
+      <c r="OL3">
+        <f>+'UCI OCUPADA TOTAL'!OL3-'UCI OCUPADA COVID'!OL3</f>
+        <v>5</v>
+      </c>
+      <c r="OM3">
+        <f>+'UCI OCUPADA TOTAL'!OM3-'UCI OCUPADA COVID'!OM3</f>
+        <v>4</v>
+      </c>
+      <c r="ON3">
+        <f>+'UCI OCUPADA TOTAL'!ON3-'UCI OCUPADA COVID'!ON3</f>
+        <v>4</v>
+      </c>
+      <c r="OO3">
+        <f>+'UCI OCUPADA TOTAL'!OO3-'UCI OCUPADA COVID'!OO3</f>
+        <v>5</v>
+      </c>
+      <c r="OP3">
+        <f>+'UCI OCUPADA TOTAL'!OP3-'UCI OCUPADA COVID'!OP3</f>
+        <v>3</v>
+      </c>
+      <c r="OQ3">
+        <f>+'UCI OCUPADA TOTAL'!OQ3-'UCI OCUPADA COVID'!OQ3</f>
+        <v>5</v>
+      </c>
+      <c r="OR3">
+        <f>+'UCI OCUPADA TOTAL'!OR3-'UCI OCUPADA COVID'!OR3</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -78504,8 +79736,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK4-'UCI OCUPADA COVID'!OK4</f>
         <v>60</v>
       </c>
+      <c r="OL4">
+        <f>+'UCI OCUPADA TOTAL'!OL4-'UCI OCUPADA COVID'!OL4</f>
+        <v>61</v>
+      </c>
+      <c r="OM4">
+        <f>+'UCI OCUPADA TOTAL'!OM4-'UCI OCUPADA COVID'!OM4</f>
+        <v>60</v>
+      </c>
+      <c r="ON4">
+        <f>+'UCI OCUPADA TOTAL'!ON4-'UCI OCUPADA COVID'!ON4</f>
+        <v>64</v>
+      </c>
+      <c r="OO4">
+        <f>+'UCI OCUPADA TOTAL'!OO4-'UCI OCUPADA COVID'!OO4</f>
+        <v>60</v>
+      </c>
+      <c r="OP4">
+        <f>+'UCI OCUPADA TOTAL'!OP4-'UCI OCUPADA COVID'!OP4</f>
+        <v>63</v>
+      </c>
+      <c r="OQ4">
+        <f>+'UCI OCUPADA TOTAL'!OQ4-'UCI OCUPADA COVID'!OQ4</f>
+        <v>62</v>
+      </c>
+      <c r="OR4">
+        <f>+'UCI OCUPADA TOTAL'!OR4-'UCI OCUPADA COVID'!OR4</f>
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -79829,8 +81089,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK5-'UCI OCUPADA COVID'!OK5</f>
         <v>8</v>
       </c>
+      <c r="OL5">
+        <f>+'UCI OCUPADA TOTAL'!OL5-'UCI OCUPADA COVID'!OL5</f>
+        <v>6</v>
+      </c>
+      <c r="OM5">
+        <f>+'UCI OCUPADA TOTAL'!OM5-'UCI OCUPADA COVID'!OM5</f>
+        <v>5</v>
+      </c>
+      <c r="ON5">
+        <f>+'UCI OCUPADA TOTAL'!ON5-'UCI OCUPADA COVID'!ON5</f>
+        <v>4</v>
+      </c>
+      <c r="OO5">
+        <f>+'UCI OCUPADA TOTAL'!OO5-'UCI OCUPADA COVID'!OO5</f>
+        <v>6</v>
+      </c>
+      <c r="OP5">
+        <f>+'UCI OCUPADA TOTAL'!OP5-'UCI OCUPADA COVID'!OP5</f>
+        <v>6</v>
+      </c>
+      <c r="OQ5">
+        <f>+'UCI OCUPADA TOTAL'!OQ5-'UCI OCUPADA COVID'!OQ5</f>
+        <v>5</v>
+      </c>
+      <c r="OR5">
+        <f>+'UCI OCUPADA TOTAL'!OR5-'UCI OCUPADA COVID'!OR5</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -81154,8 +82442,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK6-'UCI OCUPADA COVID'!OK6</f>
         <v>31</v>
       </c>
+      <c r="OL6">
+        <f>+'UCI OCUPADA TOTAL'!OL6-'UCI OCUPADA COVID'!OL6</f>
+        <v>34</v>
+      </c>
+      <c r="OM6">
+        <f>+'UCI OCUPADA TOTAL'!OM6-'UCI OCUPADA COVID'!OM6</f>
+        <v>32</v>
+      </c>
+      <c r="ON6">
+        <f>+'UCI OCUPADA TOTAL'!ON6-'UCI OCUPADA COVID'!ON6</f>
+        <v>29</v>
+      </c>
+      <c r="OO6">
+        <f>+'UCI OCUPADA TOTAL'!OO6-'UCI OCUPADA COVID'!OO6</f>
+        <v>34</v>
+      </c>
+      <c r="OP6">
+        <f>+'UCI OCUPADA TOTAL'!OP6-'UCI OCUPADA COVID'!OP6</f>
+        <v>36</v>
+      </c>
+      <c r="OQ6">
+        <f>+'UCI OCUPADA TOTAL'!OQ6-'UCI OCUPADA COVID'!OQ6</f>
+        <v>38</v>
+      </c>
+      <c r="OR6">
+        <f>+'UCI OCUPADA TOTAL'!OR6-'UCI OCUPADA COVID'!OR6</f>
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -82479,8 +83795,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK7-'UCI OCUPADA COVID'!OK7</f>
         <v>92</v>
       </c>
+      <c r="OL7">
+        <f>+'UCI OCUPADA TOTAL'!OL7-'UCI OCUPADA COVID'!OL7</f>
+        <v>92</v>
+      </c>
+      <c r="OM7">
+        <f>+'UCI OCUPADA TOTAL'!OM7-'UCI OCUPADA COVID'!OM7</f>
+        <v>94</v>
+      </c>
+      <c r="ON7">
+        <f>+'UCI OCUPADA TOTAL'!ON7-'UCI OCUPADA COVID'!ON7</f>
+        <v>89</v>
+      </c>
+      <c r="OO7">
+        <f>+'UCI OCUPADA TOTAL'!OO7-'UCI OCUPADA COVID'!OO7</f>
+        <v>94</v>
+      </c>
+      <c r="OP7">
+        <f>+'UCI OCUPADA TOTAL'!OP7-'UCI OCUPADA COVID'!OP7</f>
+        <v>98</v>
+      </c>
+      <c r="OQ7">
+        <f>+'UCI OCUPADA TOTAL'!OQ7-'UCI OCUPADA COVID'!OQ7</f>
+        <v>106</v>
+      </c>
+      <c r="OR7">
+        <f>+'UCI OCUPADA TOTAL'!OR7-'UCI OCUPADA COVID'!OR7</f>
+        <v>110</v>
+      </c>
     </row>
-    <row r="8" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -83804,8 +85148,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK8-'UCI OCUPADA COVID'!OK8</f>
         <v>701</v>
       </c>
+      <c r="OL8">
+        <f>+'UCI OCUPADA TOTAL'!OL8-'UCI OCUPADA COVID'!OL8</f>
+        <v>695</v>
+      </c>
+      <c r="OM8">
+        <f>+'UCI OCUPADA TOTAL'!OM8-'UCI OCUPADA COVID'!OM8</f>
+        <v>715</v>
+      </c>
+      <c r="ON8">
+        <f>+'UCI OCUPADA TOTAL'!ON8-'UCI OCUPADA COVID'!ON8</f>
+        <v>691</v>
+      </c>
+      <c r="OO8">
+        <f>+'UCI OCUPADA TOTAL'!OO8-'UCI OCUPADA COVID'!OO8</f>
+        <v>717</v>
+      </c>
+      <c r="OP8">
+        <f>+'UCI OCUPADA TOTAL'!OP8-'UCI OCUPADA COVID'!OP8</f>
+        <v>720</v>
+      </c>
+      <c r="OQ8">
+        <f>+'UCI OCUPADA TOTAL'!OQ8-'UCI OCUPADA COVID'!OQ8</f>
+        <v>686</v>
+      </c>
+      <c r="OR8">
+        <f>+'UCI OCUPADA TOTAL'!OR8-'UCI OCUPADA COVID'!OR8</f>
+        <v>713</v>
+      </c>
     </row>
-    <row r="9" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -85129,8 +86501,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK9-'UCI OCUPADA COVID'!OK9</f>
         <v>47</v>
       </c>
+      <c r="OL9">
+        <f>+'UCI OCUPADA TOTAL'!OL9-'UCI OCUPADA COVID'!OL9</f>
+        <v>50</v>
+      </c>
+      <c r="OM9">
+        <f>+'UCI OCUPADA TOTAL'!OM9-'UCI OCUPADA COVID'!OM9</f>
+        <v>52</v>
+      </c>
+      <c r="ON9">
+        <f>+'UCI OCUPADA TOTAL'!ON9-'UCI OCUPADA COVID'!ON9</f>
+        <v>44</v>
+      </c>
+      <c r="OO9">
+        <f>+'UCI OCUPADA TOTAL'!OO9-'UCI OCUPADA COVID'!OO9</f>
+        <v>42</v>
+      </c>
+      <c r="OP9">
+        <f>+'UCI OCUPADA TOTAL'!OP9-'UCI OCUPADA COVID'!OP9</f>
+        <v>50</v>
+      </c>
+      <c r="OQ9">
+        <f>+'UCI OCUPADA TOTAL'!OQ9-'UCI OCUPADA COVID'!OQ9</f>
+        <v>41</v>
+      </c>
+      <c r="OR9">
+        <f>+'UCI OCUPADA TOTAL'!OR9-'UCI OCUPADA COVID'!OR9</f>
+        <v>47</v>
+      </c>
     </row>
-    <row r="10" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -86454,8 +87854,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK10-'UCI OCUPADA COVID'!OK10</f>
         <v>25</v>
       </c>
+      <c r="OL10">
+        <f>+'UCI OCUPADA TOTAL'!OL10-'UCI OCUPADA COVID'!OL10</f>
+        <v>26</v>
+      </c>
+      <c r="OM10">
+        <f>+'UCI OCUPADA TOTAL'!OM10-'UCI OCUPADA COVID'!OM10</f>
+        <v>31</v>
+      </c>
+      <c r="ON10">
+        <f>+'UCI OCUPADA TOTAL'!ON10-'UCI OCUPADA COVID'!ON10</f>
+        <v>30</v>
+      </c>
+      <c r="OO10">
+        <f>+'UCI OCUPADA TOTAL'!OO10-'UCI OCUPADA COVID'!OO10</f>
+        <v>34</v>
+      </c>
+      <c r="OP10">
+        <f>+'UCI OCUPADA TOTAL'!OP10-'UCI OCUPADA COVID'!OP10</f>
+        <v>26</v>
+      </c>
+      <c r="OQ10">
+        <f>+'UCI OCUPADA TOTAL'!OQ10-'UCI OCUPADA COVID'!OQ10</f>
+        <v>26</v>
+      </c>
+      <c r="OR10">
+        <f>+'UCI OCUPADA TOTAL'!OR10-'UCI OCUPADA COVID'!OR10</f>
+        <v>26</v>
+      </c>
     </row>
-    <row r="11" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -87779,8 +89207,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK11-'UCI OCUPADA COVID'!OK11</f>
         <v>14</v>
       </c>
+      <c r="OL11">
+        <f>+'UCI OCUPADA TOTAL'!OL11-'UCI OCUPADA COVID'!OL11</f>
+        <v>14</v>
+      </c>
+      <c r="OM11">
+        <f>+'UCI OCUPADA TOTAL'!OM11-'UCI OCUPADA COVID'!OM11</f>
+        <v>12</v>
+      </c>
+      <c r="ON11">
+        <f>+'UCI OCUPADA TOTAL'!ON11-'UCI OCUPADA COVID'!ON11</f>
+        <v>13</v>
+      </c>
+      <c r="OO11">
+        <f>+'UCI OCUPADA TOTAL'!OO11-'UCI OCUPADA COVID'!OO11</f>
+        <v>11</v>
+      </c>
+      <c r="OP11">
+        <f>+'UCI OCUPADA TOTAL'!OP11-'UCI OCUPADA COVID'!OP11</f>
+        <v>13</v>
+      </c>
+      <c r="OQ11">
+        <f>+'UCI OCUPADA TOTAL'!OQ11-'UCI OCUPADA COVID'!OQ11</f>
+        <v>14</v>
+      </c>
+      <c r="OR11">
+        <f>+'UCI OCUPADA TOTAL'!OR11-'UCI OCUPADA COVID'!OR11</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -89104,8 +90560,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK12-'UCI OCUPADA COVID'!OK12</f>
         <v>90</v>
       </c>
+      <c r="OL12">
+        <f>+'UCI OCUPADA TOTAL'!OL12-'UCI OCUPADA COVID'!OL12</f>
+        <v>101</v>
+      </c>
+      <c r="OM12">
+        <f>+'UCI OCUPADA TOTAL'!OM12-'UCI OCUPADA COVID'!OM12</f>
+        <v>96</v>
+      </c>
+      <c r="ON12">
+        <f>+'UCI OCUPADA TOTAL'!ON12-'UCI OCUPADA COVID'!ON12</f>
+        <v>98</v>
+      </c>
+      <c r="OO12">
+        <f>+'UCI OCUPADA TOTAL'!OO12-'UCI OCUPADA COVID'!OO12</f>
+        <v>97</v>
+      </c>
+      <c r="OP12">
+        <f>+'UCI OCUPADA TOTAL'!OP12-'UCI OCUPADA COVID'!OP12</f>
+        <v>94</v>
+      </c>
+      <c r="OQ12">
+        <f>+'UCI OCUPADA TOTAL'!OQ12-'UCI OCUPADA COVID'!OQ12</f>
+        <v>95</v>
+      </c>
+      <c r="OR12">
+        <f>+'UCI OCUPADA TOTAL'!OR12-'UCI OCUPADA COVID'!OR12</f>
+        <v>94</v>
+      </c>
     </row>
-    <row r="13" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -90429,8 +91913,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK13-'UCI OCUPADA COVID'!OK13</f>
         <v>34</v>
       </c>
+      <c r="OL13">
+        <f>+'UCI OCUPADA TOTAL'!OL13-'UCI OCUPADA COVID'!OL13</f>
+        <v>37</v>
+      </c>
+      <c r="OM13">
+        <f>+'UCI OCUPADA TOTAL'!OM13-'UCI OCUPADA COVID'!OM13</f>
+        <v>38</v>
+      </c>
+      <c r="ON13">
+        <f>+'UCI OCUPADA TOTAL'!ON13-'UCI OCUPADA COVID'!ON13</f>
+        <v>39</v>
+      </c>
+      <c r="OO13">
+        <f>+'UCI OCUPADA TOTAL'!OO13-'UCI OCUPADA COVID'!OO13</f>
+        <v>36</v>
+      </c>
+      <c r="OP13">
+        <f>+'UCI OCUPADA TOTAL'!OP13-'UCI OCUPADA COVID'!OP13</f>
+        <v>36</v>
+      </c>
+      <c r="OQ13">
+        <f>+'UCI OCUPADA TOTAL'!OQ13-'UCI OCUPADA COVID'!OQ13</f>
+        <v>34</v>
+      </c>
+      <c r="OR13">
+        <f>+'UCI OCUPADA TOTAL'!OR13-'UCI OCUPADA COVID'!OR13</f>
+        <v>41</v>
+      </c>
     </row>
-    <row r="14" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -91754,8 +93266,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK14-'UCI OCUPADA COVID'!OK14</f>
         <v>18</v>
       </c>
+      <c r="OL14">
+        <f>+'UCI OCUPADA TOTAL'!OL14-'UCI OCUPADA COVID'!OL14</f>
+        <v>18</v>
+      </c>
+      <c r="OM14">
+        <f>+'UCI OCUPADA TOTAL'!OM14-'UCI OCUPADA COVID'!OM14</f>
+        <v>19</v>
+      </c>
+      <c r="ON14">
+        <f>+'UCI OCUPADA TOTAL'!ON14-'UCI OCUPADA COVID'!ON14</f>
+        <v>16</v>
+      </c>
+      <c r="OO14">
+        <f>+'UCI OCUPADA TOTAL'!OO14-'UCI OCUPADA COVID'!OO14</f>
+        <v>16</v>
+      </c>
+      <c r="OP14">
+        <f>+'UCI OCUPADA TOTAL'!OP14-'UCI OCUPADA COVID'!OP14</f>
+        <v>14</v>
+      </c>
+      <c r="OQ14">
+        <f>+'UCI OCUPADA TOTAL'!OQ14-'UCI OCUPADA COVID'!OQ14</f>
+        <v>13</v>
+      </c>
+      <c r="OR14">
+        <f>+'UCI OCUPADA TOTAL'!OR14-'UCI OCUPADA COVID'!OR14</f>
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -93079,8 +94619,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK15-'UCI OCUPADA COVID'!OK15</f>
         <v>43</v>
       </c>
+      <c r="OL15">
+        <f>+'UCI OCUPADA TOTAL'!OL15-'UCI OCUPADA COVID'!OL15</f>
+        <v>48</v>
+      </c>
+      <c r="OM15">
+        <f>+'UCI OCUPADA TOTAL'!OM15-'UCI OCUPADA COVID'!OM15</f>
+        <v>46</v>
+      </c>
+      <c r="ON15">
+        <f>+'UCI OCUPADA TOTAL'!ON15-'UCI OCUPADA COVID'!ON15</f>
+        <v>38</v>
+      </c>
+      <c r="OO15">
+        <f>+'UCI OCUPADA TOTAL'!OO15-'UCI OCUPADA COVID'!OO15</f>
+        <v>35</v>
+      </c>
+      <c r="OP15">
+        <f>+'UCI OCUPADA TOTAL'!OP15-'UCI OCUPADA COVID'!OP15</f>
+        <v>36</v>
+      </c>
+      <c r="OQ15">
+        <f>+'UCI OCUPADA TOTAL'!OQ15-'UCI OCUPADA COVID'!OQ15</f>
+        <v>38</v>
+      </c>
+      <c r="OR15">
+        <f>+'UCI OCUPADA TOTAL'!OR15-'UCI OCUPADA COVID'!OR15</f>
+        <v>41</v>
+      </c>
     </row>
-    <row r="16" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -94404,8 +95972,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK16-'UCI OCUPADA COVID'!OK16</f>
         <v>5</v>
       </c>
+      <c r="OL16">
+        <f>+'UCI OCUPADA TOTAL'!OL16-'UCI OCUPADA COVID'!OL16</f>
+        <v>4</v>
+      </c>
+      <c r="OM16">
+        <f>+'UCI OCUPADA TOTAL'!OM16-'UCI OCUPADA COVID'!OM16</f>
+        <v>1</v>
+      </c>
+      <c r="ON16">
+        <f>+'UCI OCUPADA TOTAL'!ON16-'UCI OCUPADA COVID'!ON16</f>
+        <v>1</v>
+      </c>
+      <c r="OO16">
+        <f>+'UCI OCUPADA TOTAL'!OO16-'UCI OCUPADA COVID'!OO16</f>
+        <v>0</v>
+      </c>
+      <c r="OP16">
+        <f>+'UCI OCUPADA TOTAL'!OP16-'UCI OCUPADA COVID'!OP16</f>
+        <v>0</v>
+      </c>
+      <c r="OQ16">
+        <f>+'UCI OCUPADA TOTAL'!OQ16-'UCI OCUPADA COVID'!OQ16</f>
+        <v>0</v>
+      </c>
+      <c r="OR16">
+        <f>+'UCI OCUPADA TOTAL'!OR16-'UCI OCUPADA COVID'!OR16</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -95729,8 +97325,36 @@
         <f>+'UCI OCUPADA TOTAL'!OK17-'UCI OCUPADA COVID'!OK17</f>
         <v>8</v>
       </c>
+      <c r="OL17">
+        <f>+'UCI OCUPADA TOTAL'!OL17-'UCI OCUPADA COVID'!OL17</f>
+        <v>8</v>
+      </c>
+      <c r="OM17">
+        <f>+'UCI OCUPADA TOTAL'!OM17-'UCI OCUPADA COVID'!OM17</f>
+        <v>10</v>
+      </c>
+      <c r="ON17">
+        <f>+'UCI OCUPADA TOTAL'!ON17-'UCI OCUPADA COVID'!ON17</f>
+        <v>10</v>
+      </c>
+      <c r="OO17">
+        <f>+'UCI OCUPADA TOTAL'!OO17-'UCI OCUPADA COVID'!OO17</f>
+        <v>9</v>
+      </c>
+      <c r="OP17">
+        <f>+'UCI OCUPADA TOTAL'!OP17-'UCI OCUPADA COVID'!OP17</f>
+        <v>10</v>
+      </c>
+      <c r="OQ17">
+        <f>+'UCI OCUPADA TOTAL'!OQ17-'UCI OCUPADA COVID'!OQ17</f>
+        <v>11</v>
+      </c>
+      <c r="OR17">
+        <f>+'UCI OCUPADA TOTAL'!OR17-'UCI OCUPADA COVID'!OR17</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="18" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -97054,48 +98678,76 @@
         <f>+'UCI OCUPADA TOTAL'!OK18-'UCI OCUPADA COVID'!OK18</f>
         <v>1187</v>
       </c>
+      <c r="OL18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OL18-'UCI OCUPADA COVID'!OL18</f>
+        <v>1205</v>
+      </c>
+      <c r="OM18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OM18-'UCI OCUPADA COVID'!OM18</f>
+        <v>1220</v>
+      </c>
+      <c r="ON18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!ON18-'UCI OCUPADA COVID'!ON18</f>
+        <v>1177</v>
+      </c>
+      <c r="OO18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OO18-'UCI OCUPADA COVID'!OO18</f>
+        <v>1201</v>
+      </c>
+      <c r="OP18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OP18-'UCI OCUPADA COVID'!OP18</f>
+        <v>1210</v>
+      </c>
+      <c r="OQ18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OQ18-'UCI OCUPADA COVID'!OQ18</f>
+        <v>1180</v>
+      </c>
+      <c r="OR18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OR18-'UCI OCUPADA COVID'!OR18</f>
+        <v>1228</v>
+      </c>
     </row>
-    <row r="19" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:401" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
balance de camas uci, 1 junio 2021
Signed-off-by: Demián Arancibia <actions@github.com>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -2910,10 +2910,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OL1" sqref="OL1:OR18"/>
+      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4160,8 +4160,29 @@
       <c r="OR1" s="8">
         <v>44341</v>
       </c>
+      <c r="OS1" s="8">
+        <v>44342</v>
+      </c>
+      <c r="OT1" s="8">
+        <v>44343</v>
+      </c>
+      <c r="OU1" s="8">
+        <v>44344</v>
+      </c>
+      <c r="OV1" s="8">
+        <v>44345</v>
+      </c>
+      <c r="OW1" s="8">
+        <v>44346</v>
+      </c>
+      <c r="OX1" s="8">
+        <v>44347</v>
+      </c>
+      <c r="OY1" s="8">
+        <v>44348</v>
+      </c>
     </row>
-    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5386,8 +5407,29 @@
       <c r="OR2" s="11">
         <v>40</v>
       </c>
+      <c r="OS2" s="11">
+        <v>40</v>
+      </c>
+      <c r="OT2" s="11">
+        <v>38</v>
+      </c>
+      <c r="OU2" s="11">
+        <v>36</v>
+      </c>
+      <c r="OV2" s="11">
+        <v>36</v>
+      </c>
+      <c r="OW2" s="11">
+        <v>34</v>
+      </c>
+      <c r="OX2" s="11">
+        <v>34</v>
+      </c>
+      <c r="OY2" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6612,8 +6654,29 @@
       <c r="OR3" s="11">
         <v>62</v>
       </c>
+      <c r="OS3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OT3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OU3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OV3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OW3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OX3" s="11">
+        <v>62</v>
+      </c>
+      <c r="OY3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7838,8 +7901,29 @@
       <c r="OR4" s="11">
         <v>164</v>
       </c>
+      <c r="OS4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OT4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OU4" s="11">
+        <v>164</v>
+      </c>
+      <c r="OV4" s="11">
+        <v>165</v>
+      </c>
+      <c r="OW4" s="11">
+        <v>166</v>
+      </c>
+      <c r="OX4" s="11">
+        <v>166</v>
+      </c>
+      <c r="OY4" s="11">
+        <v>166</v>
+      </c>
     </row>
-    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -9064,8 +9148,29 @@
       <c r="OR5" s="11">
         <v>34</v>
       </c>
+      <c r="OS5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OT5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OU5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OV5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OW5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OX5" s="11">
+        <v>34</v>
+      </c>
+      <c r="OY5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10290,8 +10395,29 @@
       <c r="OR6" s="11">
         <v>132</v>
       </c>
+      <c r="OS6" s="11">
+        <v>134</v>
+      </c>
+      <c r="OT6" s="11">
+        <v>133</v>
+      </c>
+      <c r="OU6" s="11">
+        <v>138</v>
+      </c>
+      <c r="OV6" s="11">
+        <v>138</v>
+      </c>
+      <c r="OW6" s="11">
+        <v>133</v>
+      </c>
+      <c r="OX6" s="11">
+        <v>126</v>
+      </c>
+      <c r="OY6" s="11">
+        <v>132</v>
+      </c>
     </row>
-    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -11516,8 +11642,29 @@
       <c r="OR7" s="11">
         <v>329</v>
       </c>
+      <c r="OS7" s="11">
+        <v>329</v>
+      </c>
+      <c r="OT7" s="11">
+        <v>331</v>
+      </c>
+      <c r="OU7" s="11">
+        <v>331</v>
+      </c>
+      <c r="OV7" s="11">
+        <v>332</v>
+      </c>
+      <c r="OW7" s="11">
+        <v>332</v>
+      </c>
+      <c r="OX7" s="11">
+        <v>332</v>
+      </c>
+      <c r="OY7" s="11">
+        <v>332</v>
+      </c>
     </row>
-    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12742,8 +12889,29 @@
       <c r="OR8" s="11">
         <v>2577</v>
       </c>
+      <c r="OS8" s="11">
+        <v>2572</v>
+      </c>
+      <c r="OT8" s="11">
+        <v>2567</v>
+      </c>
+      <c r="OU8" s="11">
+        <v>2572</v>
+      </c>
+      <c r="OV8" s="11">
+        <v>2575</v>
+      </c>
+      <c r="OW8" s="11">
+        <v>2577</v>
+      </c>
+      <c r="OX8" s="11">
+        <v>2577</v>
+      </c>
+      <c r="OY8" s="11">
+        <v>2571</v>
+      </c>
     </row>
-    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -13968,8 +14136,29 @@
       <c r="OR9" s="11">
         <v>206</v>
       </c>
+      <c r="OS9" s="11">
+        <v>203</v>
+      </c>
+      <c r="OT9" s="11">
+        <v>203</v>
+      </c>
+      <c r="OU9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OV9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OW9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OX9" s="11">
+        <v>206</v>
+      </c>
+      <c r="OY9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -15194,8 +15383,29 @@
       <c r="OR10" s="11">
         <v>138</v>
       </c>
+      <c r="OS10" s="11">
+        <v>138</v>
+      </c>
+      <c r="OT10" s="11">
+        <v>157</v>
+      </c>
+      <c r="OU10" s="11">
+        <v>157</v>
+      </c>
+      <c r="OV10" s="11">
+        <v>157</v>
+      </c>
+      <c r="OW10" s="11">
+        <v>144</v>
+      </c>
+      <c r="OX10" s="11">
+        <v>143</v>
+      </c>
+      <c r="OY10" s="11">
+        <v>157</v>
+      </c>
     </row>
-    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -16420,8 +16630,29 @@
       <c r="OR11" s="11">
         <v>73</v>
       </c>
+      <c r="OS11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OT11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OU11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OV11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OW11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OX11" s="11">
+        <v>73</v>
+      </c>
+      <c r="OY11" s="11">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -17646,8 +17877,29 @@
       <c r="OR12" s="11">
         <v>306</v>
       </c>
+      <c r="OS12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OT12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OU12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OV12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OW12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OX12" s="11">
+        <v>309</v>
+      </c>
+      <c r="OY12" s="11">
+        <v>310</v>
+      </c>
     </row>
-    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -18872,8 +19124,29 @@
       <c r="OR13" s="11">
         <v>150</v>
       </c>
+      <c r="OS13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OT13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OU13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OV13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OW13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OX13" s="11">
+        <v>150</v>
+      </c>
+      <c r="OY13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -20098,8 +20371,29 @@
       <c r="OR14" s="11">
         <v>41</v>
       </c>
+      <c r="OS14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OT14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OU14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OV14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OW14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OX14" s="11">
+        <v>41</v>
+      </c>
+      <c r="OY14" s="11">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -21324,8 +21618,29 @@
       <c r="OR15" s="11">
         <v>126</v>
       </c>
+      <c r="OS15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OT15" s="11">
+        <v>126</v>
+      </c>
+      <c r="OU15" s="11">
+        <v>128</v>
+      </c>
+      <c r="OV15" s="11">
+        <v>129</v>
+      </c>
+      <c r="OW15" s="11">
+        <v>130</v>
+      </c>
+      <c r="OX15" s="11">
+        <v>129</v>
+      </c>
+      <c r="OY15" s="11">
+        <v>129</v>
+      </c>
     </row>
-    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -22550,8 +22865,29 @@
       <c r="OR16" s="11">
         <v>10</v>
       </c>
+      <c r="OS16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OT16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OU16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OV16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OW16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OX16" s="11">
+        <v>10</v>
+      </c>
+      <c r="OY16" s="11">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -23776,8 +24112,29 @@
       <c r="OR17" s="11">
         <v>47</v>
       </c>
+      <c r="OS17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OT17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OU17" s="11">
+        <v>47</v>
+      </c>
+      <c r="OV17" s="11">
+        <v>43</v>
+      </c>
+      <c r="OW17" s="11">
+        <v>43</v>
+      </c>
+      <c r="OX17" s="11">
+        <v>43</v>
+      </c>
+      <c r="OY17" s="11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="18" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -24953,7 +25310,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:OR18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:OY18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -25136,9 +25493,37 @@
         <f t="shared" si="7"/>
         <v>4435</v>
       </c>
+      <c r="OS18" s="6">
+        <f t="shared" si="7"/>
+        <v>4433</v>
+      </c>
+      <c r="OT18" s="6">
+        <f t="shared" si="7"/>
+        <v>4446</v>
+      </c>
+      <c r="OU18" s="6">
+        <f t="shared" si="7"/>
+        <v>4458</v>
+      </c>
+      <c r="OV18" s="6">
+        <f t="shared" si="7"/>
+        <v>4460</v>
+      </c>
+      <c r="OW18" s="6">
+        <f t="shared" si="7"/>
+        <v>4444</v>
+      </c>
+      <c r="OX18" s="6">
+        <f t="shared" si="7"/>
+        <v>4435</v>
+      </c>
+      <c r="OY18" s="6">
+        <f t="shared" si="7"/>
+        <v>4450</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:408 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -25156,12 +25541,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OR36"/>
+  <dimension ref="A1:OY36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
+      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25181,7 +25566,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -26406,8 +26791,29 @@
       <c r="OR1" s="8">
         <v>44341</v>
       </c>
+      <c r="OS1" s="8">
+        <v>44342</v>
+      </c>
+      <c r="OT1" s="8">
+        <v>44343</v>
+      </c>
+      <c r="OU1" s="8">
+        <v>44344</v>
+      </c>
+      <c r="OV1" s="8">
+        <v>44345</v>
+      </c>
+      <c r="OW1" s="8">
+        <v>44346</v>
+      </c>
+      <c r="OX1" s="8">
+        <v>44347</v>
+      </c>
+      <c r="OY1" s="8">
+        <v>44348</v>
+      </c>
     </row>
-    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -27632,8 +28038,29 @@
       <c r="OR2">
         <v>38</v>
       </c>
+      <c r="OS2">
+        <v>34</v>
+      </c>
+      <c r="OT2">
+        <v>35</v>
+      </c>
+      <c r="OU2">
+        <v>34</v>
+      </c>
+      <c r="OV2">
+        <v>33</v>
+      </c>
+      <c r="OW2">
+        <v>31</v>
+      </c>
+      <c r="OX2">
+        <v>31</v>
+      </c>
+      <c r="OY2">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -28858,8 +29285,29 @@
       <c r="OR3">
         <v>58</v>
       </c>
+      <c r="OS3">
+        <v>58</v>
+      </c>
+      <c r="OT3">
+        <v>54</v>
+      </c>
+      <c r="OU3">
+        <v>57</v>
+      </c>
+      <c r="OV3">
+        <v>58</v>
+      </c>
+      <c r="OW3">
+        <v>58</v>
+      </c>
+      <c r="OX3">
+        <v>60</v>
+      </c>
+      <c r="OY3">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -30084,8 +30532,29 @@
       <c r="OR4">
         <v>155</v>
       </c>
+      <c r="OS4">
+        <v>154</v>
+      </c>
+      <c r="OT4">
+        <v>156</v>
+      </c>
+      <c r="OU4">
+        <v>156</v>
+      </c>
+      <c r="OV4">
+        <v>154</v>
+      </c>
+      <c r="OW4">
+        <v>156</v>
+      </c>
+      <c r="OX4">
+        <v>153</v>
+      </c>
+      <c r="OY4">
+        <v>153</v>
+      </c>
     </row>
-    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -31310,8 +31779,29 @@
       <c r="OR5">
         <v>29</v>
       </c>
+      <c r="OS5">
+        <v>28</v>
+      </c>
+      <c r="OT5">
+        <v>29</v>
+      </c>
+      <c r="OU5">
+        <v>28</v>
+      </c>
+      <c r="OV5">
+        <v>28</v>
+      </c>
+      <c r="OW5">
+        <v>28</v>
+      </c>
+      <c r="OX5">
+        <v>28</v>
+      </c>
+      <c r="OY5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -32536,8 +33026,29 @@
       <c r="OR6">
         <v>127</v>
       </c>
+      <c r="OS6">
+        <v>126</v>
+      </c>
+      <c r="OT6">
+        <v>125</v>
+      </c>
+      <c r="OU6">
+        <v>135</v>
+      </c>
+      <c r="OV6">
+        <v>130</v>
+      </c>
+      <c r="OW6">
+        <v>127</v>
+      </c>
+      <c r="OX6">
+        <v>122</v>
+      </c>
+      <c r="OY6">
+        <v>130</v>
+      </c>
     </row>
-    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -33762,8 +34273,29 @@
       <c r="OR7">
         <v>321</v>
       </c>
+      <c r="OS7">
+        <v>315</v>
+      </c>
+      <c r="OT7">
+        <v>318</v>
+      </c>
+      <c r="OU7">
+        <v>315</v>
+      </c>
+      <c r="OV7">
+        <v>317</v>
+      </c>
+      <c r="OW7">
+        <v>322</v>
+      </c>
+      <c r="OX7">
+        <v>323</v>
+      </c>
+      <c r="OY7">
+        <v>323</v>
+      </c>
     </row>
-    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -34988,8 +35520,29 @@
       <c r="OR8">
         <v>2518</v>
       </c>
+      <c r="OS8">
+        <v>2507</v>
+      </c>
+      <c r="OT8">
+        <v>2506</v>
+      </c>
+      <c r="OU8">
+        <v>2509</v>
+      </c>
+      <c r="OV8">
+        <v>2527</v>
+      </c>
+      <c r="OW8">
+        <v>2531</v>
+      </c>
+      <c r="OX8">
+        <v>2534</v>
+      </c>
+      <c r="OY8">
+        <v>2536</v>
+      </c>
     </row>
-    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -36214,8 +36767,29 @@
       <c r="OR9">
         <v>175</v>
       </c>
+      <c r="OS9">
+        <v>179</v>
+      </c>
+      <c r="OT9">
+        <v>179</v>
+      </c>
+      <c r="OU9">
+        <v>185</v>
+      </c>
+      <c r="OV9">
+        <v>188</v>
+      </c>
+      <c r="OW9">
+        <v>183</v>
+      </c>
+      <c r="OX9">
+        <v>193</v>
+      </c>
+      <c r="OY9">
+        <v>191</v>
+      </c>
     </row>
-    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -37440,8 +38014,29 @@
       <c r="OR10">
         <v>135</v>
       </c>
+      <c r="OS10">
+        <v>132</v>
+      </c>
+      <c r="OT10">
+        <v>129</v>
+      </c>
+      <c r="OU10">
+        <v>132</v>
+      </c>
+      <c r="OV10">
+        <v>132</v>
+      </c>
+      <c r="OW10">
+        <v>135</v>
+      </c>
+      <c r="OX10">
+        <v>136</v>
+      </c>
+      <c r="OY10">
+        <v>137</v>
+      </c>
     </row>
-    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -38666,8 +39261,29 @@
       <c r="OR11">
         <v>69</v>
       </c>
+      <c r="OS11">
+        <v>68</v>
+      </c>
+      <c r="OT11">
+        <v>67</v>
+      </c>
+      <c r="OU11">
+        <v>67</v>
+      </c>
+      <c r="OV11">
+        <v>58</v>
+      </c>
+      <c r="OW11">
+        <v>58</v>
+      </c>
+      <c r="OX11">
+        <v>66</v>
+      </c>
+      <c r="OY11">
+        <v>68</v>
+      </c>
     </row>
-    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -39892,8 +40508,29 @@
       <c r="OR12">
         <v>278</v>
       </c>
+      <c r="OS12">
+        <v>281</v>
+      </c>
+      <c r="OT12">
+        <v>281</v>
+      </c>
+      <c r="OU12">
+        <v>285</v>
+      </c>
+      <c r="OV12">
+        <v>290</v>
+      </c>
+      <c r="OW12">
+        <v>284</v>
+      </c>
+      <c r="OX12">
+        <v>285</v>
+      </c>
+      <c r="OY12">
+        <v>289</v>
+      </c>
     </row>
-    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -41118,8 +41755,29 @@
       <c r="OR13">
         <v>141</v>
       </c>
+      <c r="OS13">
+        <v>140</v>
+      </c>
+      <c r="OT13">
+        <v>141</v>
+      </c>
+      <c r="OU13">
+        <v>143</v>
+      </c>
+      <c r="OV13">
+        <v>140</v>
+      </c>
+      <c r="OW13">
+        <v>142</v>
+      </c>
+      <c r="OX13">
+        <v>143</v>
+      </c>
+      <c r="OY13">
+        <v>141</v>
+      </c>
     </row>
-    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -42344,8 +43002,29 @@
       <c r="OR14">
         <v>37</v>
       </c>
+      <c r="OS14">
+        <v>39</v>
+      </c>
+      <c r="OT14">
+        <v>39</v>
+      </c>
+      <c r="OU14">
+        <v>38</v>
+      </c>
+      <c r="OV14">
+        <v>40</v>
+      </c>
+      <c r="OW14">
+        <v>41</v>
+      </c>
+      <c r="OX14">
+        <v>39</v>
+      </c>
+      <c r="OY14">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -43570,8 +44249,29 @@
       <c r="OR15">
         <v>123</v>
       </c>
+      <c r="OS15">
+        <v>121</v>
+      </c>
+      <c r="OT15">
+        <v>124</v>
+      </c>
+      <c r="OU15">
+        <v>122</v>
+      </c>
+      <c r="OV15">
+        <v>126</v>
+      </c>
+      <c r="OW15">
+        <v>126</v>
+      </c>
+      <c r="OX15">
+        <v>124</v>
+      </c>
+      <c r="OY15">
+        <v>127</v>
+      </c>
     </row>
-    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -44796,8 +45496,29 @@
       <c r="OR16">
         <v>10</v>
       </c>
+      <c r="OS16">
+        <v>10</v>
+      </c>
+      <c r="OT16">
+        <v>10</v>
+      </c>
+      <c r="OU16">
+        <v>10</v>
+      </c>
+      <c r="OV16">
+        <v>10</v>
+      </c>
+      <c r="OW16">
+        <v>10</v>
+      </c>
+      <c r="OX16">
+        <v>10</v>
+      </c>
+      <c r="OY16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -46022,8 +46743,29 @@
       <c r="OR17">
         <v>40</v>
       </c>
+      <c r="OS17">
+        <v>37</v>
+      </c>
+      <c r="OT17">
+        <v>36</v>
+      </c>
+      <c r="OU17">
+        <v>35</v>
+      </c>
+      <c r="OV17">
+        <v>34</v>
+      </c>
+      <c r="OW17">
+        <v>34</v>
+      </c>
+      <c r="OX17">
+        <v>38</v>
+      </c>
+      <c r="OY17">
+        <v>39</v>
+      </c>
     </row>
-    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -47115,7 +47857,7 @@
         <v>3309</v>
       </c>
       <c r="MI18" s="6">
-        <f t="shared" ref="MI18:OR18" si="1">SUM(MI2:MI17)</f>
+        <f t="shared" ref="MI18:OT18" si="1">SUM(MI2:MI17)</f>
         <v>3336</v>
       </c>
       <c r="MJ18" s="6">
@@ -47362,8 +48104,36 @@
         <f t="shared" si="1"/>
         <v>4254</v>
       </c>
+      <c r="OS18" s="6">
+        <f t="shared" si="1"/>
+        <v>4229</v>
+      </c>
+      <c r="OT18" s="6">
+        <f t="shared" si="1"/>
+        <v>4229</v>
+      </c>
+      <c r="OU18" s="6">
+        <f t="shared" ref="OU18:OY18" si="2">SUM(OU2:OU17)</f>
+        <v>4251</v>
+      </c>
+      <c r="OV18" s="6">
+        <f t="shared" si="2"/>
+        <v>4265</v>
+      </c>
+      <c r="OW18" s="6">
+        <f t="shared" si="2"/>
+        <v>4266</v>
+      </c>
+      <c r="OX18" s="6">
+        <f t="shared" si="2"/>
+        <v>4285</v>
+      </c>
+      <c r="OY18" s="6">
+        <f t="shared" si="2"/>
+        <v>4303</v>
+      </c>
     </row>
-    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -47646,7 +48416,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -47929,7 +48699,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -48212,7 +48982,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -48495,7 +49265,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -48778,7 +49548,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -49061,7 +49831,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -49344,7 +50114,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -49627,7 +50397,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -49910,7 +50680,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -50193,7 +50963,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -50476,7 +51246,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -50759,7 +51529,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -52182,12 +52952,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OR34"/>
+  <dimension ref="A1:OY34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
+      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52208,7 +52978,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -53433,8 +54203,29 @@
       <c r="OR1" s="8">
         <v>44341</v>
       </c>
+      <c r="OS1" s="8">
+        <v>44342</v>
+      </c>
+      <c r="OT1" s="8">
+        <v>44343</v>
+      </c>
+      <c r="OU1" s="8">
+        <v>44344</v>
+      </c>
+      <c r="OV1" s="8">
+        <v>44345</v>
+      </c>
+      <c r="OW1" s="8">
+        <v>44346</v>
+      </c>
+      <c r="OX1" s="8">
+        <v>44347</v>
+      </c>
+      <c r="OY1" s="8">
+        <v>44348</v>
+      </c>
     </row>
-    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -54659,8 +55450,29 @@
       <c r="OR2">
         <v>31</v>
       </c>
+      <c r="OS2">
+        <v>30</v>
+      </c>
+      <c r="OT2">
+        <v>31</v>
+      </c>
+      <c r="OU2">
+        <v>31</v>
+      </c>
+      <c r="OV2">
+        <v>30</v>
+      </c>
+      <c r="OW2">
+        <v>29</v>
+      </c>
+      <c r="OX2">
+        <v>28</v>
+      </c>
+      <c r="OY2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -55885,8 +56697,29 @@
       <c r="OR3">
         <v>52</v>
       </c>
+      <c r="OS3">
+        <v>51</v>
+      </c>
+      <c r="OT3">
+        <v>48</v>
+      </c>
+      <c r="OU3">
+        <v>51</v>
+      </c>
+      <c r="OV3">
+        <v>51</v>
+      </c>
+      <c r="OW3">
+        <v>51</v>
+      </c>
+      <c r="OX3">
+        <v>54</v>
+      </c>
+      <c r="OY3">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -57111,8 +57944,29 @@
       <c r="OR4">
         <v>93</v>
       </c>
+      <c r="OS4">
+        <v>91</v>
+      </c>
+      <c r="OT4">
+        <v>88</v>
+      </c>
+      <c r="OU4">
+        <v>91</v>
+      </c>
+      <c r="OV4">
+        <v>93</v>
+      </c>
+      <c r="OW4">
+        <v>91</v>
+      </c>
+      <c r="OX4">
+        <v>87</v>
+      </c>
+      <c r="OY4">
+        <v>90</v>
+      </c>
     </row>
-    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -58337,8 +59191,29 @@
       <c r="OR5">
         <v>23</v>
       </c>
+      <c r="OS5">
+        <v>23</v>
+      </c>
+      <c r="OT5">
+        <v>23</v>
+      </c>
+      <c r="OU5">
+        <v>24</v>
+      </c>
+      <c r="OV5">
+        <v>23</v>
+      </c>
+      <c r="OW5">
+        <v>24</v>
+      </c>
+      <c r="OX5">
+        <v>24</v>
+      </c>
+      <c r="OY5">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -59563,8 +60438,29 @@
       <c r="OR6">
         <v>92</v>
       </c>
+      <c r="OS6">
+        <v>89</v>
+      </c>
+      <c r="OT6">
+        <v>89</v>
+      </c>
+      <c r="OU6">
+        <v>88</v>
+      </c>
+      <c r="OV6">
+        <v>93</v>
+      </c>
+      <c r="OW6">
+        <v>89</v>
+      </c>
+      <c r="OX6">
+        <v>87</v>
+      </c>
+      <c r="OY6">
+        <v>95</v>
+      </c>
     </row>
-    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -60789,8 +61685,29 @@
       <c r="OR7">
         <v>211</v>
       </c>
+      <c r="OS7">
+        <v>223</v>
+      </c>
+      <c r="OT7">
+        <v>217</v>
+      </c>
+      <c r="OU7">
+        <v>207</v>
+      </c>
+      <c r="OV7">
+        <v>216</v>
+      </c>
+      <c r="OW7">
+        <v>213</v>
+      </c>
+      <c r="OX7">
+        <v>213</v>
+      </c>
+      <c r="OY7">
+        <v>217</v>
+      </c>
     </row>
-    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -62015,8 +62932,29 @@
       <c r="OR8">
         <v>1805</v>
       </c>
+      <c r="OS8">
+        <v>1792</v>
+      </c>
+      <c r="OT8">
+        <v>1787</v>
+      </c>
+      <c r="OU8">
+        <v>1835</v>
+      </c>
+      <c r="OV8">
+        <v>1840</v>
+      </c>
+      <c r="OW8">
+        <v>1878</v>
+      </c>
+      <c r="OX8">
+        <v>1881</v>
+      </c>
+      <c r="OY8">
+        <v>1908</v>
+      </c>
     </row>
-    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -63241,8 +64179,29 @@
       <c r="OR9">
         <v>128</v>
       </c>
+      <c r="OS9">
+        <v>135</v>
+      </c>
+      <c r="OT9">
+        <v>142</v>
+      </c>
+      <c r="OU9">
+        <v>142</v>
+      </c>
+      <c r="OV9">
+        <v>141</v>
+      </c>
+      <c r="OW9">
+        <v>148</v>
+      </c>
+      <c r="OX9">
+        <v>154</v>
+      </c>
+      <c r="OY9">
+        <v>155</v>
+      </c>
     </row>
-    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -64467,8 +65426,29 @@
       <c r="OR10">
         <v>109</v>
       </c>
+      <c r="OS10">
+        <v>106</v>
+      </c>
+      <c r="OT10">
+        <v>104</v>
+      </c>
+      <c r="OU10">
+        <v>105</v>
+      </c>
+      <c r="OV10">
+        <v>106</v>
+      </c>
+      <c r="OW10">
+        <v>110</v>
+      </c>
+      <c r="OX10">
+        <v>110</v>
+      </c>
+      <c r="OY10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -65693,8 +66673,29 @@
       <c r="OR11">
         <v>53</v>
       </c>
+      <c r="OS11">
+        <v>54</v>
+      </c>
+      <c r="OT11">
+        <v>53</v>
+      </c>
+      <c r="OU11">
+        <v>51</v>
+      </c>
+      <c r="OV11">
+        <v>45</v>
+      </c>
+      <c r="OW11">
+        <v>47</v>
+      </c>
+      <c r="OX11">
+        <v>50</v>
+      </c>
+      <c r="OY11">
+        <v>52</v>
+      </c>
     </row>
-    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -66919,8 +67920,29 @@
       <c r="OR12">
         <v>184</v>
       </c>
+      <c r="OS12">
+        <v>182</v>
+      </c>
+      <c r="OT12">
+        <v>181</v>
+      </c>
+      <c r="OU12">
+        <v>190</v>
+      </c>
+      <c r="OV12">
+        <v>195</v>
+      </c>
+      <c r="OW12">
+        <v>185</v>
+      </c>
+      <c r="OX12">
+        <v>189</v>
+      </c>
+      <c r="OY12">
+        <v>196</v>
+      </c>
     </row>
-    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -68145,8 +69167,29 @@
       <c r="OR13">
         <v>100</v>
       </c>
+      <c r="OS13">
+        <v>101</v>
+      </c>
+      <c r="OT13">
+        <v>104</v>
+      </c>
+      <c r="OU13">
+        <v>103</v>
+      </c>
+      <c r="OV13">
+        <v>102</v>
+      </c>
+      <c r="OW13">
+        <v>106</v>
+      </c>
+      <c r="OX13">
+        <v>108</v>
+      </c>
+      <c r="OY13">
+        <v>105</v>
+      </c>
     </row>
-    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -69371,8 +70414,29 @@
       <c r="OR14">
         <v>24</v>
       </c>
+      <c r="OS14">
+        <v>24</v>
+      </c>
+      <c r="OT14">
+        <v>25</v>
+      </c>
+      <c r="OU14">
+        <v>26</v>
+      </c>
+      <c r="OV14">
+        <v>28</v>
+      </c>
+      <c r="OW14">
+        <v>30</v>
+      </c>
+      <c r="OX14">
+        <v>29</v>
+      </c>
+      <c r="OY14">
+        <v>30</v>
+      </c>
     </row>
-    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -70597,8 +71661,29 @@
       <c r="OR15">
         <v>82</v>
       </c>
+      <c r="OS15">
+        <v>82</v>
+      </c>
+      <c r="OT15">
+        <v>86</v>
+      </c>
+      <c r="OU15">
+        <v>89</v>
+      </c>
+      <c r="OV15">
+        <v>92</v>
+      </c>
+      <c r="OW15">
+        <v>91</v>
+      </c>
+      <c r="OX15">
+        <v>91</v>
+      </c>
+      <c r="OY15">
+        <v>92</v>
+      </c>
     </row>
-    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -71823,8 +72908,29 @@
       <c r="OR16">
         <v>9</v>
       </c>
+      <c r="OS16">
+        <v>10</v>
+      </c>
+      <c r="OT16">
+        <v>10</v>
+      </c>
+      <c r="OU16">
+        <v>10</v>
+      </c>
+      <c r="OV16">
+        <v>10</v>
+      </c>
+      <c r="OW16">
+        <v>10</v>
+      </c>
+      <c r="OX16">
+        <v>10</v>
+      </c>
+      <c r="OY16">
+        <v>10</v>
+      </c>
     </row>
-    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -73049,8 +74155,29 @@
       <c r="OR17">
         <v>30</v>
       </c>
+      <c r="OS17">
+        <v>30</v>
+      </c>
+      <c r="OT17">
+        <v>26</v>
+      </c>
+      <c r="OU17">
+        <v>24</v>
+      </c>
+      <c r="OV17">
+        <v>27</v>
+      </c>
+      <c r="OW17">
+        <v>25</v>
+      </c>
+      <c r="OX17">
+        <v>27</v>
+      </c>
+      <c r="OY17">
+        <v>29</v>
+      </c>
     </row>
-    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -74187,7 +75314,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:OR18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:OY18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -74394,50 +75521,78 @@
         <f t="shared" si="1"/>
         <v>3026</v>
       </c>
+      <c r="OS18" s="6">
+        <f t="shared" si="1"/>
+        <v>3023</v>
+      </c>
+      <c r="OT18" s="6">
+        <f t="shared" si="1"/>
+        <v>3014</v>
+      </c>
+      <c r="OU18" s="6">
+        <f t="shared" si="1"/>
+        <v>3067</v>
+      </c>
+      <c r="OV18" s="6">
+        <f t="shared" si="1"/>
+        <v>3092</v>
+      </c>
+      <c r="OW18" s="6">
+        <f t="shared" si="1"/>
+        <v>3127</v>
+      </c>
+      <c r="OX18" s="6">
+        <f t="shared" si="1"/>
+        <v>3142</v>
+      </c>
+      <c r="OY18" s="6">
+        <f t="shared" si="1"/>
+        <v>3193</v>
+      </c>
     </row>
-    <row r="19" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -74457,12 +75612,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:OR34"/>
+  <dimension ref="A1:OY34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OK1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="OL2" sqref="OL2:OR18"/>
+      <selection pane="topRight" activeCell="PA20" sqref="PA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74480,7 +75635,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -75705,8 +76860,29 @@
       <c r="OR1" s="8">
         <v>44341</v>
       </c>
+      <c r="OS1" s="8">
+        <v>44342</v>
+      </c>
+      <c r="OT1" s="8">
+        <v>44343</v>
+      </c>
+      <c r="OU1" s="8">
+        <v>44344</v>
+      </c>
+      <c r="OV1" s="8">
+        <v>44345</v>
+      </c>
+      <c r="OW1" s="8">
+        <v>44346</v>
+      </c>
+      <c r="OX1" s="8">
+        <v>44347</v>
+      </c>
+      <c r="OY1" s="8">
+        <v>44348</v>
+      </c>
     </row>
-    <row r="2" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -77058,8 +78234,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR2-'UCI OCUPADA COVID'!OR2</f>
         <v>7</v>
       </c>
+      <c r="OS2">
+        <f>+'UCI OCUPADA TOTAL'!OS2-'UCI OCUPADA COVID'!OS2</f>
+        <v>4</v>
+      </c>
+      <c r="OT2">
+        <f>+'UCI OCUPADA TOTAL'!OT2-'UCI OCUPADA COVID'!OT2</f>
+        <v>4</v>
+      </c>
+      <c r="OU2">
+        <f>+'UCI OCUPADA TOTAL'!OU2-'UCI OCUPADA COVID'!OU2</f>
+        <v>3</v>
+      </c>
+      <c r="OV2">
+        <f>+'UCI OCUPADA TOTAL'!OV2-'UCI OCUPADA COVID'!OV2</f>
+        <v>3</v>
+      </c>
+      <c r="OW2">
+        <f>+'UCI OCUPADA TOTAL'!OW2-'UCI OCUPADA COVID'!OW2</f>
+        <v>2</v>
+      </c>
+      <c r="OX2">
+        <f>+'UCI OCUPADA TOTAL'!OX2-'UCI OCUPADA COVID'!OX2</f>
+        <v>3</v>
+      </c>
+      <c r="OY2">
+        <f>+'UCI OCUPADA TOTAL'!OY2-'UCI OCUPADA COVID'!OY2</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -78411,8 +79615,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR3-'UCI OCUPADA COVID'!OR3</f>
         <v>6</v>
       </c>
+      <c r="OS3">
+        <f>+'UCI OCUPADA TOTAL'!OS3-'UCI OCUPADA COVID'!OS3</f>
+        <v>7</v>
+      </c>
+      <c r="OT3">
+        <f>+'UCI OCUPADA TOTAL'!OT3-'UCI OCUPADA COVID'!OT3</f>
+        <v>6</v>
+      </c>
+      <c r="OU3">
+        <f>+'UCI OCUPADA TOTAL'!OU3-'UCI OCUPADA COVID'!OU3</f>
+        <v>6</v>
+      </c>
+      <c r="OV3">
+        <f>+'UCI OCUPADA TOTAL'!OV3-'UCI OCUPADA COVID'!OV3</f>
+        <v>7</v>
+      </c>
+      <c r="OW3">
+        <f>+'UCI OCUPADA TOTAL'!OW3-'UCI OCUPADA COVID'!OW3</f>
+        <v>7</v>
+      </c>
+      <c r="OX3">
+        <f>+'UCI OCUPADA TOTAL'!OX3-'UCI OCUPADA COVID'!OX3</f>
+        <v>6</v>
+      </c>
+      <c r="OY3">
+        <f>+'UCI OCUPADA TOTAL'!OY3-'UCI OCUPADA COVID'!OY3</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -79764,8 +80996,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR4-'UCI OCUPADA COVID'!OR4</f>
         <v>62</v>
       </c>
+      <c r="OS4">
+        <f>+'UCI OCUPADA TOTAL'!OS4-'UCI OCUPADA COVID'!OS4</f>
+        <v>63</v>
+      </c>
+      <c r="OT4">
+        <f>+'UCI OCUPADA TOTAL'!OT4-'UCI OCUPADA COVID'!OT4</f>
+        <v>68</v>
+      </c>
+      <c r="OU4">
+        <f>+'UCI OCUPADA TOTAL'!OU4-'UCI OCUPADA COVID'!OU4</f>
+        <v>65</v>
+      </c>
+      <c r="OV4">
+        <f>+'UCI OCUPADA TOTAL'!OV4-'UCI OCUPADA COVID'!OV4</f>
+        <v>61</v>
+      </c>
+      <c r="OW4">
+        <f>+'UCI OCUPADA TOTAL'!OW4-'UCI OCUPADA COVID'!OW4</f>
+        <v>65</v>
+      </c>
+      <c r="OX4">
+        <f>+'UCI OCUPADA TOTAL'!OX4-'UCI OCUPADA COVID'!OX4</f>
+        <v>66</v>
+      </c>
+      <c r="OY4">
+        <f>+'UCI OCUPADA TOTAL'!OY4-'UCI OCUPADA COVID'!OY4</f>
+        <v>63</v>
+      </c>
     </row>
-    <row r="5" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -81117,8 +82377,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR5-'UCI OCUPADA COVID'!OR5</f>
         <v>6</v>
       </c>
+      <c r="OS5">
+        <f>+'UCI OCUPADA TOTAL'!OS5-'UCI OCUPADA COVID'!OS5</f>
+        <v>5</v>
+      </c>
+      <c r="OT5">
+        <f>+'UCI OCUPADA TOTAL'!OT5-'UCI OCUPADA COVID'!OT5</f>
+        <v>6</v>
+      </c>
+      <c r="OU5">
+        <f>+'UCI OCUPADA TOTAL'!OU5-'UCI OCUPADA COVID'!OU5</f>
+        <v>4</v>
+      </c>
+      <c r="OV5">
+        <f>+'UCI OCUPADA TOTAL'!OV5-'UCI OCUPADA COVID'!OV5</f>
+        <v>5</v>
+      </c>
+      <c r="OW5">
+        <f>+'UCI OCUPADA TOTAL'!OW5-'UCI OCUPADA COVID'!OW5</f>
+        <v>4</v>
+      </c>
+      <c r="OX5">
+        <f>+'UCI OCUPADA TOTAL'!OX5-'UCI OCUPADA COVID'!OX5</f>
+        <v>4</v>
+      </c>
+      <c r="OY5">
+        <f>+'UCI OCUPADA TOTAL'!OY5-'UCI OCUPADA COVID'!OY5</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -82470,8 +83758,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR6-'UCI OCUPADA COVID'!OR6</f>
         <v>35</v>
       </c>
+      <c r="OS6">
+        <f>+'UCI OCUPADA TOTAL'!OS6-'UCI OCUPADA COVID'!OS6</f>
+        <v>37</v>
+      </c>
+      <c r="OT6">
+        <f>+'UCI OCUPADA TOTAL'!OT6-'UCI OCUPADA COVID'!OT6</f>
+        <v>36</v>
+      </c>
+      <c r="OU6">
+        <f>+'UCI OCUPADA TOTAL'!OU6-'UCI OCUPADA COVID'!OU6</f>
+        <v>47</v>
+      </c>
+      <c r="OV6">
+        <f>+'UCI OCUPADA TOTAL'!OV6-'UCI OCUPADA COVID'!OV6</f>
+        <v>37</v>
+      </c>
+      <c r="OW6">
+        <f>+'UCI OCUPADA TOTAL'!OW6-'UCI OCUPADA COVID'!OW6</f>
+        <v>38</v>
+      </c>
+      <c r="OX6">
+        <f>+'UCI OCUPADA TOTAL'!OX6-'UCI OCUPADA COVID'!OX6</f>
+        <v>35</v>
+      </c>
+      <c r="OY6">
+        <f>+'UCI OCUPADA TOTAL'!OY6-'UCI OCUPADA COVID'!OY6</f>
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -83823,8 +85139,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR7-'UCI OCUPADA COVID'!OR7</f>
         <v>110</v>
       </c>
+      <c r="OS7">
+        <f>+'UCI OCUPADA TOTAL'!OS7-'UCI OCUPADA COVID'!OS7</f>
+        <v>92</v>
+      </c>
+      <c r="OT7">
+        <f>+'UCI OCUPADA TOTAL'!OT7-'UCI OCUPADA COVID'!OT7</f>
+        <v>101</v>
+      </c>
+      <c r="OU7">
+        <f>+'UCI OCUPADA TOTAL'!OU7-'UCI OCUPADA COVID'!OU7</f>
+        <v>108</v>
+      </c>
+      <c r="OV7">
+        <f>+'UCI OCUPADA TOTAL'!OV7-'UCI OCUPADA COVID'!OV7</f>
+        <v>101</v>
+      </c>
+      <c r="OW7">
+        <f>+'UCI OCUPADA TOTAL'!OW7-'UCI OCUPADA COVID'!OW7</f>
+        <v>109</v>
+      </c>
+      <c r="OX7">
+        <f>+'UCI OCUPADA TOTAL'!OX7-'UCI OCUPADA COVID'!OX7</f>
+        <v>110</v>
+      </c>
+      <c r="OY7">
+        <f>+'UCI OCUPADA TOTAL'!OY7-'UCI OCUPADA COVID'!OY7</f>
+        <v>106</v>
+      </c>
     </row>
-    <row r="8" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -85176,8 +86520,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR8-'UCI OCUPADA COVID'!OR8</f>
         <v>713</v>
       </c>
+      <c r="OS8">
+        <f>+'UCI OCUPADA TOTAL'!OS8-'UCI OCUPADA COVID'!OS8</f>
+        <v>715</v>
+      </c>
+      <c r="OT8">
+        <f>+'UCI OCUPADA TOTAL'!OT8-'UCI OCUPADA COVID'!OT8</f>
+        <v>719</v>
+      </c>
+      <c r="OU8">
+        <f>+'UCI OCUPADA TOTAL'!OU8-'UCI OCUPADA COVID'!OU8</f>
+        <v>674</v>
+      </c>
+      <c r="OV8">
+        <f>+'UCI OCUPADA TOTAL'!OV8-'UCI OCUPADA COVID'!OV8</f>
+        <v>687</v>
+      </c>
+      <c r="OW8">
+        <f>+'UCI OCUPADA TOTAL'!OW8-'UCI OCUPADA COVID'!OW8</f>
+        <v>653</v>
+      </c>
+      <c r="OX8">
+        <f>+'UCI OCUPADA TOTAL'!OX8-'UCI OCUPADA COVID'!OX8</f>
+        <v>653</v>
+      </c>
+      <c r="OY8">
+        <f>+'UCI OCUPADA TOTAL'!OY8-'UCI OCUPADA COVID'!OY8</f>
+        <v>628</v>
+      </c>
     </row>
-    <row r="9" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -86529,8 +87901,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR9-'UCI OCUPADA COVID'!OR9</f>
         <v>47</v>
       </c>
+      <c r="OS9">
+        <f>+'UCI OCUPADA TOTAL'!OS9-'UCI OCUPADA COVID'!OS9</f>
+        <v>44</v>
+      </c>
+      <c r="OT9">
+        <f>+'UCI OCUPADA TOTAL'!OT9-'UCI OCUPADA COVID'!OT9</f>
+        <v>37</v>
+      </c>
+      <c r="OU9">
+        <f>+'UCI OCUPADA TOTAL'!OU9-'UCI OCUPADA COVID'!OU9</f>
+        <v>43</v>
+      </c>
+      <c r="OV9">
+        <f>+'UCI OCUPADA TOTAL'!OV9-'UCI OCUPADA COVID'!OV9</f>
+        <v>47</v>
+      </c>
+      <c r="OW9">
+        <f>+'UCI OCUPADA TOTAL'!OW9-'UCI OCUPADA COVID'!OW9</f>
+        <v>35</v>
+      </c>
+      <c r="OX9">
+        <f>+'UCI OCUPADA TOTAL'!OX9-'UCI OCUPADA COVID'!OX9</f>
+        <v>39</v>
+      </c>
+      <c r="OY9">
+        <f>+'UCI OCUPADA TOTAL'!OY9-'UCI OCUPADA COVID'!OY9</f>
+        <v>36</v>
+      </c>
     </row>
-    <row r="10" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -87882,8 +89282,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR10-'UCI OCUPADA COVID'!OR10</f>
         <v>26</v>
       </c>
+      <c r="OS10">
+        <f>+'UCI OCUPADA TOTAL'!OS10-'UCI OCUPADA COVID'!OS10</f>
+        <v>26</v>
+      </c>
+      <c r="OT10">
+        <f>+'UCI OCUPADA TOTAL'!OT10-'UCI OCUPADA COVID'!OT10</f>
+        <v>25</v>
+      </c>
+      <c r="OU10">
+        <f>+'UCI OCUPADA TOTAL'!OU10-'UCI OCUPADA COVID'!OU10</f>
+        <v>27</v>
+      </c>
+      <c r="OV10">
+        <f>+'UCI OCUPADA TOTAL'!OV10-'UCI OCUPADA COVID'!OV10</f>
+        <v>26</v>
+      </c>
+      <c r="OW10">
+        <f>+'UCI OCUPADA TOTAL'!OW10-'UCI OCUPADA COVID'!OW10</f>
+        <v>25</v>
+      </c>
+      <c r="OX10">
+        <f>+'UCI OCUPADA TOTAL'!OX10-'UCI OCUPADA COVID'!OX10</f>
+        <v>26</v>
+      </c>
+      <c r="OY10">
+        <f>+'UCI OCUPADA TOTAL'!OY10-'UCI OCUPADA COVID'!OY10</f>
+        <v>26</v>
+      </c>
     </row>
-    <row r="11" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -89235,8 +90663,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR11-'UCI OCUPADA COVID'!OR11</f>
         <v>16</v>
       </c>
+      <c r="OS11">
+        <f>+'UCI OCUPADA TOTAL'!OS11-'UCI OCUPADA COVID'!OS11</f>
+        <v>14</v>
+      </c>
+      <c r="OT11">
+        <f>+'UCI OCUPADA TOTAL'!OT11-'UCI OCUPADA COVID'!OT11</f>
+        <v>14</v>
+      </c>
+      <c r="OU11">
+        <f>+'UCI OCUPADA TOTAL'!OU11-'UCI OCUPADA COVID'!OU11</f>
+        <v>16</v>
+      </c>
+      <c r="OV11">
+        <f>+'UCI OCUPADA TOTAL'!OV11-'UCI OCUPADA COVID'!OV11</f>
+        <v>13</v>
+      </c>
+      <c r="OW11">
+        <f>+'UCI OCUPADA TOTAL'!OW11-'UCI OCUPADA COVID'!OW11</f>
+        <v>11</v>
+      </c>
+      <c r="OX11">
+        <f>+'UCI OCUPADA TOTAL'!OX11-'UCI OCUPADA COVID'!OX11</f>
+        <v>16</v>
+      </c>
+      <c r="OY11">
+        <f>+'UCI OCUPADA TOTAL'!OY11-'UCI OCUPADA COVID'!OY11</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -90588,8 +92044,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR12-'UCI OCUPADA COVID'!OR12</f>
         <v>94</v>
       </c>
+      <c r="OS12">
+        <f>+'UCI OCUPADA TOTAL'!OS12-'UCI OCUPADA COVID'!OS12</f>
+        <v>99</v>
+      </c>
+      <c r="OT12">
+        <f>+'UCI OCUPADA TOTAL'!OT12-'UCI OCUPADA COVID'!OT12</f>
+        <v>100</v>
+      </c>
+      <c r="OU12">
+        <f>+'UCI OCUPADA TOTAL'!OU12-'UCI OCUPADA COVID'!OU12</f>
+        <v>95</v>
+      </c>
+      <c r="OV12">
+        <f>+'UCI OCUPADA TOTAL'!OV12-'UCI OCUPADA COVID'!OV12</f>
+        <v>95</v>
+      </c>
+      <c r="OW12">
+        <f>+'UCI OCUPADA TOTAL'!OW12-'UCI OCUPADA COVID'!OW12</f>
+        <v>99</v>
+      </c>
+      <c r="OX12">
+        <f>+'UCI OCUPADA TOTAL'!OX12-'UCI OCUPADA COVID'!OX12</f>
+        <v>96</v>
+      </c>
+      <c r="OY12">
+        <f>+'UCI OCUPADA TOTAL'!OY12-'UCI OCUPADA COVID'!OY12</f>
+        <v>93</v>
+      </c>
     </row>
-    <row r="13" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -91941,8 +93425,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR13-'UCI OCUPADA COVID'!OR13</f>
         <v>41</v>
       </c>
+      <c r="OS13">
+        <f>+'UCI OCUPADA TOTAL'!OS13-'UCI OCUPADA COVID'!OS13</f>
+        <v>39</v>
+      </c>
+      <c r="OT13">
+        <f>+'UCI OCUPADA TOTAL'!OT13-'UCI OCUPADA COVID'!OT13</f>
+        <v>37</v>
+      </c>
+      <c r="OU13">
+        <f>+'UCI OCUPADA TOTAL'!OU13-'UCI OCUPADA COVID'!OU13</f>
+        <v>40</v>
+      </c>
+      <c r="OV13">
+        <f>+'UCI OCUPADA TOTAL'!OV13-'UCI OCUPADA COVID'!OV13</f>
+        <v>38</v>
+      </c>
+      <c r="OW13">
+        <f>+'UCI OCUPADA TOTAL'!OW13-'UCI OCUPADA COVID'!OW13</f>
+        <v>36</v>
+      </c>
+      <c r="OX13">
+        <f>+'UCI OCUPADA TOTAL'!OX13-'UCI OCUPADA COVID'!OX13</f>
+        <v>35</v>
+      </c>
+      <c r="OY13">
+        <f>+'UCI OCUPADA TOTAL'!OY13-'UCI OCUPADA COVID'!OY13</f>
+        <v>36</v>
+      </c>
     </row>
-    <row r="14" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -93294,8 +94806,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR14-'UCI OCUPADA COVID'!OR14</f>
         <v>13</v>
       </c>
+      <c r="OS14">
+        <f>+'UCI OCUPADA TOTAL'!OS14-'UCI OCUPADA COVID'!OS14</f>
+        <v>15</v>
+      </c>
+      <c r="OT14">
+        <f>+'UCI OCUPADA TOTAL'!OT14-'UCI OCUPADA COVID'!OT14</f>
+        <v>14</v>
+      </c>
+      <c r="OU14">
+        <f>+'UCI OCUPADA TOTAL'!OU14-'UCI OCUPADA COVID'!OU14</f>
+        <v>12</v>
+      </c>
+      <c r="OV14">
+        <f>+'UCI OCUPADA TOTAL'!OV14-'UCI OCUPADA COVID'!OV14</f>
+        <v>12</v>
+      </c>
+      <c r="OW14">
+        <f>+'UCI OCUPADA TOTAL'!OW14-'UCI OCUPADA COVID'!OW14</f>
+        <v>11</v>
+      </c>
+      <c r="OX14">
+        <f>+'UCI OCUPADA TOTAL'!OX14-'UCI OCUPADA COVID'!OX14</f>
+        <v>10</v>
+      </c>
+      <c r="OY14">
+        <f>+'UCI OCUPADA TOTAL'!OY14-'UCI OCUPADA COVID'!OY14</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -94647,8 +96187,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR15-'UCI OCUPADA COVID'!OR15</f>
         <v>41</v>
       </c>
+      <c r="OS15">
+        <f>+'UCI OCUPADA TOTAL'!OS15-'UCI OCUPADA COVID'!OS15</f>
+        <v>39</v>
+      </c>
+      <c r="OT15">
+        <f>+'UCI OCUPADA TOTAL'!OT15-'UCI OCUPADA COVID'!OT15</f>
+        <v>38</v>
+      </c>
+      <c r="OU15">
+        <f>+'UCI OCUPADA TOTAL'!OU15-'UCI OCUPADA COVID'!OU15</f>
+        <v>33</v>
+      </c>
+      <c r="OV15">
+        <f>+'UCI OCUPADA TOTAL'!OV15-'UCI OCUPADA COVID'!OV15</f>
+        <v>34</v>
+      </c>
+      <c r="OW15">
+        <f>+'UCI OCUPADA TOTAL'!OW15-'UCI OCUPADA COVID'!OW15</f>
+        <v>35</v>
+      </c>
+      <c r="OX15">
+        <f>+'UCI OCUPADA TOTAL'!OX15-'UCI OCUPADA COVID'!OX15</f>
+        <v>33</v>
+      </c>
+      <c r="OY15">
+        <f>+'UCI OCUPADA TOTAL'!OY15-'UCI OCUPADA COVID'!OY15</f>
+        <v>35</v>
+      </c>
     </row>
-    <row r="16" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -96000,8 +97568,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR16-'UCI OCUPADA COVID'!OR16</f>
         <v>1</v>
       </c>
+      <c r="OS16">
+        <f>+'UCI OCUPADA TOTAL'!OS16-'UCI OCUPADA COVID'!OS16</f>
+        <v>0</v>
+      </c>
+      <c r="OT16">
+        <f>+'UCI OCUPADA TOTAL'!OT16-'UCI OCUPADA COVID'!OT16</f>
+        <v>0</v>
+      </c>
+      <c r="OU16">
+        <f>+'UCI OCUPADA TOTAL'!OU16-'UCI OCUPADA COVID'!OU16</f>
+        <v>0</v>
+      </c>
+      <c r="OV16">
+        <f>+'UCI OCUPADA TOTAL'!OV16-'UCI OCUPADA COVID'!OV16</f>
+        <v>0</v>
+      </c>
+      <c r="OW16">
+        <f>+'UCI OCUPADA TOTAL'!OW16-'UCI OCUPADA COVID'!OW16</f>
+        <v>0</v>
+      </c>
+      <c r="OX16">
+        <f>+'UCI OCUPADA TOTAL'!OX16-'UCI OCUPADA COVID'!OX16</f>
+        <v>0</v>
+      </c>
+      <c r="OY16">
+        <f>+'UCI OCUPADA TOTAL'!OY16-'UCI OCUPADA COVID'!OY16</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -97353,8 +98949,36 @@
         <f>+'UCI OCUPADA TOTAL'!OR17-'UCI OCUPADA COVID'!OR17</f>
         <v>10</v>
       </c>
+      <c r="OS17">
+        <f>+'UCI OCUPADA TOTAL'!OS17-'UCI OCUPADA COVID'!OS17</f>
+        <v>7</v>
+      </c>
+      <c r="OT17">
+        <f>+'UCI OCUPADA TOTAL'!OT17-'UCI OCUPADA COVID'!OT17</f>
+        <v>10</v>
+      </c>
+      <c r="OU17">
+        <f>+'UCI OCUPADA TOTAL'!OU17-'UCI OCUPADA COVID'!OU17</f>
+        <v>11</v>
+      </c>
+      <c r="OV17">
+        <f>+'UCI OCUPADA TOTAL'!OV17-'UCI OCUPADA COVID'!OV17</f>
+        <v>7</v>
+      </c>
+      <c r="OW17">
+        <f>+'UCI OCUPADA TOTAL'!OW17-'UCI OCUPADA COVID'!OW17</f>
+        <v>9</v>
+      </c>
+      <c r="OX17">
+        <f>+'UCI OCUPADA TOTAL'!OX17-'UCI OCUPADA COVID'!OX17</f>
+        <v>11</v>
+      </c>
+      <c r="OY17">
+        <f>+'UCI OCUPADA TOTAL'!OY17-'UCI OCUPADA COVID'!OY17</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="18" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -98706,48 +100330,76 @@
         <f>+'UCI OCUPADA TOTAL'!OR18-'UCI OCUPADA COVID'!OR18</f>
         <v>1228</v>
       </c>
+      <c r="OS18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OS18-'UCI OCUPADA COVID'!OS18</f>
+        <v>1206</v>
+      </c>
+      <c r="OT18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OT18-'UCI OCUPADA COVID'!OT18</f>
+        <v>1215</v>
+      </c>
+      <c r="OU18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OU18-'UCI OCUPADA COVID'!OU18</f>
+        <v>1184</v>
+      </c>
+      <c r="OV18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OV18-'UCI OCUPADA COVID'!OV18</f>
+        <v>1173</v>
+      </c>
+      <c r="OW18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OW18-'UCI OCUPADA COVID'!OW18</f>
+        <v>1139</v>
+      </c>
+      <c r="OX18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OX18-'UCI OCUPADA COVID'!OX18</f>
+        <v>1143</v>
+      </c>
+      <c r="OY18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OY18-'UCI OCUPADA COVID'!OY18</f>
+        <v>1110</v>
+      </c>
     </row>
-    <row r="19" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:408" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
balance diario, junio 9 2021
Signed-off-by: Demián Arancibia <dna33@cornell.edu>
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci.xlsx
+++ b/input/Camas_uci/last_uci.xlsx
@@ -2911,9 +2911,9 @@
   <dimension ref="A1:XFD20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OX1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
+      <selection pane="topRight" activeCell="PH7" sqref="PH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,7 +2935,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4181,8 +4181,29 @@
       <c r="OY1" s="8">
         <v>44348</v>
       </c>
+      <c r="OZ1" s="8">
+        <v>44349</v>
+      </c>
+      <c r="PA1" s="8">
+        <v>44350</v>
+      </c>
+      <c r="PB1" s="8">
+        <v>44351</v>
+      </c>
+      <c r="PC1" s="8">
+        <v>44352</v>
+      </c>
+      <c r="PD1" s="8">
+        <v>44353</v>
+      </c>
+      <c r="PE1" s="8">
+        <v>44354</v>
+      </c>
+      <c r="PF1" s="8">
+        <v>44355</v>
+      </c>
     </row>
-    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5428,8 +5449,29 @@
       <c r="OY2" s="11">
         <v>34</v>
       </c>
+      <c r="OZ2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PA2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PB2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PC2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PD2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PE2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PF2" s="11">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6675,8 +6717,29 @@
       <c r="OY3" s="11">
         <v>62</v>
       </c>
+      <c r="OZ3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PA3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PB3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PC3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PD3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PE3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PF3" s="11">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -7922,8 +7985,29 @@
       <c r="OY4" s="11">
         <v>166</v>
       </c>
+      <c r="OZ4" s="11">
+        <v>164</v>
+      </c>
+      <c r="PA4" s="11">
+        <v>165</v>
+      </c>
+      <c r="PB4" s="11">
+        <v>165</v>
+      </c>
+      <c r="PC4" s="11">
+        <v>166</v>
+      </c>
+      <c r="PD4" s="11">
+        <v>164</v>
+      </c>
+      <c r="PE4" s="11">
+        <v>166</v>
+      </c>
+      <c r="PF4" s="11">
+        <v>165</v>
+      </c>
     </row>
-    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -9169,8 +9253,29 @@
       <c r="OY5" s="11">
         <v>34</v>
       </c>
+      <c r="OZ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PA5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PB5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PC5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PD5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PE5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PF5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10416,8 +10521,29 @@
       <c r="OY6" s="11">
         <v>132</v>
       </c>
+      <c r="OZ6" s="11">
+        <v>132</v>
+      </c>
+      <c r="PA6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PB6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PC6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PD6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PE6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PF6" s="11">
+        <v>135</v>
+      </c>
     </row>
-    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -11663,8 +11789,29 @@
       <c r="OY7" s="11">
         <v>332</v>
       </c>
+      <c r="OZ7" s="11">
+        <v>333</v>
+      </c>
+      <c r="PA7" s="11">
+        <v>333</v>
+      </c>
+      <c r="PB7" s="11">
+        <v>333</v>
+      </c>
+      <c r="PC7" s="11">
+        <v>332</v>
+      </c>
+      <c r="PD7" s="11">
+        <v>332</v>
+      </c>
+      <c r="PE7" s="11">
+        <v>330</v>
+      </c>
+      <c r="PF7" s="11">
+        <v>330</v>
+      </c>
     </row>
-    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -12910,8 +13057,29 @@
       <c r="OY8" s="11">
         <v>2571</v>
       </c>
+      <c r="OZ8" s="11">
+        <v>2574</v>
+      </c>
+      <c r="PA8" s="11">
+        <v>2579</v>
+      </c>
+      <c r="PB8" s="11">
+        <v>2584</v>
+      </c>
+      <c r="PC8" s="11">
+        <v>2584</v>
+      </c>
+      <c r="PD8" s="11">
+        <v>2597</v>
+      </c>
+      <c r="PE8" s="11">
+        <v>2596</v>
+      </c>
+      <c r="PF8" s="11">
+        <v>2599</v>
+      </c>
     </row>
-    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -14157,8 +14325,29 @@
       <c r="OY9" s="11">
         <v>206</v>
       </c>
+      <c r="OZ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PA9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PB9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PC9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PD9" s="11">
+        <v>205</v>
+      </c>
+      <c r="PE9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PF9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -15404,8 +15593,29 @@
       <c r="OY10" s="11">
         <v>157</v>
       </c>
+      <c r="OZ10" s="11">
+        <v>157</v>
+      </c>
+      <c r="PA10" s="11">
+        <v>156</v>
+      </c>
+      <c r="PB10" s="11">
+        <v>155</v>
+      </c>
+      <c r="PC10" s="11">
+        <v>156</v>
+      </c>
+      <c r="PD10" s="11">
+        <v>156</v>
+      </c>
+      <c r="PE10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PF10" s="11">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -16651,8 +16861,29 @@
       <c r="OY11" s="11">
         <v>73</v>
       </c>
+      <c r="OZ11" s="11">
+        <v>73</v>
+      </c>
+      <c r="PA11" s="11">
+        <v>73</v>
+      </c>
+      <c r="PB11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PC11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PD11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PE11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PF11" s="11">
+        <v>70</v>
+      </c>
     </row>
-    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -17898,8 +18129,29 @@
       <c r="OY12" s="11">
         <v>310</v>
       </c>
+      <c r="OZ12" s="11">
+        <v>309</v>
+      </c>
+      <c r="PA12" s="11">
+        <v>309</v>
+      </c>
+      <c r="PB12" s="11">
+        <v>309</v>
+      </c>
+      <c r="PC12" s="11">
+        <v>309</v>
+      </c>
+      <c r="PD12" s="11">
+        <v>310</v>
+      </c>
+      <c r="PE12" s="11">
+        <v>310</v>
+      </c>
+      <c r="PF12" s="11">
+        <v>310</v>
+      </c>
     </row>
-    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -19145,8 +19397,29 @@
       <c r="OY13" s="11">
         <v>150</v>
       </c>
+      <c r="OZ13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PA13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PB13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PC13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PD13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PE13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PF13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -20392,8 +20665,29 @@
       <c r="OY14" s="11">
         <v>41</v>
       </c>
+      <c r="OZ14" s="11">
+        <v>41</v>
+      </c>
+      <c r="PA14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PB14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PC14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PD14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PE14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PF14" s="11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -21639,8 +21933,29 @@
       <c r="OY15" s="11">
         <v>129</v>
       </c>
+      <c r="OZ15" s="11">
+        <v>130</v>
+      </c>
+      <c r="PA15" s="11">
+        <v>130</v>
+      </c>
+      <c r="PB15" s="11">
+        <v>132</v>
+      </c>
+      <c r="PC15" s="11">
+        <v>132</v>
+      </c>
+      <c r="PD15" s="11">
+        <v>132</v>
+      </c>
+      <c r="PE15" s="11">
+        <v>132</v>
+      </c>
+      <c r="PF15" s="11">
+        <v>134</v>
+      </c>
     </row>
-    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -22886,8 +23201,29 @@
       <c r="OY16" s="11">
         <v>10</v>
       </c>
+      <c r="OZ16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PA16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PB16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PC16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PD16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PE16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PF16" s="11">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:422 16384:16384" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -24133,8 +24469,29 @@
       <c r="OY17" s="11">
         <v>43</v>
       </c>
+      <c r="OZ17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PA17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PB17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PC17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PD17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PE17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PF17" s="11">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:422 16384:16384" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -25310,7 +25667,7 @@
         <v>4103</v>
       </c>
       <c r="MY18" s="6">
-        <f t="shared" ref="MY18:OY18" si="7">SUM(MY2:MY17)</f>
+        <f t="shared" ref="MY18:PF18" si="7">SUM(MY2:MY17)</f>
         <v>4123</v>
       </c>
       <c r="MZ18" s="6">
@@ -25521,9 +25878,37 @@
         <f t="shared" si="7"/>
         <v>4450</v>
       </c>
+      <c r="OZ18" s="6">
+        <f t="shared" si="7"/>
+        <v>4458</v>
+      </c>
+      <c r="PA18" s="6">
+        <f t="shared" si="7"/>
+        <v>4469</v>
+      </c>
+      <c r="PB18" s="6">
+        <f t="shared" si="7"/>
+        <v>4472</v>
+      </c>
+      <c r="PC18" s="6">
+        <f t="shared" si="7"/>
+        <v>4473</v>
+      </c>
+      <c r="PD18" s="6">
+        <f t="shared" si="7"/>
+        <v>4484</v>
+      </c>
+      <c r="PE18" s="6">
+        <f t="shared" si="7"/>
+        <v>4486</v>
+      </c>
+      <c r="PF18" s="6">
+        <f t="shared" si="7"/>
+        <v>4490</v>
+      </c>
       <c r="XFD18" s="6"/>
     </row>
-    <row r="20" spans="1:415 16384:16384" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:422 16384:16384" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -25541,12 +25926,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OY36"/>
+  <dimension ref="A1:PF36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OX1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
+      <selection pane="topRight" activeCell="PI23" sqref="PI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25566,7 +25951,7 @@
     <col min="261" max="273" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -26812,8 +27197,29 @@
       <c r="OY1" s="8">
         <v>44348</v>
       </c>
+      <c r="OZ1" s="8">
+        <v>44349</v>
+      </c>
+      <c r="PA1" s="8">
+        <v>44350</v>
+      </c>
+      <c r="PB1" s="8">
+        <v>44351</v>
+      </c>
+      <c r="PC1" s="8">
+        <v>44352</v>
+      </c>
+      <c r="PD1" s="8">
+        <v>44353</v>
+      </c>
+      <c r="PE1" s="8">
+        <v>44354</v>
+      </c>
+      <c r="PF1" s="8">
+        <v>44355</v>
+      </c>
     </row>
-    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -28059,8 +28465,29 @@
       <c r="OY2">
         <v>28</v>
       </c>
+      <c r="OZ2">
+        <v>30</v>
+      </c>
+      <c r="PA2">
+        <v>31</v>
+      </c>
+      <c r="PB2">
+        <v>31</v>
+      </c>
+      <c r="PC2">
+        <v>30</v>
+      </c>
+      <c r="PD2">
+        <v>30</v>
+      </c>
+      <c r="PE2">
+        <v>31</v>
+      </c>
+      <c r="PF2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -29306,8 +29733,29 @@
       <c r="OY3">
         <v>61</v>
       </c>
+      <c r="OZ3">
+        <v>61</v>
+      </c>
+      <c r="PA3">
+        <v>58</v>
+      </c>
+      <c r="PB3">
+        <v>60</v>
+      </c>
+      <c r="PC3">
+        <v>60</v>
+      </c>
+      <c r="PD3">
+        <v>60</v>
+      </c>
+      <c r="PE3">
+        <v>62</v>
+      </c>
+      <c r="PF3">
+        <v>59</v>
+      </c>
     </row>
-    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -30553,8 +31001,29 @@
       <c r="OY4">
         <v>153</v>
       </c>
+      <c r="OZ4">
+        <v>158</v>
+      </c>
+      <c r="PA4">
+        <v>152</v>
+      </c>
+      <c r="PB4">
+        <v>151</v>
+      </c>
+      <c r="PC4">
+        <v>151</v>
+      </c>
+      <c r="PD4">
+        <v>148</v>
+      </c>
+      <c r="PE4">
+        <v>149</v>
+      </c>
+      <c r="PF4">
+        <v>156</v>
+      </c>
     </row>
-    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -31800,8 +32269,29 @@
       <c r="OY5">
         <v>30</v>
       </c>
+      <c r="OZ5">
+        <v>31</v>
+      </c>
+      <c r="PA5">
+        <v>30</v>
+      </c>
+      <c r="PB5">
+        <v>29</v>
+      </c>
+      <c r="PC5">
+        <v>29</v>
+      </c>
+      <c r="PD5">
+        <v>29</v>
+      </c>
+      <c r="PE5">
+        <v>29</v>
+      </c>
+      <c r="PF5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -33047,8 +33537,29 @@
       <c r="OY6">
         <v>130</v>
       </c>
+      <c r="OZ6">
+        <v>130</v>
+      </c>
+      <c r="PA6">
+        <v>130</v>
+      </c>
+      <c r="PB6">
+        <v>133</v>
+      </c>
+      <c r="PC6">
+        <v>135</v>
+      </c>
+      <c r="PD6">
+        <v>133</v>
+      </c>
+      <c r="PE6">
+        <v>129</v>
+      </c>
+      <c r="PF6">
+        <v>132</v>
+      </c>
     </row>
-    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -34294,8 +34805,29 @@
       <c r="OY7">
         <v>323</v>
       </c>
+      <c r="OZ7">
+        <v>323</v>
+      </c>
+      <c r="PA7">
+        <v>327</v>
+      </c>
+      <c r="PB7">
+        <v>326</v>
+      </c>
+      <c r="PC7">
+        <v>321</v>
+      </c>
+      <c r="PD7">
+        <v>315</v>
+      </c>
+      <c r="PE7">
+        <v>315</v>
+      </c>
+      <c r="PF7">
+        <v>316</v>
+      </c>
     </row>
-    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -35541,8 +36073,29 @@
       <c r="OY8">
         <v>2536</v>
       </c>
+      <c r="OZ8">
+        <v>2539</v>
+      </c>
+      <c r="PA8">
+        <v>2543</v>
+      </c>
+      <c r="PB8">
+        <v>2547</v>
+      </c>
+      <c r="PC8">
+        <v>2554</v>
+      </c>
+      <c r="PD8">
+        <v>2565</v>
+      </c>
+      <c r="PE8">
+        <v>2557</v>
+      </c>
+      <c r="PF8">
+        <v>2569</v>
+      </c>
     </row>
-    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -36788,8 +37341,29 @@
       <c r="OY9">
         <v>191</v>
       </c>
+      <c r="OZ9">
+        <v>185</v>
+      </c>
+      <c r="PA9">
+        <v>185</v>
+      </c>
+      <c r="PB9">
+        <v>184</v>
+      </c>
+      <c r="PC9">
+        <v>182</v>
+      </c>
+      <c r="PD9">
+        <v>186</v>
+      </c>
+      <c r="PE9">
+        <v>198</v>
+      </c>
+      <c r="PF9">
+        <v>193</v>
+      </c>
     </row>
-    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -38035,8 +38609,29 @@
       <c r="OY10">
         <v>137</v>
       </c>
+      <c r="OZ10">
+        <v>138</v>
+      </c>
+      <c r="PA10">
+        <v>139</v>
+      </c>
+      <c r="PB10">
+        <v>138</v>
+      </c>
+      <c r="PC10">
+        <v>132</v>
+      </c>
+      <c r="PD10">
+        <v>133</v>
+      </c>
+      <c r="PE10">
+        <v>136</v>
+      </c>
+      <c r="PF10">
+        <v>133</v>
+      </c>
     </row>
-    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -39282,8 +39877,29 @@
       <c r="OY11">
         <v>68</v>
       </c>
+      <c r="OZ11">
+        <v>71</v>
+      </c>
+      <c r="PA11">
+        <v>69</v>
+      </c>
+      <c r="PB11">
+        <v>65</v>
+      </c>
+      <c r="PC11">
+        <v>61</v>
+      </c>
+      <c r="PD11">
+        <v>62</v>
+      </c>
+      <c r="PE11">
+        <v>64</v>
+      </c>
+      <c r="PF11">
+        <v>63</v>
+      </c>
     </row>
-    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -40529,8 +41145,29 @@
       <c r="OY12">
         <v>289</v>
       </c>
+      <c r="OZ12">
+        <v>289</v>
+      </c>
+      <c r="PA12">
+        <v>293</v>
+      </c>
+      <c r="PB12">
+        <v>290</v>
+      </c>
+      <c r="PC12">
+        <v>291</v>
+      </c>
+      <c r="PD12">
+        <v>287</v>
+      </c>
+      <c r="PE12">
+        <v>288</v>
+      </c>
+      <c r="PF12">
+        <v>293</v>
+      </c>
     </row>
-    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -41776,8 +42413,29 @@
       <c r="OY13">
         <v>141</v>
       </c>
+      <c r="OZ13">
+        <v>141</v>
+      </c>
+      <c r="PA13">
+        <v>144</v>
+      </c>
+      <c r="PB13">
+        <v>141</v>
+      </c>
+      <c r="PC13">
+        <v>146</v>
+      </c>
+      <c r="PD13">
+        <v>145</v>
+      </c>
+      <c r="PE13">
+        <v>141</v>
+      </c>
+      <c r="PF13">
+        <v>146</v>
+      </c>
     </row>
-    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -43023,8 +43681,29 @@
       <c r="OY14">
         <v>40</v>
       </c>
+      <c r="OZ14">
+        <v>40</v>
+      </c>
+      <c r="PA14">
+        <v>37</v>
+      </c>
+      <c r="PB14">
+        <v>41</v>
+      </c>
+      <c r="PC14">
+        <v>39</v>
+      </c>
+      <c r="PD14">
+        <v>41</v>
+      </c>
+      <c r="PE14">
+        <v>40</v>
+      </c>
+      <c r="PF14">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -44270,8 +44949,29 @@
       <c r="OY15">
         <v>127</v>
       </c>
+      <c r="OZ15">
+        <v>123</v>
+      </c>
+      <c r="PA15">
+        <v>128</v>
+      </c>
+      <c r="PB15">
+        <v>130</v>
+      </c>
+      <c r="PC15">
+        <v>126</v>
+      </c>
+      <c r="PD15">
+        <v>127</v>
+      </c>
+      <c r="PE15">
+        <v>127</v>
+      </c>
+      <c r="PF15">
+        <v>132</v>
+      </c>
     </row>
-    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -45517,8 +46217,29 @@
       <c r="OY16">
         <v>10</v>
       </c>
+      <c r="OZ16">
+        <v>13</v>
+      </c>
+      <c r="PA16">
+        <v>13</v>
+      </c>
+      <c r="PB16">
+        <v>11</v>
+      </c>
+      <c r="PC16">
+        <v>12</v>
+      </c>
+      <c r="PD16">
+        <v>11</v>
+      </c>
+      <c r="PE16">
+        <v>13</v>
+      </c>
+      <c r="PF16">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -46764,8 +47485,29 @@
       <c r="OY17">
         <v>39</v>
       </c>
+      <c r="OZ17">
+        <v>40</v>
+      </c>
+      <c r="PA17">
+        <v>41</v>
+      </c>
+      <c r="PB17">
+        <v>38</v>
+      </c>
+      <c r="PC17">
+        <v>37</v>
+      </c>
+      <c r="PD17">
+        <v>36</v>
+      </c>
+      <c r="PE17">
+        <v>41</v>
+      </c>
+      <c r="PF17">
+        <v>40</v>
+      </c>
     </row>
-    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -48113,7 +48855,7 @@
         <v>4229</v>
       </c>
       <c r="OU18" s="6">
-        <f t="shared" ref="OU18:OY18" si="2">SUM(OU2:OU17)</f>
+        <f t="shared" ref="OU18:PF18" si="2">SUM(OU2:OU17)</f>
         <v>4251</v>
       </c>
       <c r="OV18" s="6">
@@ -48132,8 +48874,36 @@
         <f t="shared" si="2"/>
         <v>4303</v>
       </c>
+      <c r="OZ18" s="6">
+        <f t="shared" si="2"/>
+        <v>4312</v>
+      </c>
+      <c r="PA18" s="6">
+        <f t="shared" si="2"/>
+        <v>4320</v>
+      </c>
+      <c r="PB18" s="6">
+        <f t="shared" si="2"/>
+        <v>4315</v>
+      </c>
+      <c r="PC18" s="6">
+        <f t="shared" si="2"/>
+        <v>4306</v>
+      </c>
+      <c r="PD18" s="6">
+        <f t="shared" si="2"/>
+        <v>4308</v>
+      </c>
+      <c r="PE18" s="6">
+        <f t="shared" si="2"/>
+        <v>4320</v>
+      </c>
+      <c r="PF18" s="6">
+        <f t="shared" si="2"/>
+        <v>4345</v>
+      </c>
     </row>
-    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -48416,7 +49186,7 @@
       <c r="JT20" s="9"/>
       <c r="JU20" s="9"/>
     </row>
-    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -48699,7 +49469,7 @@
       <c r="JT21" s="9"/>
       <c r="JU21" s="9"/>
     </row>
-    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -48982,7 +49752,7 @@
       <c r="JT22" s="9"/>
       <c r="JU22" s="9"/>
     </row>
-    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -49265,7 +50035,7 @@
       <c r="JT23" s="9"/>
       <c r="JU23" s="9"/>
     </row>
-    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -49548,7 +50318,7 @@
       <c r="JT24" s="9"/>
       <c r="JU24" s="9"/>
     </row>
-    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -49831,7 +50601,7 @@
       <c r="JT25" s="9"/>
       <c r="JU25" s="9"/>
     </row>
-    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -50114,7 +50884,7 @@
       <c r="JT26" s="9"/>
       <c r="JU26" s="9"/>
     </row>
-    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -50397,7 +51167,7 @@
       <c r="JT27" s="9"/>
       <c r="JU27" s="9"/>
     </row>
-    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -50680,7 +51450,7 @@
       <c r="JT28" s="9"/>
       <c r="JU28" s="9"/>
     </row>
-    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -50963,7 +51733,7 @@
       <c r="JT29" s="9"/>
       <c r="JU29" s="9"/>
     </row>
-    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -51246,7 +52016,7 @@
       <c r="JT30" s="9"/>
       <c r="JU30" s="9"/>
     </row>
-    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -51529,7 +52299,7 @@
       <c r="JT31" s="9"/>
       <c r="JU31" s="9"/>
     </row>
-    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -52952,12 +53722,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:OY34"/>
+  <dimension ref="A1:PF34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OY1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="OY2" sqref="OY2:OY17"/>
+      <selection pane="topRight" activeCell="PF2" sqref="PF2:PF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52978,7 +53748,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -54224,8 +54994,29 @@
       <c r="OY1" s="8">
         <v>44348</v>
       </c>
+      <c r="OZ1" s="8">
+        <v>44349</v>
+      </c>
+      <c r="PA1" s="8">
+        <v>44350</v>
+      </c>
+      <c r="PB1" s="8">
+        <v>44351</v>
+      </c>
+      <c r="PC1" s="8">
+        <v>44352</v>
+      </c>
+      <c r="PD1" s="8">
+        <v>44353</v>
+      </c>
+      <c r="PE1" s="8">
+        <v>44354</v>
+      </c>
+      <c r="PF1" s="8">
+        <v>44355</v>
+      </c>
     </row>
-    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -55471,8 +56262,29 @@
       <c r="OY2">
         <v>25</v>
       </c>
+      <c r="OZ2">
+        <v>25</v>
+      </c>
+      <c r="PA2">
+        <v>26</v>
+      </c>
+      <c r="PB2">
+        <v>26</v>
+      </c>
+      <c r="PC2">
+        <v>25</v>
+      </c>
+      <c r="PD2">
+        <v>24</v>
+      </c>
+      <c r="PE2">
+        <v>24</v>
+      </c>
+      <c r="PF2">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -56718,8 +57530,29 @@
       <c r="OY3">
         <v>55</v>
       </c>
+      <c r="OZ3">
+        <v>55</v>
+      </c>
+      <c r="PA3">
+        <v>52</v>
+      </c>
+      <c r="PB3">
+        <v>55</v>
+      </c>
+      <c r="PC3">
+        <v>54</v>
+      </c>
+      <c r="PD3">
+        <v>54</v>
+      </c>
+      <c r="PE3">
+        <v>56</v>
+      </c>
+      <c r="PF3">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -57965,8 +58798,29 @@
       <c r="OY4">
         <v>90</v>
       </c>
+      <c r="OZ4">
+        <v>88</v>
+      </c>
+      <c r="PA4">
+        <v>92</v>
+      </c>
+      <c r="PB4">
+        <v>86</v>
+      </c>
+      <c r="PC4">
+        <v>87</v>
+      </c>
+      <c r="PD4">
+        <v>85</v>
+      </c>
+      <c r="PE4">
+        <v>84</v>
+      </c>
+      <c r="PF4">
+        <v>84</v>
+      </c>
     </row>
-    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -59212,8 +60066,29 @@
       <c r="OY5">
         <v>23</v>
       </c>
+      <c r="OZ5">
+        <v>22</v>
+      </c>
+      <c r="PA5">
+        <v>22</v>
+      </c>
+      <c r="PB5">
+        <v>20</v>
+      </c>
+      <c r="PC5">
+        <v>20</v>
+      </c>
+      <c r="PD5">
+        <v>19</v>
+      </c>
+      <c r="PE5">
+        <v>20</v>
+      </c>
+      <c r="PF5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -60459,8 +61334,29 @@
       <c r="OY6">
         <v>95</v>
       </c>
+      <c r="OZ6">
+        <v>96</v>
+      </c>
+      <c r="PA6">
+        <v>98</v>
+      </c>
+      <c r="PB6">
+        <v>100</v>
+      </c>
+      <c r="PC6">
+        <v>101</v>
+      </c>
+      <c r="PD6">
+        <v>104</v>
+      </c>
+      <c r="PE6">
+        <v>103</v>
+      </c>
+      <c r="PF6">
+        <v>104</v>
+      </c>
     </row>
-    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -61706,8 +62602,29 @@
       <c r="OY7">
         <v>217</v>
       </c>
+      <c r="OZ7">
+        <v>214</v>
+      </c>
+      <c r="PA7">
+        <v>217</v>
+      </c>
+      <c r="PB7">
+        <v>216</v>
+      </c>
+      <c r="PC7">
+        <v>212</v>
+      </c>
+      <c r="PD7">
+        <v>212</v>
+      </c>
+      <c r="PE7">
+        <v>211</v>
+      </c>
+      <c r="PF7">
+        <v>213</v>
+      </c>
     </row>
-    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -62953,8 +63870,29 @@
       <c r="OY8">
         <v>1908</v>
       </c>
+      <c r="OZ8">
+        <v>1886</v>
+      </c>
+      <c r="PA8">
+        <v>1930</v>
+      </c>
+      <c r="PB8">
+        <v>1936</v>
+      </c>
+      <c r="PC8">
+        <v>1934</v>
+      </c>
+      <c r="PD8">
+        <v>1957</v>
+      </c>
+      <c r="PE8">
+        <v>1966</v>
+      </c>
+      <c r="PF8">
+        <v>1971</v>
+      </c>
     </row>
-    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -64200,8 +65138,29 @@
       <c r="OY9">
         <v>155</v>
       </c>
+      <c r="OZ9">
+        <v>151</v>
+      </c>
+      <c r="PA9">
+        <v>151</v>
+      </c>
+      <c r="PB9">
+        <v>149</v>
+      </c>
+      <c r="PC9">
+        <v>153</v>
+      </c>
+      <c r="PD9">
+        <v>153</v>
+      </c>
+      <c r="PE9">
+        <v>151</v>
+      </c>
+      <c r="PF9">
+        <v>156</v>
+      </c>
     </row>
-    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -65447,8 +66406,29 @@
       <c r="OY10">
         <v>111</v>
       </c>
+      <c r="OZ10">
+        <v>110</v>
+      </c>
+      <c r="PA10">
+        <v>109</v>
+      </c>
+      <c r="PB10">
+        <v>108</v>
+      </c>
+      <c r="PC10">
+        <v>109</v>
+      </c>
+      <c r="PD10">
+        <v>110</v>
+      </c>
+      <c r="PE10">
+        <v>111</v>
+      </c>
+      <c r="PF10">
+        <v>110</v>
+      </c>
     </row>
-    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -66694,8 +67674,29 @@
       <c r="OY11">
         <v>52</v>
       </c>
+      <c r="OZ11">
+        <v>54</v>
+      </c>
+      <c r="PA11">
+        <v>53</v>
+      </c>
+      <c r="PB11">
+        <v>48</v>
+      </c>
+      <c r="PC11">
+        <v>46</v>
+      </c>
+      <c r="PD11">
+        <v>46</v>
+      </c>
+      <c r="PE11">
+        <v>47</v>
+      </c>
+      <c r="PF11">
+        <v>45</v>
+      </c>
     </row>
-    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -67941,8 +68942,29 @@
       <c r="OY12">
         <v>196</v>
       </c>
+      <c r="OZ12">
+        <v>194</v>
+      </c>
+      <c r="PA12">
+        <v>192</v>
+      </c>
+      <c r="PB12">
+        <v>193</v>
+      </c>
+      <c r="PC12">
+        <v>194</v>
+      </c>
+      <c r="PD12">
+        <v>189</v>
+      </c>
+      <c r="PE12">
+        <v>194</v>
+      </c>
+      <c r="PF12">
+        <v>198</v>
+      </c>
     </row>
-    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -69188,8 +70210,29 @@
       <c r="OY13">
         <v>105</v>
       </c>
+      <c r="OZ13">
+        <v>105</v>
+      </c>
+      <c r="PA13">
+        <v>107</v>
+      </c>
+      <c r="PB13">
+        <v>107</v>
+      </c>
+      <c r="PC13">
+        <v>108</v>
+      </c>
+      <c r="PD13">
+        <v>117</v>
+      </c>
+      <c r="PE13">
+        <v>109</v>
+      </c>
+      <c r="PF13">
+        <v>109</v>
+      </c>
     </row>
-    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -70435,8 +71478,29 @@
       <c r="OY14">
         <v>30</v>
       </c>
+      <c r="OZ14">
+        <v>31</v>
+      </c>
+      <c r="PA14">
+        <v>27</v>
+      </c>
+      <c r="PB14">
+        <v>30</v>
+      </c>
+      <c r="PC14">
+        <v>29</v>
+      </c>
+      <c r="PD14">
+        <v>31</v>
+      </c>
+      <c r="PE14">
+        <v>31</v>
+      </c>
+      <c r="PF14">
+        <v>33</v>
+      </c>
     </row>
-    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -71682,8 +72746,29 @@
       <c r="OY15">
         <v>92</v>
       </c>
+      <c r="OZ15">
+        <v>98</v>
+      </c>
+      <c r="PA15">
+        <v>102</v>
+      </c>
+      <c r="PB15">
+        <v>103</v>
+      </c>
+      <c r="PC15">
+        <v>103</v>
+      </c>
+      <c r="PD15">
+        <v>102</v>
+      </c>
+      <c r="PE15">
+        <v>102</v>
+      </c>
+      <c r="PF15">
+        <v>107</v>
+      </c>
     </row>
-    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -72929,8 +74014,29 @@
       <c r="OY16">
         <v>10</v>
       </c>
+      <c r="OZ16">
+        <v>13</v>
+      </c>
+      <c r="PA16">
+        <v>12</v>
+      </c>
+      <c r="PB16">
+        <v>10</v>
+      </c>
+      <c r="PC16">
+        <v>11</v>
+      </c>
+      <c r="PD16">
+        <v>11</v>
+      </c>
+      <c r="PE16">
+        <v>10</v>
+      </c>
+      <c r="PF16">
+        <v>11</v>
+      </c>
     </row>
-    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -74176,8 +75282,29 @@
       <c r="OY17">
         <v>29</v>
       </c>
+      <c r="OZ17">
+        <v>28</v>
+      </c>
+      <c r="PA17">
+        <v>29</v>
+      </c>
+      <c r="PB17">
+        <v>29</v>
+      </c>
+      <c r="PC17">
+        <v>27</v>
+      </c>
+      <c r="PD17">
+        <v>28</v>
+      </c>
+      <c r="PE17">
+        <v>28</v>
+      </c>
+      <c r="PF17">
+        <v>28</v>
+      </c>
     </row>
-    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -75314,7 +76441,7 @@
         <v>2867</v>
       </c>
       <c r="MS18" s="6">
-        <f t="shared" ref="MS18:OY18" si="1">SUM(MS2:MS17)</f>
+        <f t="shared" ref="MS18:PD18" si="1">SUM(MS2:MS17)</f>
         <v>2884</v>
       </c>
       <c r="MT18" s="6">
@@ -75549,50 +76676,78 @@
         <f t="shared" si="1"/>
         <v>3193</v>
       </c>
+      <c r="OZ18" s="6">
+        <f t="shared" si="1"/>
+        <v>3170</v>
+      </c>
+      <c r="PA18" s="6">
+        <f t="shared" si="1"/>
+        <v>3219</v>
+      </c>
+      <c r="PB18" s="6">
+        <f t="shared" si="1"/>
+        <v>3216</v>
+      </c>
+      <c r="PC18" s="6">
+        <f t="shared" si="1"/>
+        <v>3213</v>
+      </c>
+      <c r="PD18" s="6">
+        <f t="shared" si="1"/>
+        <v>3242</v>
+      </c>
+      <c r="PE18" s="6">
+        <f t="shared" ref="PE18:PF18" si="2">SUM(PE2:PE17)</f>
+        <v>3247</v>
+      </c>
+      <c r="PF18" s="6">
+        <f t="shared" si="2"/>
+        <v>3265</v>
+      </c>
     </row>
-    <row r="19" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:422" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:422" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:422" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -75612,12 +76767,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:OY34"/>
+  <dimension ref="A1:PF34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OR1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="OV1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="PA20" sqref="PA20"/>
+      <selection pane="topRight" activeCell="PF21" sqref="PF21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75635,7 +76790,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -76881,8 +78036,29 @@
       <c r="OY1" s="8">
         <v>44348</v>
       </c>
+      <c r="OZ1" s="8">
+        <v>44349</v>
+      </c>
+      <c r="PA1" s="8">
+        <v>44350</v>
+      </c>
+      <c r="PB1" s="8">
+        <v>44351</v>
+      </c>
+      <c r="PC1" s="8">
+        <v>44352</v>
+      </c>
+      <c r="PD1" s="8">
+        <v>44353</v>
+      </c>
+      <c r="PE1" s="8">
+        <v>44354</v>
+      </c>
+      <c r="PF1" s="8">
+        <v>44355</v>
+      </c>
     </row>
-    <row r="2" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -78262,8 +79438,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY2-'UCI OCUPADA COVID'!OY2</f>
         <v>3</v>
       </c>
+      <c r="OZ2">
+        <f>+'UCI OCUPADA TOTAL'!OZ2-'UCI OCUPADA COVID'!OZ2</f>
+        <v>5</v>
+      </c>
+      <c r="PA2">
+        <f>+'UCI OCUPADA TOTAL'!PA2-'UCI OCUPADA COVID'!PA2</f>
+        <v>5</v>
+      </c>
+      <c r="PB2">
+        <f>+'UCI OCUPADA TOTAL'!PB2-'UCI OCUPADA COVID'!PB2</f>
+        <v>5</v>
+      </c>
+      <c r="PC2">
+        <f>+'UCI OCUPADA TOTAL'!PC2-'UCI OCUPADA COVID'!PC2</f>
+        <v>5</v>
+      </c>
+      <c r="PD2">
+        <f>+'UCI OCUPADA TOTAL'!PD2-'UCI OCUPADA COVID'!PD2</f>
+        <v>6</v>
+      </c>
+      <c r="PE2">
+        <f>+'UCI OCUPADA TOTAL'!PE2-'UCI OCUPADA COVID'!PE2</f>
+        <v>7</v>
+      </c>
+      <c r="PF2">
+        <f>+'UCI OCUPADA TOTAL'!PF2-'UCI OCUPADA COVID'!PF2</f>
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -79643,8 +80847,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY3-'UCI OCUPADA COVID'!OY3</f>
         <v>6</v>
       </c>
+      <c r="OZ3">
+        <f>+'UCI OCUPADA TOTAL'!OZ3-'UCI OCUPADA COVID'!OZ3</f>
+        <v>6</v>
+      </c>
+      <c r="PA3">
+        <f>+'UCI OCUPADA TOTAL'!PA3-'UCI OCUPADA COVID'!PA3</f>
+        <v>6</v>
+      </c>
+      <c r="PB3">
+        <f>+'UCI OCUPADA TOTAL'!PB3-'UCI OCUPADA COVID'!PB3</f>
+        <v>5</v>
+      </c>
+      <c r="PC3">
+        <f>+'UCI OCUPADA TOTAL'!PC3-'UCI OCUPADA COVID'!PC3</f>
+        <v>6</v>
+      </c>
+      <c r="PD3">
+        <f>+'UCI OCUPADA TOTAL'!PD3-'UCI OCUPADA COVID'!PD3</f>
+        <v>6</v>
+      </c>
+      <c r="PE3">
+        <f>+'UCI OCUPADA TOTAL'!PE3-'UCI OCUPADA COVID'!PE3</f>
+        <v>6</v>
+      </c>
+      <c r="PF3">
+        <f>+'UCI OCUPADA TOTAL'!PF3-'UCI OCUPADA COVID'!PF3</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -81024,8 +82256,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY4-'UCI OCUPADA COVID'!OY4</f>
         <v>63</v>
       </c>
+      <c r="OZ4">
+        <f>+'UCI OCUPADA TOTAL'!OZ4-'UCI OCUPADA COVID'!OZ4</f>
+        <v>70</v>
+      </c>
+      <c r="PA4">
+        <f>+'UCI OCUPADA TOTAL'!PA4-'UCI OCUPADA COVID'!PA4</f>
+        <v>60</v>
+      </c>
+      <c r="PB4">
+        <f>+'UCI OCUPADA TOTAL'!PB4-'UCI OCUPADA COVID'!PB4</f>
+        <v>65</v>
+      </c>
+      <c r="PC4">
+        <f>+'UCI OCUPADA TOTAL'!PC4-'UCI OCUPADA COVID'!PC4</f>
+        <v>64</v>
+      </c>
+      <c r="PD4">
+        <f>+'UCI OCUPADA TOTAL'!PD4-'UCI OCUPADA COVID'!PD4</f>
+        <v>63</v>
+      </c>
+      <c r="PE4">
+        <f>+'UCI OCUPADA TOTAL'!PE4-'UCI OCUPADA COVID'!PE4</f>
+        <v>65</v>
+      </c>
+      <c r="PF4">
+        <f>+'UCI OCUPADA TOTAL'!PF4-'UCI OCUPADA COVID'!PF4</f>
+        <v>72</v>
+      </c>
     </row>
-    <row r="5" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -82405,8 +83665,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY5-'UCI OCUPADA COVID'!OY5</f>
         <v>7</v>
       </c>
+      <c r="OZ5">
+        <f>+'UCI OCUPADA TOTAL'!OZ5-'UCI OCUPADA COVID'!OZ5</f>
+        <v>9</v>
+      </c>
+      <c r="PA5">
+        <f>+'UCI OCUPADA TOTAL'!PA5-'UCI OCUPADA COVID'!PA5</f>
+        <v>8</v>
+      </c>
+      <c r="PB5">
+        <f>+'UCI OCUPADA TOTAL'!PB5-'UCI OCUPADA COVID'!PB5</f>
+        <v>9</v>
+      </c>
+      <c r="PC5">
+        <f>+'UCI OCUPADA TOTAL'!PC5-'UCI OCUPADA COVID'!PC5</f>
+        <v>9</v>
+      </c>
+      <c r="PD5">
+        <f>+'UCI OCUPADA TOTAL'!PD5-'UCI OCUPADA COVID'!PD5</f>
+        <v>10</v>
+      </c>
+      <c r="PE5">
+        <f>+'UCI OCUPADA TOTAL'!PE5-'UCI OCUPADA COVID'!PE5</f>
+        <v>9</v>
+      </c>
+      <c r="PF5">
+        <f>+'UCI OCUPADA TOTAL'!PF5-'UCI OCUPADA COVID'!PF5</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -83786,8 +85074,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY6-'UCI OCUPADA COVID'!OY6</f>
         <v>35</v>
       </c>
+      <c r="OZ6">
+        <f>+'UCI OCUPADA TOTAL'!OZ6-'UCI OCUPADA COVID'!OZ6</f>
+        <v>34</v>
+      </c>
+      <c r="PA6">
+        <f>+'UCI OCUPADA TOTAL'!PA6-'UCI OCUPADA COVID'!PA6</f>
+        <v>32</v>
+      </c>
+      <c r="PB6">
+        <f>+'UCI OCUPADA TOTAL'!PB6-'UCI OCUPADA COVID'!PB6</f>
+        <v>33</v>
+      </c>
+      <c r="PC6">
+        <f>+'UCI OCUPADA TOTAL'!PC6-'UCI OCUPADA COVID'!PC6</f>
+        <v>34</v>
+      </c>
+      <c r="PD6">
+        <f>+'UCI OCUPADA TOTAL'!PD6-'UCI OCUPADA COVID'!PD6</f>
+        <v>29</v>
+      </c>
+      <c r="PE6">
+        <f>+'UCI OCUPADA TOTAL'!PE6-'UCI OCUPADA COVID'!PE6</f>
+        <v>26</v>
+      </c>
+      <c r="PF6">
+        <f>+'UCI OCUPADA TOTAL'!PF6-'UCI OCUPADA COVID'!PF6</f>
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -85167,8 +86483,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY7-'UCI OCUPADA COVID'!OY7</f>
         <v>106</v>
       </c>
+      <c r="OZ7">
+        <f>+'UCI OCUPADA TOTAL'!OZ7-'UCI OCUPADA COVID'!OZ7</f>
+        <v>109</v>
+      </c>
+      <c r="PA7">
+        <f>+'UCI OCUPADA TOTAL'!PA7-'UCI OCUPADA COVID'!PA7</f>
+        <v>110</v>
+      </c>
+      <c r="PB7">
+        <f>+'UCI OCUPADA TOTAL'!PB7-'UCI OCUPADA COVID'!PB7</f>
+        <v>110</v>
+      </c>
+      <c r="PC7">
+        <f>+'UCI OCUPADA TOTAL'!PC7-'UCI OCUPADA COVID'!PC7</f>
+        <v>109</v>
+      </c>
+      <c r="PD7">
+        <f>+'UCI OCUPADA TOTAL'!PD7-'UCI OCUPADA COVID'!PD7</f>
+        <v>103</v>
+      </c>
+      <c r="PE7">
+        <f>+'UCI OCUPADA TOTAL'!PE7-'UCI OCUPADA COVID'!PE7</f>
+        <v>104</v>
+      </c>
+      <c r="PF7">
+        <f>+'UCI OCUPADA TOTAL'!PF7-'UCI OCUPADA COVID'!PF7</f>
+        <v>103</v>
+      </c>
     </row>
-    <row r="8" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -86548,8 +87892,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY8-'UCI OCUPADA COVID'!OY8</f>
         <v>628</v>
       </c>
+      <c r="OZ8">
+        <f>+'UCI OCUPADA TOTAL'!OZ8-'UCI OCUPADA COVID'!OZ8</f>
+        <v>653</v>
+      </c>
+      <c r="PA8">
+        <f>+'UCI OCUPADA TOTAL'!PA8-'UCI OCUPADA COVID'!PA8</f>
+        <v>613</v>
+      </c>
+      <c r="PB8">
+        <f>+'UCI OCUPADA TOTAL'!PB8-'UCI OCUPADA COVID'!PB8</f>
+        <v>611</v>
+      </c>
+      <c r="PC8">
+        <f>+'UCI OCUPADA TOTAL'!PC8-'UCI OCUPADA COVID'!PC8</f>
+        <v>620</v>
+      </c>
+      <c r="PD8">
+        <f>+'UCI OCUPADA TOTAL'!PD8-'UCI OCUPADA COVID'!PD8</f>
+        <v>608</v>
+      </c>
+      <c r="PE8">
+        <f>+'UCI OCUPADA TOTAL'!PE8-'UCI OCUPADA COVID'!PE8</f>
+        <v>591</v>
+      </c>
+      <c r="PF8">
+        <f>+'UCI OCUPADA TOTAL'!PF8-'UCI OCUPADA COVID'!PF8</f>
+        <v>598</v>
+      </c>
     </row>
-    <row r="9" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -87929,8 +89301,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY9-'UCI OCUPADA COVID'!OY9</f>
         <v>36</v>
       </c>
+      <c r="OZ9">
+        <f>+'UCI OCUPADA TOTAL'!OZ9-'UCI OCUPADA COVID'!OZ9</f>
+        <v>34</v>
+      </c>
+      <c r="PA9">
+        <f>+'UCI OCUPADA TOTAL'!PA9-'UCI OCUPADA COVID'!PA9</f>
+        <v>34</v>
+      </c>
+      <c r="PB9">
+        <f>+'UCI OCUPADA TOTAL'!PB9-'UCI OCUPADA COVID'!PB9</f>
+        <v>35</v>
+      </c>
+      <c r="PC9">
+        <f>+'UCI OCUPADA TOTAL'!PC9-'UCI OCUPADA COVID'!PC9</f>
+        <v>29</v>
+      </c>
+      <c r="PD9">
+        <f>+'UCI OCUPADA TOTAL'!PD9-'UCI OCUPADA COVID'!PD9</f>
+        <v>33</v>
+      </c>
+      <c r="PE9">
+        <f>+'UCI OCUPADA TOTAL'!PE9-'UCI OCUPADA COVID'!PE9</f>
+        <v>47</v>
+      </c>
+      <c r="PF9">
+        <f>+'UCI OCUPADA TOTAL'!PF9-'UCI OCUPADA COVID'!PF9</f>
+        <v>37</v>
+      </c>
     </row>
-    <row r="10" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -89310,8 +90710,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY10-'UCI OCUPADA COVID'!OY10</f>
         <v>26</v>
       </c>
+      <c r="OZ10">
+        <f>+'UCI OCUPADA TOTAL'!OZ10-'UCI OCUPADA COVID'!OZ10</f>
+        <v>28</v>
+      </c>
+      <c r="PA10">
+        <f>+'UCI OCUPADA TOTAL'!PA10-'UCI OCUPADA COVID'!PA10</f>
+        <v>30</v>
+      </c>
+      <c r="PB10">
+        <f>+'UCI OCUPADA TOTAL'!PB10-'UCI OCUPADA COVID'!PB10</f>
+        <v>30</v>
+      </c>
+      <c r="PC10">
+        <f>+'UCI OCUPADA TOTAL'!PC10-'UCI OCUPADA COVID'!PC10</f>
+        <v>23</v>
+      </c>
+      <c r="PD10">
+        <f>+'UCI OCUPADA TOTAL'!PD10-'UCI OCUPADA COVID'!PD10</f>
+        <v>23</v>
+      </c>
+      <c r="PE10">
+        <f>+'UCI OCUPADA TOTAL'!PE10-'UCI OCUPADA COVID'!PE10</f>
+        <v>25</v>
+      </c>
+      <c r="PF10">
+        <f>+'UCI OCUPADA TOTAL'!PF10-'UCI OCUPADA COVID'!PF10</f>
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -90691,8 +92119,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY11-'UCI OCUPADA COVID'!OY11</f>
         <v>16</v>
       </c>
+      <c r="OZ11">
+        <f>+'UCI OCUPADA TOTAL'!OZ11-'UCI OCUPADA COVID'!OZ11</f>
+        <v>17</v>
+      </c>
+      <c r="PA11">
+        <f>+'UCI OCUPADA TOTAL'!PA11-'UCI OCUPADA COVID'!PA11</f>
+        <v>16</v>
+      </c>
+      <c r="PB11">
+        <f>+'UCI OCUPADA TOTAL'!PB11-'UCI OCUPADA COVID'!PB11</f>
+        <v>17</v>
+      </c>
+      <c r="PC11">
+        <f>+'UCI OCUPADA TOTAL'!PC11-'UCI OCUPADA COVID'!PC11</f>
+        <v>15</v>
+      </c>
+      <c r="PD11">
+        <f>+'UCI OCUPADA TOTAL'!PD11-'UCI OCUPADA COVID'!PD11</f>
+        <v>16</v>
+      </c>
+      <c r="PE11">
+        <f>+'UCI OCUPADA TOTAL'!PE11-'UCI OCUPADA COVID'!PE11</f>
+        <v>17</v>
+      </c>
+      <c r="PF11">
+        <f>+'UCI OCUPADA TOTAL'!PF11-'UCI OCUPADA COVID'!PF11</f>
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -92072,8 +93528,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY12-'UCI OCUPADA COVID'!OY12</f>
         <v>93</v>
       </c>
+      <c r="OZ12">
+        <f>+'UCI OCUPADA TOTAL'!OZ12-'UCI OCUPADA COVID'!OZ12</f>
+        <v>95</v>
+      </c>
+      <c r="PA12">
+        <f>+'UCI OCUPADA TOTAL'!PA12-'UCI OCUPADA COVID'!PA12</f>
+        <v>101</v>
+      </c>
+      <c r="PB12">
+        <f>+'UCI OCUPADA TOTAL'!PB12-'UCI OCUPADA COVID'!PB12</f>
+        <v>97</v>
+      </c>
+      <c r="PC12">
+        <f>+'UCI OCUPADA TOTAL'!PC12-'UCI OCUPADA COVID'!PC12</f>
+        <v>97</v>
+      </c>
+      <c r="PD12">
+        <f>+'UCI OCUPADA TOTAL'!PD12-'UCI OCUPADA COVID'!PD12</f>
+        <v>98</v>
+      </c>
+      <c r="PE12">
+        <f>+'UCI OCUPADA TOTAL'!PE12-'UCI OCUPADA COVID'!PE12</f>
+        <v>94</v>
+      </c>
+      <c r="PF12">
+        <f>+'UCI OCUPADA TOTAL'!PF12-'UCI OCUPADA COVID'!PF12</f>
+        <v>95</v>
+      </c>
     </row>
-    <row r="13" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -93453,8 +94937,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY13-'UCI OCUPADA COVID'!OY13</f>
         <v>36</v>
       </c>
+      <c r="OZ13">
+        <f>+'UCI OCUPADA TOTAL'!OZ13-'UCI OCUPADA COVID'!OZ13</f>
+        <v>36</v>
+      </c>
+      <c r="PA13">
+        <f>+'UCI OCUPADA TOTAL'!PA13-'UCI OCUPADA COVID'!PA13</f>
+        <v>37</v>
+      </c>
+      <c r="PB13">
+        <f>+'UCI OCUPADA TOTAL'!PB13-'UCI OCUPADA COVID'!PB13</f>
+        <v>34</v>
+      </c>
+      <c r="PC13">
+        <f>+'UCI OCUPADA TOTAL'!PC13-'UCI OCUPADA COVID'!PC13</f>
+        <v>38</v>
+      </c>
+      <c r="PD13">
+        <f>+'UCI OCUPADA TOTAL'!PD13-'UCI OCUPADA COVID'!PD13</f>
+        <v>28</v>
+      </c>
+      <c r="PE13">
+        <f>+'UCI OCUPADA TOTAL'!PE13-'UCI OCUPADA COVID'!PE13</f>
+        <v>32</v>
+      </c>
+      <c r="PF13">
+        <f>+'UCI OCUPADA TOTAL'!PF13-'UCI OCUPADA COVID'!PF13</f>
+        <v>37</v>
+      </c>
     </row>
-    <row r="14" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -94834,8 +96346,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY14-'UCI OCUPADA COVID'!OY14</f>
         <v>10</v>
       </c>
+      <c r="OZ14">
+        <f>+'UCI OCUPADA TOTAL'!OZ14-'UCI OCUPADA COVID'!OZ14</f>
+        <v>9</v>
+      </c>
+      <c r="PA14">
+        <f>+'UCI OCUPADA TOTAL'!PA14-'UCI OCUPADA COVID'!PA14</f>
+        <v>10</v>
+      </c>
+      <c r="PB14">
+        <f>+'UCI OCUPADA TOTAL'!PB14-'UCI OCUPADA COVID'!PB14</f>
+        <v>11</v>
+      </c>
+      <c r="PC14">
+        <f>+'UCI OCUPADA TOTAL'!PC14-'UCI OCUPADA COVID'!PC14</f>
+        <v>10</v>
+      </c>
+      <c r="PD14">
+        <f>+'UCI OCUPADA TOTAL'!PD14-'UCI OCUPADA COVID'!PD14</f>
+        <v>10</v>
+      </c>
+      <c r="PE14">
+        <f>+'UCI OCUPADA TOTAL'!PE14-'UCI OCUPADA COVID'!PE14</f>
+        <v>9</v>
+      </c>
+      <c r="PF14">
+        <f>+'UCI OCUPADA TOTAL'!PF14-'UCI OCUPADA COVID'!PF14</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="15" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -96215,8 +97755,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY15-'UCI OCUPADA COVID'!OY15</f>
         <v>35</v>
       </c>
+      <c r="OZ15">
+        <f>+'UCI OCUPADA TOTAL'!OZ15-'UCI OCUPADA COVID'!OZ15</f>
+        <v>25</v>
+      </c>
+      <c r="PA15">
+        <f>+'UCI OCUPADA TOTAL'!PA15-'UCI OCUPADA COVID'!PA15</f>
+        <v>26</v>
+      </c>
+      <c r="PB15">
+        <f>+'UCI OCUPADA TOTAL'!PB15-'UCI OCUPADA COVID'!PB15</f>
+        <v>27</v>
+      </c>
+      <c r="PC15">
+        <f>+'UCI OCUPADA TOTAL'!PC15-'UCI OCUPADA COVID'!PC15</f>
+        <v>23</v>
+      </c>
+      <c r="PD15">
+        <f>+'UCI OCUPADA TOTAL'!PD15-'UCI OCUPADA COVID'!PD15</f>
+        <v>25</v>
+      </c>
+      <c r="PE15">
+        <f>+'UCI OCUPADA TOTAL'!PE15-'UCI OCUPADA COVID'!PE15</f>
+        <v>25</v>
+      </c>
+      <c r="PF15">
+        <f>+'UCI OCUPADA TOTAL'!PF15-'UCI OCUPADA COVID'!PF15</f>
+        <v>25</v>
+      </c>
     </row>
-    <row r="16" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -97596,8 +99164,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY16-'UCI OCUPADA COVID'!OY16</f>
         <v>0</v>
       </c>
+      <c r="OZ16">
+        <f>+'UCI OCUPADA TOTAL'!OZ16-'UCI OCUPADA COVID'!OZ16</f>
+        <v>0</v>
+      </c>
+      <c r="PA16">
+        <f>+'UCI OCUPADA TOTAL'!PA16-'UCI OCUPADA COVID'!PA16</f>
+        <v>1</v>
+      </c>
+      <c r="PB16">
+        <f>+'UCI OCUPADA TOTAL'!PB16-'UCI OCUPADA COVID'!PB16</f>
+        <v>1</v>
+      </c>
+      <c r="PC16">
+        <f>+'UCI OCUPADA TOTAL'!PC16-'UCI OCUPADA COVID'!PC16</f>
+        <v>1</v>
+      </c>
+      <c r="PD16">
+        <f>+'UCI OCUPADA TOTAL'!PD16-'UCI OCUPADA COVID'!PD16</f>
+        <v>0</v>
+      </c>
+      <c r="PE16">
+        <f>+'UCI OCUPADA TOTAL'!PE16-'UCI OCUPADA COVID'!PE16</f>
+        <v>3</v>
+      </c>
+      <c r="PF16">
+        <f>+'UCI OCUPADA TOTAL'!PF16-'UCI OCUPADA COVID'!PF16</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -98977,8 +100573,36 @@
         <f>+'UCI OCUPADA TOTAL'!OY17-'UCI OCUPADA COVID'!OY17</f>
         <v>10</v>
       </c>
+      <c r="OZ17">
+        <f>+'UCI OCUPADA TOTAL'!OZ17-'UCI OCUPADA COVID'!OZ17</f>
+        <v>12</v>
+      </c>
+      <c r="PA17">
+        <f>+'UCI OCUPADA TOTAL'!PA17-'UCI OCUPADA COVID'!PA17</f>
+        <v>12</v>
+      </c>
+      <c r="PB17">
+        <f>+'UCI OCUPADA TOTAL'!PB17-'UCI OCUPADA COVID'!PB17</f>
+        <v>9</v>
+      </c>
+      <c r="PC17">
+        <f>+'UCI OCUPADA TOTAL'!PC17-'UCI OCUPADA COVID'!PC17</f>
+        <v>10</v>
+      </c>
+      <c r="PD17">
+        <f>+'UCI OCUPADA TOTAL'!PD17-'UCI OCUPADA COVID'!PD17</f>
+        <v>8</v>
+      </c>
+      <c r="PE17">
+        <f>+'UCI OCUPADA TOTAL'!PE17-'UCI OCUPADA COVID'!PE17</f>
+        <v>13</v>
+      </c>
+      <c r="PF17">
+        <f>+'UCI OCUPADA TOTAL'!PF17-'UCI OCUPADA COVID'!PF17</f>
+        <v>12</v>
+      </c>
     </row>
-    <row r="18" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -100358,48 +101982,76 @@
         <f>+'UCI OCUPADA TOTAL'!OY18-'UCI OCUPADA COVID'!OY18</f>
         <v>1110</v>
       </c>
+      <c r="OZ18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!OZ18-'UCI OCUPADA COVID'!OZ18</f>
+        <v>1142</v>
+      </c>
+      <c r="PA18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PA18-'UCI OCUPADA COVID'!PA18</f>
+        <v>1101</v>
+      </c>
+      <c r="PB18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PB18-'UCI OCUPADA COVID'!PB18</f>
+        <v>1099</v>
+      </c>
+      <c r="PC18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PC18-'UCI OCUPADA COVID'!PC18</f>
+        <v>1093</v>
+      </c>
+      <c r="PD18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PD18-'UCI OCUPADA COVID'!PD18</f>
+        <v>1066</v>
+      </c>
+      <c r="PE18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PE18-'UCI OCUPADA COVID'!PE18</f>
+        <v>1073</v>
+      </c>
+      <c r="PF18" s="20">
+        <f>+'UCI OCUPADA TOTAL'!PF18-'UCI OCUPADA COVID'!PF18</f>
+        <v>1080</v>
+      </c>
     </row>
-    <row r="19" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:415" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:422" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">

</xml_diff>